<commit_message>
add sustainability info sheet
</commit_message>
<xml_diff>
--- a/data/context_data.xlsx
+++ b/data/context_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m.haller\Documents\code\ptx-boa\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDC16062-C2FC-4172-AE98-5863456ECFE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C18D647B-F47B-47A4-9ADF-E5D3A53F06E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{D16C601B-E1D6-40C0-8CC1-80505BE1FBB6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D16C601B-E1D6-40C0-8CC1-80505BE1FBB6}"/>
   </bookViews>
   <sheets>
     <sheet name="certification_schemes" sheetId="6" r:id="rId1"/>
@@ -25,94 +25,94 @@
     <externalReference r:id="rId8"/>
   </externalReferences>
   <definedNames>
-    <definedName name="can_use_pipeline" localSheetId="3">INDEX([1]!chains[CAN_PIPELINE],supply!sel_chain_index)</definedName>
-    <definedName name="can_use_pipeline">INDEX([1]!chains[CAN_PIPELINE],sel_chain_index)</definedName>
-    <definedName name="chains_chain">[1]!chains[chain]</definedName>
-    <definedName name="compCostCountries_DELETE">[1]!Table23[Country code]</definedName>
-    <definedName name="context_data_carbonsource" localSheetId="3">[2]!Table33353637[#All]</definedName>
+    <definedName name="can_use_pipeline" localSheetId="3">INDEX([2]!chains[CAN_PIPELINE],supply!sel_chain_index)</definedName>
+    <definedName name="can_use_pipeline">INDEX([2]!chains[CAN_PIPELINE],sel_chain_index)</definedName>
+    <definedName name="chains_chain">[2]!chains[chain]</definedName>
+    <definedName name="compCostCountries_DELETE">[2]!Table23[Country code]</definedName>
+    <definedName name="context_data_carbonsource" localSheetId="3">[1]!Table33353637[#All]</definedName>
     <definedName name="context_data_carbonsource">#REF!</definedName>
-    <definedName name="context_data_infobox" localSheetId="3">[2]!Table32[#Data]</definedName>
+    <definedName name="context_data_infobox" localSheetId="3">[1]!Table32[#Data]</definedName>
     <definedName name="context_data_infobox">#REF!</definedName>
-    <definedName name="context_data_re" localSheetId="3">[2]!Table33[#All]</definedName>
+    <definedName name="context_data_re" localSheetId="3">[1]!Table33[#All]</definedName>
     <definedName name="context_data_re">#REF!</definedName>
-    <definedName name="context_data_transport_mode" localSheetId="3">[2]!Table3335[#All]</definedName>
+    <definedName name="context_data_transport_mode" localSheetId="3">[1]!Table3335[#All]</definedName>
     <definedName name="context_data_transport_mode">#REF!</definedName>
-    <definedName name="context_data_watersource" localSheetId="3">[2]!Table333536[#All]</definedName>
+    <definedName name="context_data_watersource" localSheetId="3">[1]!Table333536[#All]</definedName>
     <definedName name="context_data_watersource">#REF!</definedName>
-    <definedName name="conv_fact_to_mass">[1]_calc!$BM$6</definedName>
-    <definedName name="country_area">[1]!Table22[#All]</definedName>
-    <definedName name="country_country_code">[1]!country[target_country_code]</definedName>
-    <definedName name="country_country_name">[1]!country[target_country_name]</definedName>
-    <definedName name="country_energy_use">[1]!Table25[#All]</definedName>
-    <definedName name="country_pop">[1]!Table26[#All]</definedName>
-    <definedName name="country_pop_and_energy_use" localSheetId="3">[1]!Table26[#Data]</definedName>
-    <definedName name="country_pop_and_energy_use">[1]!Table26[#Data]</definedName>
-    <definedName name="default_scenarios">[1]!tab_default_scenario[default_scenario]</definedName>
-    <definedName name="dim_bool_bool">[1]!dim_bool[BOOL]</definedName>
-    <definedName name="flh_deriv">[1]_calc!$X$257:$X$335</definedName>
-    <definedName name="flh_ely">[1]_calc!$Q$257:$Q$335</definedName>
-    <definedName name="flh_region_code">[1]_calc!$B$257:$B$335</definedName>
-    <definedName name="flow_flow_code">[1]!flow[flow_code]</definedName>
-    <definedName name="flow_flow_name">[1]!flow[flow_name]</definedName>
-    <definedName name="flow_short_names">[1]_dims!$X$22:$Y$37</definedName>
-    <definedName name="input_scenarios">[1]!tabDatasetsInput[name]</definedName>
-    <definedName name="mapMaxValue">[1]_map!$G$3</definedName>
-    <definedName name="mapMinValue">[1]_map!$G$2</definedName>
-    <definedName name="output_scenario_name">[1]_todo_dev!$A$9</definedName>
-    <definedName name="output_scenario_names">[1]!output_scenarios[scenario]</definedName>
-    <definedName name="output_units">[1]!tabOutputUnit[output_unit]</definedName>
-    <definedName name="process_classes_process_class">[1]!process_classes[process_class]</definedName>
-    <definedName name="process_classes_process_class_name">[1]!process_classes[process_class_name]</definedName>
-    <definedName name="process_main_flow_code_out">[1]!process[main_flow_code_out]</definedName>
-    <definedName name="process_process_class">[1]!process[process_class]</definedName>
-    <definedName name="process_process_code">[1]!process[process_code]</definedName>
-    <definedName name="process_process_name">[1]!process[process_name]</definedName>
-    <definedName name="process_res_gen_name">[1]!process_res_gen[process_name]</definedName>
-    <definedName name="process_res_gen_process_code">[1]!process_res_gen[process_code]</definedName>
-    <definedName name="process_res_gen_process_name">[1]!process_res_gen[process_name]</definedName>
-    <definedName name="region_region_code">[1]!region[source_region_code]</definedName>
-    <definedName name="region_region_name">[1]!region[region_name]</definedName>
-    <definedName name="regions_by_cost">[1]!Table21[#All]</definedName>
-    <definedName name="release_date">[1]_release!$B$2</definedName>
-    <definedName name="release_version">[1]_release!$B$1</definedName>
-    <definedName name="saved_outputs">[1]!tabDatasetsOutput[name]</definedName>
-    <definedName name="secondary_process_CO2_G">[1]!tabSelCo2[name]</definedName>
-    <definedName name="secondary_process_H2O_L">[1]!tabSelWater[name]</definedName>
-    <definedName name="sel_chain">[1]b_dashboard!$D$23</definedName>
-    <definedName name="sel_chain_deriv_proc_code">[1]_calc!$X$2</definedName>
-    <definedName name="sel_chain_ely_proc_code">[1]_calc!$Q$2</definedName>
-    <definedName name="sel_chain_flow_out">[1]_calc!$BM$5</definedName>
-    <definedName name="sel_chain_index" localSheetId="3">MATCH(sel_chain,[1]!chains[chain],)</definedName>
-    <definedName name="sel_chain_index">MATCH(sel_chain,[1]!chains[chain],)</definedName>
-    <definedName name="sel_chain_range" localSheetId="3">OFFSET([1]!chains[[#Headers],[chain]],supply!sel_chain_index,1,1,COUNTA([1]!chains[#Headers])-1)</definedName>
-    <definedName name="sel_chain_range">OFFSET([1]!chains[[#Headers],[chain]],sel_chain_index,1,1,COUNTA([1]!chains[#Headers])-1)</definedName>
-    <definedName name="sel_chain_range_word" localSheetId="3">OFFSET([1]!chains[[#Headers],[chain]],sel_chain_index_world,1,1,COUNTA([1]!chains[#Headers])-1)</definedName>
-    <definedName name="sel_chain_range_word">OFFSET([1]!chains[[#Headers],[chain]],sel_chain_index_world,1,1,COUNTA([1]!chains[#Headers])-1)</definedName>
-    <definedName name="sel_choices_transport" localSheetId="3">OFFSET([1]!choicesTransport[none],0,supply!sel_pipeline_possible*2+sel_ship_possible,supply!sel_pipeline_possible+sel_ship_possible)</definedName>
-    <definedName name="sel_choices_transport">OFFSET([1]!choicesTransport[none],0,sel_pipeline_possible*2+sel_ship_possible,sel_pipeline_possible+sel_ship_possible)</definedName>
+    <definedName name="conv_fact_to_mass">[2]_calc!$BM$6</definedName>
+    <definedName name="country_area">[2]!Table22[#All]</definedName>
+    <definedName name="country_country_code">[2]!country[target_country_code]</definedName>
+    <definedName name="country_country_name">[2]!country[target_country_name]</definedName>
+    <definedName name="country_energy_use">[2]!Table25[#All]</definedName>
+    <definedName name="country_pop">[2]!Table26[#All]</definedName>
+    <definedName name="country_pop_and_energy_use" localSheetId="3">[2]!Table26[#Data]</definedName>
+    <definedName name="country_pop_and_energy_use">[2]!Table26[#Data]</definedName>
+    <definedName name="default_scenarios">[2]!tab_default_scenario[default_scenario]</definedName>
+    <definedName name="dim_bool_bool">[2]!dim_bool[BOOL]</definedName>
+    <definedName name="flh_deriv">[2]_calc!$X$257:$X$335</definedName>
+    <definedName name="flh_ely">[2]_calc!$Q$257:$Q$335</definedName>
+    <definedName name="flh_region_code">[2]_calc!$B$257:$B$335</definedName>
+    <definedName name="flow_flow_code">[2]!flow[flow_code]</definedName>
+    <definedName name="flow_flow_name">[2]!flow[flow_name]</definedName>
+    <definedName name="flow_short_names">[2]_dims!$X$22:$Y$37</definedName>
+    <definedName name="input_scenarios">[2]!tabDatasetsInput[name]</definedName>
+    <definedName name="mapMaxValue">[2]_map!$G$3</definedName>
+    <definedName name="mapMinValue">[2]_map!$G$2</definedName>
+    <definedName name="output_scenario_name">[2]_todo_dev!$A$9</definedName>
+    <definedName name="output_scenario_names">[2]!output_scenarios[scenario]</definedName>
+    <definedName name="output_units">[2]!tabOutputUnit[output_unit]</definedName>
+    <definedName name="process_classes_process_class">[2]!process_classes[process_class]</definedName>
+    <definedName name="process_classes_process_class_name">[2]!process_classes[process_class_name]</definedName>
+    <definedName name="process_main_flow_code_out">[2]!process[main_flow_code_out]</definedName>
+    <definedName name="process_process_class">[2]!process[process_class]</definedName>
+    <definedName name="process_process_code">[2]!process[process_code]</definedName>
+    <definedName name="process_process_name">[2]!process[process_name]</definedName>
+    <definedName name="process_res_gen_name">[2]!process_res_gen[process_name]</definedName>
+    <definedName name="process_res_gen_process_code">[2]!process_res_gen[process_code]</definedName>
+    <definedName name="process_res_gen_process_name">[2]!process_res_gen[process_name]</definedName>
+    <definedName name="region_region_code">[2]!region[source_region_code]</definedName>
+    <definedName name="region_region_name">[2]!region[region_name]</definedName>
+    <definedName name="regions_by_cost">[2]!Table21[#All]</definedName>
+    <definedName name="release_date">[2]_release!$B$2</definedName>
+    <definedName name="release_version">[2]_release!$B$1</definedName>
+    <definedName name="saved_outputs">[2]!tabDatasetsOutput[name]</definedName>
+    <definedName name="secondary_process_CO2_G">[2]!tabSelCo2[name]</definedName>
+    <definedName name="secondary_process_H2O_L">[2]!tabSelWater[name]</definedName>
+    <definedName name="sel_chain">[2]b_dashboard!$D$23</definedName>
+    <definedName name="sel_chain_deriv_proc_code">[2]_calc!$X$2</definedName>
+    <definedName name="sel_chain_ely_proc_code">[2]_calc!$Q$2</definedName>
+    <definedName name="sel_chain_flow_out">[2]_calc!$BM$5</definedName>
+    <definedName name="sel_chain_index" localSheetId="3">MATCH(sel_chain,[2]!chains[chain],)</definedName>
+    <definedName name="sel_chain_index">MATCH(sel_chain,[2]!chains[chain],)</definedName>
+    <definedName name="sel_chain_range" localSheetId="3">OFFSET([2]!chains[[#Headers],[chain]],supply!sel_chain_index,1,1,COUNTA([2]!chains[#Headers])-1)</definedName>
+    <definedName name="sel_chain_range">OFFSET([2]!chains[[#Headers],[chain]],sel_chain_index,1,1,COUNTA([2]!chains[#Headers])-1)</definedName>
+    <definedName name="sel_chain_range_word" localSheetId="3">OFFSET([2]!chains[[#Headers],[chain]],sel_chain_index_world,1,1,COUNTA([2]!chains[#Headers])-1)</definedName>
+    <definedName name="sel_chain_range_word">OFFSET([2]!chains[[#Headers],[chain]],sel_chain_index_world,1,1,COUNTA([2]!chains[#Headers])-1)</definedName>
+    <definedName name="sel_choices_transport" localSheetId="3">OFFSET([2]!choicesTransport[none],0,supply!sel_pipeline_possible*2+sel_ship_possible,supply!sel_pipeline_possible+sel_ship_possible)</definedName>
+    <definedName name="sel_choices_transport">OFFSET([2]!choicesTransport[none],0,sel_pipeline_possible*2+sel_ship_possible,sel_pipeline_possible+sel_ship_possible)</definedName>
     <definedName name="sel_country_code" localSheetId="3">IF(sel_country_name="","",INDEX(country_country_code,MATCH(sel_country_name,country_country_name,0),1))</definedName>
     <definedName name="sel_country_code">IF(sel_country_name="","",INDEX(country_country_code,MATCH(sel_country_name,country_country_name,0),1))</definedName>
-    <definedName name="sel_country_name">[1]b_dashboard!$D$22</definedName>
-    <definedName name="sel_pipeline_possible" localSheetId="3">AND(INDEX([1]_calc!$AQ$14:$AQ$92,MATCH(_xlfn.SINGLE(supply!sel_region_code),[1]_calc!$B$14:$B$92,0))&gt;0,_xlfn.SINGLE(supply!can_use_pipeline)=TRUE)</definedName>
-    <definedName name="sel_pipeline_possible">AND(INDEX([1]_calc!$AQ$14:$AQ$92,MATCH(_xlfn.SINGLE(sel_region_code),[1]_calc!$B$14:$B$92,0))&gt;0,_xlfn.SINGLE(can_use_pipeline)=TRUE)</definedName>
-    <definedName name="sel_region_code" localSheetId="3">IF(sel_region_name="","",INDEX([1]!region[source_region_code],MATCH(sel_region_name,[1]!region[region_name],0),1))</definedName>
-    <definedName name="sel_region_code">IF(sel_region_name="","",INDEX([1]!region[source_region_code],MATCH(sel_region_name,[1]!region[region_name],0),1))</definedName>
+    <definedName name="sel_country_name">[2]b_dashboard!$D$22</definedName>
+    <definedName name="sel_pipeline_possible" localSheetId="3">AND(INDEX([2]_calc!$AQ$14:$AQ$92,MATCH(_xlfn.SINGLE(supply!sel_region_code),[2]_calc!$B$14:$B$92,0))&gt;0,_xlfn.SINGLE(supply!can_use_pipeline)=TRUE)</definedName>
+    <definedName name="sel_pipeline_possible">AND(INDEX([2]_calc!$AQ$14:$AQ$92,MATCH(_xlfn.SINGLE(sel_region_code),[2]_calc!$B$14:$B$92,0))&gt;0,_xlfn.SINGLE(can_use_pipeline)=TRUE)</definedName>
+    <definedName name="sel_region_code" localSheetId="3">IF(sel_region_name="","",INDEX([2]!region[source_region_code],MATCH(sel_region_name,[2]!region[region_name],0),1))</definedName>
+    <definedName name="sel_region_code">IF(sel_region_name="","",INDEX([2]!region[source_region_code],MATCH(sel_region_name,[2]!region[region_name],0),1))</definedName>
     <definedName name="sel_region_country_code" localSheetId="3">IF(supply!sel_region_code="","",LEFT(supply!sel_region_code,3))</definedName>
     <definedName name="sel_region_country_code">IF(sel_region_code="","",LEFT(sel_region_code,3))</definedName>
-    <definedName name="sel_region_name">[1]b_dashboard!$D$21</definedName>
-    <definedName name="sel_res_gen" localSheetId="3">IF(sel_res_gen_name="","",INDEX([1]!process[#Data],MATCH(sel_res_gen_name,[1]!process[process_name],0),1))</definedName>
-    <definedName name="sel_res_gen">IF(sel_res_gen_name="","",INDEX([1]!process[#Data],MATCH(sel_res_gen_name,[1]!process[process_name],0),1))</definedName>
-    <definedName name="sel_res_gen_name">[1]b_dashboard!$D$24</definedName>
-    <definedName name="sel_scenario">[1]b_dashboard!$D$25</definedName>
-    <definedName name="sel_secproc_co2">[1]b_dashboard!$D$30</definedName>
-    <definedName name="sel_secproc_water">[1]b_dashboard!$D$31</definedName>
-    <definedName name="sel_ship_own_fuel">[1]b_dashboard!$D$33</definedName>
+    <definedName name="sel_region_name">[2]b_dashboard!$D$21</definedName>
+    <definedName name="sel_res_gen" localSheetId="3">IF(sel_res_gen_name="","",INDEX([2]!process[#Data],MATCH(sel_res_gen_name,[2]!process[process_name],0),1))</definedName>
+    <definedName name="sel_res_gen">IF(sel_res_gen_name="","",INDEX([2]!process[#Data],MATCH(sel_res_gen_name,[2]!process[process_name],0),1))</definedName>
+    <definedName name="sel_res_gen_name">[2]b_dashboard!$D$24</definedName>
+    <definedName name="sel_scenario">[2]b_dashboard!$D$25</definedName>
+    <definedName name="sel_secproc_co2">[2]b_dashboard!$D$30</definedName>
+    <definedName name="sel_secproc_water">[2]b_dashboard!$D$31</definedName>
+    <definedName name="sel_ship_own_fuel">[2]b_dashboard!$D$33</definedName>
     <definedName name="sel_ship_possible">TRUE</definedName>
-    <definedName name="sel_transport">[1]b_dashboard!$D$32</definedName>
-    <definedName name="selOutputUnit">[1]b_dashboard!$D$34</definedName>
-    <definedName name="selOutputUnit2">[1]_dims!$CA$2</definedName>
-    <definedName name="tabDatasets_name">[1]!tabDatasetsInput[name]</definedName>
-    <definedName name="target_countries">[1]!country[target_country_code]</definedName>
+    <definedName name="sel_transport">[2]b_dashboard!$D$32</definedName>
+    <definedName name="selOutputUnit">[2]b_dashboard!$D$34</definedName>
+    <definedName name="selOutputUnit2">[2]_dims!$CA$2</definedName>
+    <definedName name="tabDatasets_name">[2]!tabDatasetsInput[name]</definedName>
+    <definedName name="target_countries">[2]!country[target_country_code]</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -840,10 +840,6 @@
     <t>ISCC (2020);ISCC (2021);Sailer et al. (2022)</t>
   </si>
   <si>
-    <t>TÜV Süd CMS 70 (Green Hydrogen, 
-Green Hydrogen+)</t>
-  </si>
-  <si>
     <t xml:space="preserve">**Certification scheme**
 Voluntary certification scheme based on German and European legislation. The certificate has two boundaries for GHG accounting: well-to-gate (label: Green H2; use of RFNBOs in transport) and well-to-wheel (label: Green H2+; use of RFNBOs for all other activities). The Green H2+ label thus requires proof of GHG emissions below a set threshold within a broader assessment scope. In general, the scheme allows H2 producers to demonstrate specific product characteristics, in alignment with RED II requirements. </t>
   </si>
@@ -1095,11 +1091,6 @@
     <t>To secure that existing RES-E plants are not withdrawn from existing capacities, **electricity should be sourced from new, additional RES-E plants.** (How) Can you ensure this additionality of electricity supply?</t>
   </si>
   <si>
-    <t xml:space="preserve">**If electricity is sourced from the public grid**, further questions regarding temporal and geographical correlction should be considered. 
-- How do RES-E production and PTX production relate to each other on a time scale? (How) Can you ensure a **temporal correlation to RES-E production?** 
-- How do RES-E production and PTX production relate to each other on a geographical scale? (How) Can you ensure a **geographical correlation to RES-E production?** </t>
-  </si>
-  <si>
     <t>**Conversion of hydrogen** for transport is associated with efficiency losses. 
 (How) Can conversion processes be kept to a minimum to avoid efficiency losses? Is transport in the desired PTX product possible without further conversion processes?</t>
   </si>
@@ -1126,12 +1117,6 @@
     <t xml:space="preserve">Is the region affected by **water stress**? If yes, how is this issue addressed? </t>
   </si>
   <si>
-    <t>**If sourcing from Sea Water Desalination (SWD)**, further questions should be considered.
-- How is **brine disposal** managed? Can chemicals be reduced to a minimum?
-- How are **additional energy requirements of SWD plants** sourced? Are there sufficient available RES-e capacities to power SWD plants?
-- To secure that existing **SWD plants are not withdrawn from exisiting capacities, SWD plants should be new and additional**? (How) Can you ensure this additionality?</t>
-  </si>
-  <si>
     <t>**Which land uses are excluded** for project development? Is it ensured that no protected areas are compromised?</t>
   </si>
   <si>
@@ -1207,24 +1192,10 @@
     <t>Have **local stakeholders been consulted** about the project? Is involvement planned for before and/or during the project?</t>
   </si>
   <si>
-    <t>May the PtX production **harm local (informal) land and/or water rights**? 
-- How can **local (informal) claims be respected** and appropriately be integrated into planning processes?
-- Could **additional water demand lead to rising water costs** to local public?
-- (How) Are **potential conflicts adressed*?</t>
-  </si>
-  <si>
     <t xml:space="preserve">(How) Is it secured that an appropriate **proportion of the workforce is made up of local staff**? </t>
   </si>
   <si>
     <t>(How) Can it be ensured that a **long-term demand for skilled labour** is generated and met with local workforce?</t>
-  </si>
-  <si>
-    <t>May the PtX production **harm human rights**? 
-- (How) Can **compliance with human rights** be ensured during all project phases (project planning, construction &amp; operation)?</t>
-  </si>
-  <si>
-    <t>Does the PtX production **comply with due diligence**? 
-- (How) Can **compliance with due diligence be proven**?</t>
   </si>
   <si>
     <t>Where in the production chain do **health and safety risks** potentially occur? 
@@ -2173,6 +2144,34 @@
   </si>
   <si>
     <t>source_h2_demand_2030</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**If electricity is sourced from the public grid**, further questions regarding temporal and geographical correlction should be considered. 
+  - How do RES-E production and PTX production relate to each other on a time scale? (How) Can you ensure a **temporal correlation to RES-E production?** 
+  - How do RES-E production and PTX production relate to each other on a geographical scale? (How) Can you ensure a **geographical correlation to RES-E production?** </t>
+  </si>
+  <si>
+    <t>**If sourcing from Sea Water Desalination (SWD)**, further questions should be considered.
+  - How is **brine disposal** managed? Can chemicals be reduced to a minimum?
+  - How are **additional energy requirements of SWD plants** sourced? Are there sufficient available RES-e capacities to power SWD plants?
+  - To secure that existing **SWD plants are not withdrawn from exisiting capacities, SWD plants should be new and additional**? (How) Can you ensure this additionality?</t>
+  </si>
+  <si>
+    <t>May the PtX production **harm local (informal) land and/or water rights**? 
+  - How can **local (informal) claims be respected** and appropriately be integrated into planning processes?
+  - Could **additional water demand lead to rising water costs** to local public?
+  - (How) Are **potential conflicts adressed*?</t>
+  </si>
+  <si>
+    <t>May the PtX production **harm human rights**? 
+  - (How) Can **compliance with human rights** be ensured during all project phases (project planning, construction &amp; operation)?</t>
+  </si>
+  <si>
+    <t>Does the PtX production **comply with due diligence**? 
+  - (How) Can **compliance with due diligence be proven**?</t>
+  </si>
+  <si>
+    <t>TÜV Süd CMS 70 (Green Hydrogen, Green Hydrogen+)</t>
   </si>
 </sst>
 </file>
@@ -3028,6 +3027,37 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
+      <sheetName val="Sheet1"/>
+      <sheetName val="context_cs_type"/>
+      <sheetName val="context_cs_scope"/>
+      <sheetName val="context_cs_countries"/>
+      <sheetName val="_context_data_infobox"/>
+      <sheetName val="certification_schemes"/>
+      <sheetName val="demand_countries"/>
+      <sheetName val="literature"/>
+      <sheetName val="sustainability"/>
+      <sheetName val="context_data"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
       <sheetName val="b_disclaimer"/>
       <sheetName val="b_Info"/>
       <sheetName val="b_dashboard"/>
@@ -3078,7 +3108,6 @@
       <sheetName val="_scenario_2030_medium"/>
       <sheetName val="_scenario_2040_high"/>
       <sheetName val="_scenario_2030_high"/>
-      <sheetName val="ptxboa_v19 - Kopie"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
@@ -3143,7 +3172,7 @@
         </row>
         <row r="2">
           <cell r="B2">
-            <v>45197</v>
+            <v>45205</v>
           </cell>
         </row>
       </sheetData>
@@ -4864,38 +4893,6 @@
       <sheetData sheetId="47"/>
       <sheetData sheetId="48"/>
       <sheetData sheetId="49"/>
-      <sheetData sheetId="50" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sheet1"/>
-      <sheetName val="context_cs_type"/>
-      <sheetName val="context_cs_scope"/>
-      <sheetName val="context_cs_countries"/>
-      <sheetName val="_context_data_infobox"/>
-      <sheetName val="certification_schemes"/>
-      <sheetName val="demand_countries"/>
-      <sheetName val="literature"/>
-      <sheetName val="sustainability"/>
-      <sheetName val="context_data"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -5240,8 +5237,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE04771-D0C8-4928-A647-849B136F2B55}">
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -5292,7 +5289,7 @@
     </row>
     <row r="2" spans="1:16" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>18</v>
@@ -5339,7 +5336,7 @@
     </row>
     <row r="3" spans="1:16" ht="178.5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>16</v>
@@ -5348,7 +5345,7 @@
         <v>136</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>25</v>
@@ -5384,16 +5381,16 @@
     </row>
     <row r="4" spans="1:16" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>235</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>236</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>136</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>140</v>
@@ -5411,20 +5408,20 @@
         <v>142</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
       <c r="O4" s="2" t="s">
-        <v>603</v>
+        <v>597</v>
       </c>
       <c r="P4" s="2"/>
     </row>
     <row r="5" spans="1:16" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>13</v>
@@ -5433,7 +5430,7 @@
         <v>136</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>143</v>
@@ -5451,7 +5448,7 @@
         <v>147</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="K5" s="2"/>
       <c r="L5" s="2" t="s">
@@ -5462,12 +5459,12 @@
       </c>
       <c r="N5" s="2"/>
       <c r="O5" s="2" t="s">
-        <v>540</v>
+        <v>534</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="242.25" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>17</v>
@@ -5476,7 +5473,7 @@
         <v>136</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>150</v>
@@ -5491,7 +5488,7 @@
         <v>151</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>153</v>
@@ -5503,7 +5500,7 @@
         <v>155</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="O6" s="2" t="s">
         <v>156</v>
@@ -5511,16 +5508,16 @@
     </row>
     <row r="7" spans="1:16" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>239</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>240</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>136</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>157</v>
@@ -5538,7 +5535,7 @@
         <v>147</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>158</v>
@@ -5547,13 +5544,13 @@
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
       <c r="O7" s="2" t="s">
-        <v>541</v>
+        <v>535</v>
       </c>
       <c r="P7" s="2"/>
     </row>
     <row r="8" spans="1:16" ht="197.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>159</v>
@@ -5562,7 +5559,7 @@
         <v>136</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>140</v>
@@ -5591,7 +5588,7 @@
     </row>
     <row r="9" spans="1:16" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>47</v>
@@ -5600,7 +5597,7 @@
         <v>137</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>163</v>
@@ -5618,7 +5615,7 @@
         <v>142</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L9" s="2" t="s">
         <v>166</v>
@@ -5626,7 +5623,7 @@
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
       <c r="O9" s="2" t="s">
-        <v>594</v>
+        <v>588</v>
       </c>
       <c r="P9" s="2"/>
     </row>
@@ -5641,7 +5638,7 @@
         <v>137</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>167</v>
@@ -5659,10 +5656,10 @@
         <v>171</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
@@ -5673,7 +5670,7 @@
     </row>
     <row r="11" spans="1:16" ht="215.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>48</v>
@@ -5682,7 +5679,7 @@
         <v>137</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>172</v>
@@ -5700,10 +5697,10 @@
         <v>178</v>
       </c>
       <c r="J11" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="K11" s="5" t="s">
         <v>221</v>
-      </c>
-      <c r="K11" s="5" t="s">
-        <v>222</v>
       </c>
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
@@ -5724,7 +5721,7 @@
         <v>137</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>172</v>
@@ -5742,7 +5739,7 @@
         <v>181</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
@@ -5755,16 +5752,16 @@
     </row>
     <row r="13" spans="1:16" ht="333" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>245</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>246</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>137</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>184</v>
@@ -5782,7 +5779,7 @@
         <v>147</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K13" s="2" t="s">
         <v>187</v>
@@ -5801,7 +5798,7 @@
       </c>
       <c r="P13" s="2"/>
     </row>
-    <row r="14" spans="1:16" ht="178.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" ht="191.25" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>174</v>
       </c>
@@ -5812,7 +5809,7 @@
         <v>137</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>194</v>
@@ -5827,19 +5824,19 @@
         <v>141</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
       <c r="O14" s="2" t="s">
-        <v>542</v>
+        <v>536</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="178.5" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>195</v>
@@ -5848,7 +5845,7 @@
         <v>137</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>196</v>
@@ -5866,7 +5863,7 @@
         <v>147</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>197</v>
@@ -5883,16 +5880,16 @@
         <v>175</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>199</v>
+        <v>604</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>137</v>
       </c>
       <c r="D16" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>200</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>201</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>168</v>
@@ -5901,22 +5898,22 @@
         <v>145</v>
       </c>
       <c r="H16" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="J16" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="I16" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="J16" s="2" t="s">
+      <c r="K16" s="2" t="s">
         <v>230</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>231</v>
       </c>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
       <c r="O16" s="2" t="s">
-        <v>543</v>
+        <v>537</v>
       </c>
     </row>
   </sheetData>
@@ -6229,43 +6226,43 @@
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="13"/>
       <c r="B1" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="C1" s="11" t="s">
         <v>234</v>
       </c>
-      <c r="C1" s="11" t="s">
-        <v>235</v>
-      </c>
       <c r="D1" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>236</v>
+      </c>
+      <c r="F1" s="11" t="s">
         <v>238</v>
       </c>
-      <c r="E1" s="11" t="s">
-        <v>237</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>239</v>
-      </c>
       <c r="G1" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="H1" s="11" t="s">
         <v>241</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>242</v>
       </c>
       <c r="I1" s="11" t="s">
         <v>14</v>
       </c>
       <c r="J1" s="11" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="K1" s="11" t="s">
         <v>173</v>
       </c>
       <c r="L1" s="11" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="M1" s="11" t="s">
         <v>174</v>
       </c>
       <c r="N1" s="11" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O1" s="11" t="s">
         <v>175</v>
@@ -6278,30 +6275,30 @@
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
       <c r="D2" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E2" s="12"/>
       <c r="F2" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
       <c r="I2" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="J2" s="12"/>
       <c r="K2" s="12"/>
       <c r="L2" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="N2" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
@@ -6317,14 +6314,14 @@
       <c r="H3" s="12"/>
       <c r="I3" s="12"/>
       <c r="J3" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="K3" s="12"/>
       <c r="L3" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="M3" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="N3" s="12"/>
       <c r="O3" s="12"/>
@@ -6336,34 +6333,34 @@
       <c r="B4" s="12"/>
       <c r="C4" s="12"/>
       <c r="D4" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G4" s="12"/>
       <c r="H4" s="12"/>
       <c r="I4" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="J4" s="12"/>
       <c r="K4" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="L4" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="M4" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="N4" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="O4" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -6381,10 +6378,10 @@
       <c r="J5" s="12"/>
       <c r="K5" s="12"/>
       <c r="L5" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="M5" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="N5" s="12"/>
       <c r="O5" s="12"/>
@@ -6400,18 +6397,18 @@
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
       <c r="H6" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="I6" s="12"/>
       <c r="J6" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="K6" s="12"/>
       <c r="L6" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="M6" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="N6" s="12"/>
       <c r="O6" s="12"/>
@@ -6423,30 +6420,30 @@
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
       <c r="D7" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E7" s="12"/>
       <c r="F7" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>
       <c r="I7" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="J7" s="12"/>
       <c r="K7" s="12"/>
       <c r="L7" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="M7" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="N7" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="O7" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
@@ -6459,17 +6456,17 @@
       <c r="E8" s="12"/>
       <c r="F8" s="12"/>
       <c r="G8" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
       <c r="J8" s="12"/>
       <c r="K8" s="12"/>
       <c r="L8" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="M8" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="N8" s="12"/>
       <c r="O8" s="12"/>
@@ -6481,30 +6478,30 @@
       <c r="B9" s="12"/>
       <c r="C9" s="12"/>
       <c r="D9" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E9" s="12"/>
       <c r="F9" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
       <c r="I9" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="J9" s="12"/>
       <c r="K9" s="12"/>
       <c r="L9" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="M9" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="N9" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="O9" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
@@ -6512,10 +6509,10 @@
         <v>11</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
@@ -6526,7 +6523,7 @@
       <c r="J10" s="12"/>
       <c r="K10" s="12"/>
       <c r="L10" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="M10" s="12"/>
       <c r="N10" s="12"/>
@@ -6541,8 +6538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A214DC92-F9FF-4B22-82D2-C12543A136EC}">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6579,7 +6576,7 @@
         <v>132</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -6593,7 +6590,7 @@
         <v>132</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -6607,7 +6604,7 @@
         <v>132</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -6621,7 +6618,7 @@
         <v>132</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -6635,7 +6632,7 @@
         <v>132</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -6649,7 +6646,7 @@
         <v>132</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
@@ -6663,7 +6660,7 @@
         <v>133</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
@@ -6677,7 +6674,7 @@
         <v>133</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
@@ -6691,7 +6688,7 @@
         <v>133</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>272</v>
+        <v>599</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
@@ -6705,7 +6702,7 @@
         <v>133</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
@@ -6719,7 +6716,7 @@
         <v>133</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
@@ -6730,10 +6727,10 @@
         <v>131</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -6744,10 +6741,10 @@
         <v>131</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -6758,10 +6755,10 @@
         <v>131</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -6772,10 +6769,10 @@
         <v>131</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -6786,10 +6783,10 @@
         <v>131</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>279</v>
+        <v>600</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -6800,10 +6797,10 @@
         <v>131</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
@@ -6814,10 +6811,10 @@
         <v>135</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -6828,10 +6825,10 @@
         <v>135</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
@@ -6842,10 +6839,10 @@
         <v>131</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -6856,10 +6853,10 @@
         <v>135</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -6870,10 +6867,10 @@
         <v>131</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -6884,416 +6881,416 @@
         <v>131</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B25" s="9" t="s">
         <v>131</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A26" s="9" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B26" s="9" t="s">
         <v>135</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B27" s="9" t="s">
         <v>135</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B28" s="9" t="s">
         <v>135</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A29" s="9" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B29" s="9" t="s">
         <v>131</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B30" s="9" t="s">
         <v>131</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B31" s="9" t="s">
         <v>131</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B32" s="9" t="s">
         <v>135</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B33" s="9" t="s">
         <v>135</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A34" s="9" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B34" s="9" t="s">
         <v>135</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A35" s="9" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B35" s="9" t="s">
         <v>131</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A36" s="9" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B36" s="9" t="s">
         <v>135</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A37" s="9" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B37" s="9" t="s">
         <v>135</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B38" s="9" t="s">
         <v>131</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B39" s="9" t="s">
         <v>131</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A40" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B40" s="9" t="s">
         <v>131</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>302</v>
+        <v>601</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B41" s="9" t="s">
         <v>131</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B42" s="9" t="s">
         <v>135</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A43" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B43" s="9" t="s">
         <v>131</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>305</v>
+        <v>602</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A44" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B44" s="9" t="s">
         <v>131</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>306</v>
+        <v>603</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B45" s="9" t="s">
         <v>131</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A46" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B46" s="9" t="s">
         <v>131</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A47" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B47" s="9" t="s">
         <v>135</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B48" s="9" t="s">
         <v>131</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B49" s="9" t="s">
         <v>131</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B50" s="9" t="s">
         <v>131</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D50" s="9" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A51" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B51" s="9" t="s">
         <v>135</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D51" s="9" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B52" s="9" t="s">
         <v>131</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A53" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B53" s="9" t="s">
         <v>135</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D53" s="9" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
     </row>
   </sheetData>
@@ -7327,73 +7324,73 @@
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="34" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="D1" s="34"/>
       <c r="E1" s="34" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
       <c r="F1" s="34"/>
       <c r="G1" s="2" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>498</v>
+        <v>492</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
-        <v>479</v>
+        <v>473</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>478</v>
+        <v>472</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>455</v>
+        <v>449</v>
       </c>
       <c r="D2" s="23" t="s">
+        <v>448</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>450</v>
+      </c>
+      <c r="F2" s="23" t="s">
+        <v>451</v>
+      </c>
+      <c r="G2" s="23" t="s">
+        <v>452</v>
+      </c>
+      <c r="H2" s="23" t="s">
+        <v>453</v>
+      </c>
+      <c r="I2" s="23" t="s">
         <v>454</v>
       </c>
-      <c r="E2" s="23" t="s">
-        <v>456</v>
-      </c>
-      <c r="F2" s="23" t="s">
-        <v>457</v>
-      </c>
-      <c r="G2" s="23" t="s">
-        <v>458</v>
-      </c>
-      <c r="H2" s="23" t="s">
-        <v>459</v>
-      </c>
-      <c r="I2" s="23" t="s">
-        <v>460</v>
-      </c>
       <c r="J2" s="28" t="s">
-        <v>499</v>
+        <v>493</v>
       </c>
       <c r="K2" s="28" t="s">
-        <v>500</v>
+        <v>494</v>
       </c>
       <c r="L2" s="28" t="s">
-        <v>501</v>
+        <v>495</v>
       </c>
       <c r="M2" s="28" t="s">
-        <v>502</v>
+        <v>496</v>
       </c>
       <c r="N2" s="28" t="s">
-        <v>503</v>
+        <v>497</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
       <c r="C3" s="25">
         <v>102687.76054053067</v>
@@ -7408,36 +7405,36 @@
         <v>0</v>
       </c>
       <c r="G3" s="24" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="H3" s="26" t="s">
         <v>12</v>
       </c>
       <c r="I3" s="27" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
       <c r="J3" s="24" t="s">
+        <v>498</v>
+      </c>
+      <c r="K3" s="24" t="s">
+        <v>503</v>
+      </c>
+      <c r="L3" s="24" t="s">
         <v>504</v>
       </c>
-      <c r="K3" s="24" t="s">
-        <v>509</v>
-      </c>
-      <c r="L3" s="24" t="s">
-        <v>510</v>
-      </c>
       <c r="M3" s="24" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="N3" s="24" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="24" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="C4" s="25">
         <v>28245.512550017502</v>
@@ -7452,36 +7449,36 @@
         <v>2</v>
       </c>
       <c r="G4" s="24" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="H4" s="26" t="s">
         <v>12</v>
       </c>
       <c r="I4" s="27" t="s">
-        <v>464</v>
+        <v>458</v>
       </c>
       <c r="J4" s="24" t="s">
+        <v>498</v>
+      </c>
+      <c r="K4" s="24" t="s">
+        <v>503</v>
+      </c>
+      <c r="L4" s="24" t="s">
         <v>504</v>
       </c>
-      <c r="K4" s="24" t="s">
-        <v>509</v>
-      </c>
-      <c r="L4" s="24" t="s">
-        <v>510</v>
-      </c>
       <c r="M4" s="24" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="N4" s="24" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="24" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="C5" s="25">
         <v>514994.41648738808</v>
@@ -7496,36 +7493,36 @@
         <v>5</v>
       </c>
       <c r="G5" s="24" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="H5" s="26" t="s">
         <v>12</v>
       </c>
       <c r="I5" s="27" t="s">
-        <v>465</v>
+        <v>459</v>
       </c>
       <c r="J5" s="24" t="s">
+        <v>498</v>
+      </c>
+      <c r="K5" s="24" t="s">
+        <v>503</v>
+      </c>
+      <c r="L5" s="24" t="s">
         <v>504</v>
       </c>
-      <c r="K5" s="24" t="s">
-        <v>509</v>
-      </c>
-      <c r="L5" s="24" t="s">
-        <v>510</v>
-      </c>
       <c r="M5" s="24" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="N5" s="24" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="24" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="C6" s="25">
         <v>86869.842891781722</v>
@@ -7540,36 +7537,36 @@
         <v>19</v>
       </c>
       <c r="G6" s="24" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
       <c r="H6" s="26" t="s">
         <v>12</v>
       </c>
       <c r="I6" s="27" t="s">
-        <v>466</v>
+        <v>460</v>
       </c>
       <c r="J6" s="24" t="s">
+        <v>498</v>
+      </c>
+      <c r="K6" s="24" t="s">
+        <v>503</v>
+      </c>
+      <c r="L6" s="24" t="s">
         <v>504</v>
       </c>
-      <c r="K6" s="24" t="s">
-        <v>509</v>
-      </c>
-      <c r="L6" s="24" t="s">
-        <v>510</v>
-      </c>
       <c r="M6" s="24" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="N6" s="24" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="24" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="C7" s="25">
         <v>15833.086291840766</v>
@@ -7590,27 +7587,27 @@
         <v>159.50488000000001</v>
       </c>
       <c r="I7" s="27" t="s">
-        <v>467</v>
+        <v>461</v>
       </c>
       <c r="J7" s="24" t="s">
+        <v>498</v>
+      </c>
+      <c r="K7" s="24" t="s">
+        <v>503</v>
+      </c>
+      <c r="L7" s="24" t="s">
         <v>504</v>
       </c>
-      <c r="K7" s="24" t="s">
-        <v>509</v>
-      </c>
-      <c r="L7" s="24" t="s">
-        <v>510</v>
-      </c>
       <c r="M7" s="24" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="N7" s="24" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="24" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
       <c r="B8" s="24" t="s">
         <v>7</v>
@@ -7628,42 +7625,42 @@
         <v>93</v>
       </c>
       <c r="G8" s="24" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
       <c r="H8" s="26" t="s">
         <v>12</v>
       </c>
       <c r="I8" s="27" t="s">
-        <v>468</v>
+        <v>462</v>
       </c>
       <c r="J8" s="24" t="s">
+        <v>498</v>
+      </c>
+      <c r="K8" s="24" t="s">
+        <v>503</v>
+      </c>
+      <c r="L8" s="24" t="s">
         <v>504</v>
       </c>
-      <c r="K8" s="24" t="s">
-        <v>509</v>
-      </c>
-      <c r="L8" s="24" t="s">
-        <v>510</v>
-      </c>
       <c r="M8" s="24" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="N8" s="24" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="24" t="s">
-        <v>398</v>
+        <v>392</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>399</v>
+        <v>393</v>
       </c>
       <c r="C9" s="25">
         <v>0</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
       <c r="E9" s="24">
         <v>0</v>
@@ -7678,30 +7675,30 @@
         <v>214.441971</v>
       </c>
       <c r="I9" s="27" t="s">
-        <v>469</v>
+        <v>463</v>
       </c>
       <c r="J9" s="24" t="s">
+        <v>498</v>
+      </c>
+      <c r="K9" s="24" t="s">
+        <v>503</v>
+      </c>
+      <c r="L9" s="24" t="s">
         <v>504</v>
       </c>
-      <c r="K9" s="24" t="s">
-        <v>509</v>
-      </c>
-      <c r="L9" s="24" t="s">
-        <v>510</v>
-      </c>
       <c r="M9" s="24" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="N9" s="24" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="24" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="C10" s="25">
         <v>3982.9900478920035</v>
@@ -7716,42 +7713,42 @@
         <v>3</v>
       </c>
       <c r="G10" s="24" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="H10" s="26" t="s">
         <v>12</v>
       </c>
       <c r="I10" s="27" t="s">
-        <v>470</v>
+        <v>464</v>
       </c>
       <c r="J10" s="24" t="s">
+        <v>498</v>
+      </c>
+      <c r="K10" s="24" t="s">
+        <v>503</v>
+      </c>
+      <c r="L10" s="24" t="s">
         <v>504</v>
       </c>
-      <c r="K10" s="24" t="s">
-        <v>509</v>
-      </c>
-      <c r="L10" s="24" t="s">
-        <v>510</v>
-      </c>
       <c r="M10" s="24" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="N10" s="24" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="24" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="C11" s="25">
         <v>2097.1640005327972</v>
       </c>
       <c r="D11" s="25" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="E11" s="24">
         <v>0</v>
@@ -7766,30 +7763,30 @@
         <v>80.084551000000005</v>
       </c>
       <c r="I11" s="27" t="s">
-        <v>471</v>
+        <v>465</v>
       </c>
       <c r="J11" s="24" t="s">
+        <v>498</v>
+      </c>
+      <c r="K11" s="24" t="s">
+        <v>503</v>
+      </c>
+      <c r="L11" s="24" t="s">
         <v>504</v>
       </c>
-      <c r="K11" s="24" t="s">
-        <v>509</v>
-      </c>
-      <c r="L11" s="24" t="s">
-        <v>510</v>
-      </c>
       <c r="M11" s="24" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="N11" s="24" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="24" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>407</v>
+        <v>401</v>
       </c>
       <c r="C12" s="25">
         <v>123653.93022264706</v>
@@ -7804,33 +7801,33 @@
         <v>1</v>
       </c>
       <c r="G12" s="24" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="H12" s="26" t="s">
         <v>12</v>
       </c>
       <c r="I12" s="27" t="s">
-        <v>472</v>
+        <v>466</v>
       </c>
       <c r="J12" s="24" t="s">
+        <v>498</v>
+      </c>
+      <c r="K12" s="24" t="s">
+        <v>503</v>
+      </c>
+      <c r="L12" s="24" t="s">
         <v>504</v>
       </c>
-      <c r="K12" s="24" t="s">
-        <v>509</v>
-      </c>
-      <c r="L12" s="24" t="s">
-        <v>510</v>
-      </c>
       <c r="M12" s="24" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="N12" s="24" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="24" t="s">
-        <v>408</v>
+        <v>402</v>
       </c>
       <c r="B13" s="24" t="s">
         <v>8</v>
@@ -7848,36 +7845,36 @@
         <v>20</v>
       </c>
       <c r="G13" s="24" t="s">
-        <v>409</v>
+        <v>403</v>
       </c>
       <c r="H13" s="26" t="s">
         <v>12</v>
       </c>
       <c r="I13" s="27" t="s">
-        <v>473</v>
+        <v>467</v>
       </c>
       <c r="J13" s="24" t="s">
+        <v>498</v>
+      </c>
+      <c r="K13" s="24" t="s">
+        <v>503</v>
+      </c>
+      <c r="L13" s="24" t="s">
         <v>504</v>
       </c>
-      <c r="K13" s="24" t="s">
-        <v>509</v>
-      </c>
-      <c r="L13" s="24" t="s">
-        <v>510</v>
-      </c>
       <c r="M13" s="24" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="N13" s="24" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="24" t="s">
-        <v>410</v>
+        <v>404</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
       <c r="C14" s="25">
         <v>13804.443716258276</v>
@@ -7898,30 +7895,30 @@
         <v>12</v>
       </c>
       <c r="I14" s="27" t="s">
-        <v>474</v>
+        <v>468</v>
       </c>
       <c r="J14" s="24" t="s">
+        <v>498</v>
+      </c>
+      <c r="K14" s="24" t="s">
+        <v>503</v>
+      </c>
+      <c r="L14" s="24" t="s">
         <v>504</v>
       </c>
-      <c r="K14" s="24" t="s">
-        <v>509</v>
-      </c>
-      <c r="L14" s="24" t="s">
-        <v>510</v>
-      </c>
       <c r="M14" s="24" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="N14" s="24" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="24" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
       <c r="B15" s="24" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="C15" s="25">
         <v>0</v>
@@ -7936,36 +7933,36 @@
         <v>1</v>
       </c>
       <c r="G15" s="24" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="H15" s="26" t="s">
         <v>12</v>
       </c>
       <c r="I15" s="27" t="s">
-        <v>475</v>
+        <v>469</v>
       </c>
       <c r="J15" s="24" t="s">
+        <v>498</v>
+      </c>
+      <c r="K15" s="24" t="s">
+        <v>503</v>
+      </c>
+      <c r="L15" s="24" t="s">
         <v>504</v>
       </c>
-      <c r="K15" s="24" t="s">
-        <v>509</v>
-      </c>
-      <c r="L15" s="24" t="s">
-        <v>510</v>
-      </c>
       <c r="M15" s="24" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="N15" s="24" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="24" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
       <c r="B16" s="24" t="s">
-        <v>415</v>
+        <v>409</v>
       </c>
       <c r="C16" s="25">
         <v>176309.43933751195</v>
@@ -7980,36 +7977,36 @@
         <v>0</v>
       </c>
       <c r="G16" s="24" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="H16" s="26" t="s">
         <v>12</v>
       </c>
       <c r="I16" s="27" t="s">
-        <v>476</v>
+        <v>470</v>
       </c>
       <c r="J16" s="24" t="s">
+        <v>498</v>
+      </c>
+      <c r="K16" s="24" t="s">
+        <v>503</v>
+      </c>
+      <c r="L16" s="24" t="s">
         <v>504</v>
       </c>
-      <c r="K16" s="24" t="s">
-        <v>509</v>
-      </c>
-      <c r="L16" s="24" t="s">
-        <v>510</v>
-      </c>
       <c r="M16" s="24" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="N16" s="24" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="24" t="s">
-        <v>416</v>
+        <v>410</v>
       </c>
       <c r="B17" s="24" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
       <c r="C17" s="25">
         <v>50841.820075831536</v>
@@ -8030,30 +8027,30 @@
         <v>12</v>
       </c>
       <c r="I17" s="27" t="s">
-        <v>477</v>
+        <v>471</v>
       </c>
       <c r="J17" s="24" t="s">
-        <v>506</v>
+        <v>500</v>
       </c>
       <c r="K17" s="24" t="s">
-        <v>509</v>
+        <v>503</v>
       </c>
       <c r="L17" s="24" t="s">
-        <v>510</v>
+        <v>504</v>
       </c>
       <c r="M17" s="24" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="N17" s="24" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="24" t="s">
-        <v>418</v>
+        <v>412</v>
       </c>
       <c r="B18" s="24" t="s">
-        <v>419</v>
+        <v>413</v>
       </c>
       <c r="C18" s="25">
         <v>27966.147643374599</v>
@@ -8074,30 +8071,30 @@
         <v>12</v>
       </c>
       <c r="I18" s="27" t="s">
-        <v>480</v>
+        <v>474</v>
       </c>
       <c r="J18" s="24" t="s">
-        <v>506</v>
+        <v>500</v>
       </c>
       <c r="K18" s="24" t="s">
-        <v>509</v>
+        <v>503</v>
       </c>
       <c r="L18" s="24" t="s">
-        <v>510</v>
+        <v>504</v>
       </c>
       <c r="M18" s="24" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="N18" s="24" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="24" t="s">
-        <v>420</v>
+        <v>414</v>
       </c>
       <c r="B19" s="24" t="s">
-        <v>421</v>
+        <v>415</v>
       </c>
       <c r="C19" s="25">
         <v>143817.34529670601</v>
@@ -8112,36 +8109,36 @@
         <v>4</v>
       </c>
       <c r="G19" s="24" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="H19" s="26" t="s">
         <v>12</v>
       </c>
       <c r="I19" s="27" t="s">
-        <v>481</v>
+        <v>475</v>
       </c>
       <c r="J19" s="24" t="s">
+        <v>498</v>
+      </c>
+      <c r="K19" s="24" t="s">
+        <v>503</v>
+      </c>
+      <c r="L19" s="24" t="s">
         <v>504</v>
       </c>
-      <c r="K19" s="24" t="s">
-        <v>509</v>
-      </c>
-      <c r="L19" s="24" t="s">
-        <v>510</v>
-      </c>
       <c r="M19" s="24" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="N19" s="24" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="24" t="s">
-        <v>422</v>
+        <v>416</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>423</v>
+        <v>417</v>
       </c>
       <c r="C20" s="25">
         <v>42147.136742444643</v>
@@ -8162,36 +8159,36 @@
         <v>12</v>
       </c>
       <c r="I20" s="27" t="s">
-        <v>482</v>
+        <v>476</v>
       </c>
       <c r="J20" s="24" t="s">
+        <v>498</v>
+      </c>
+      <c r="K20" s="24" t="s">
+        <v>503</v>
+      </c>
+      <c r="L20" s="24" t="s">
         <v>504</v>
       </c>
-      <c r="K20" s="24" t="s">
-        <v>509</v>
-      </c>
-      <c r="L20" s="24" t="s">
-        <v>510</v>
-      </c>
       <c r="M20" s="24" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="N20" s="24" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="24" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="B21" s="24" t="s">
-        <v>425</v>
+        <v>419</v>
       </c>
       <c r="C21" s="25">
         <v>99636.883371308024</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
       <c r="E21" s="24">
         <v>0</v>
@@ -8200,42 +8197,42 @@
         <v>0</v>
       </c>
       <c r="G21" s="24" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="H21" s="26" t="s">
         <v>12</v>
       </c>
       <c r="I21" s="27" t="s">
-        <v>483</v>
+        <v>477</v>
       </c>
       <c r="J21" s="24" t="s">
-        <v>506</v>
+        <v>500</v>
       </c>
       <c r="K21" s="24" t="s">
-        <v>509</v>
+        <v>503</v>
       </c>
       <c r="L21" s="24" t="s">
-        <v>510</v>
+        <v>504</v>
       </c>
       <c r="M21" s="24" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="N21" s="24" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="24" t="s">
-        <v>426</v>
+        <v>420</v>
       </c>
       <c r="B22" s="24" t="s">
-        <v>427</v>
+        <v>421</v>
       </c>
       <c r="C22" s="25">
         <v>5256.6903781170731</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="E22" s="24">
         <v>6</v>
@@ -8244,36 +8241,36 @@
         <v>2</v>
       </c>
       <c r="G22" s="24" t="s">
-        <v>409</v>
+        <v>403</v>
       </c>
       <c r="H22" s="26">
         <v>59.952992000000002</v>
       </c>
       <c r="I22" s="27" t="s">
-        <v>484</v>
+        <v>478</v>
       </c>
       <c r="J22" s="24" t="s">
+        <v>498</v>
+      </c>
+      <c r="K22" s="24" t="s">
+        <v>503</v>
+      </c>
+      <c r="L22" s="24" t="s">
         <v>504</v>
       </c>
-      <c r="K22" s="24" t="s">
-        <v>509</v>
-      </c>
-      <c r="L22" s="24" t="s">
-        <v>510</v>
-      </c>
       <c r="M22" s="24" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="N22" s="24" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="24" t="s">
-        <v>428</v>
+        <v>422</v>
       </c>
       <c r="B23" s="24" t="s">
-        <v>429</v>
+        <v>423</v>
       </c>
       <c r="C23" s="25">
         <v>29291.660047894893</v>
@@ -8294,36 +8291,36 @@
         <v>12</v>
       </c>
       <c r="I23" s="27" t="s">
-        <v>485</v>
+        <v>479</v>
       </c>
       <c r="J23" s="24" t="s">
+        <v>498</v>
+      </c>
+      <c r="K23" s="24" t="s">
+        <v>503</v>
+      </c>
+      <c r="L23" s="24" t="s">
         <v>504</v>
       </c>
-      <c r="K23" s="24" t="s">
-        <v>509</v>
-      </c>
-      <c r="L23" s="24" t="s">
-        <v>510</v>
-      </c>
       <c r="M23" s="24" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="N23" s="24" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="24" t="s">
-        <v>430</v>
+        <v>424</v>
       </c>
       <c r="B24" s="24" t="s">
-        <v>431</v>
+        <v>425</v>
       </c>
       <c r="C24" s="25">
         <v>7559.5180291508068</v>
       </c>
       <c r="D24" s="25" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="E24" s="24">
         <v>0</v>
@@ -8338,30 +8335,30 @@
         <v>129.84832399999999</v>
       </c>
       <c r="I24" s="27" t="s">
-        <v>486</v>
+        <v>480</v>
       </c>
       <c r="J24" s="24" t="s">
+        <v>498</v>
+      </c>
+      <c r="K24" s="24" t="s">
+        <v>503</v>
+      </c>
+      <c r="L24" s="24" t="s">
         <v>504</v>
       </c>
-      <c r="K24" s="24" t="s">
-        <v>509</v>
-      </c>
-      <c r="L24" s="24" t="s">
-        <v>510</v>
-      </c>
       <c r="M24" s="24" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="N24" s="24" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="24" t="s">
-        <v>432</v>
+        <v>426</v>
       </c>
       <c r="B25" s="24" t="s">
-        <v>433</v>
+        <v>427</v>
       </c>
       <c r="C25" s="25">
         <v>192895.02833307866</v>
@@ -8376,36 +8373,36 @@
         <v>1</v>
       </c>
       <c r="G25" s="24" t="s">
-        <v>409</v>
+        <v>403</v>
       </c>
       <c r="H25" s="26" t="s">
         <v>12</v>
       </c>
       <c r="I25" s="27" t="s">
-        <v>487</v>
+        <v>481</v>
       </c>
       <c r="J25" s="24" t="s">
+        <v>498</v>
+      </c>
+      <c r="K25" s="24" t="s">
+        <v>503</v>
+      </c>
+      <c r="L25" s="24" t="s">
         <v>504</v>
       </c>
-      <c r="K25" s="24" t="s">
-        <v>509</v>
-      </c>
-      <c r="L25" s="24" t="s">
-        <v>510</v>
-      </c>
       <c r="M25" s="24" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="N25" s="24" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="24" t="s">
-        <v>434</v>
+        <v>428</v>
       </c>
       <c r="B26" s="24" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
       <c r="C26" s="25">
         <v>151622.74756959747</v>
@@ -8420,36 +8417,36 @@
         <v>0</v>
       </c>
       <c r="G26" s="24" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="H26" s="26" t="s">
         <v>12</v>
       </c>
       <c r="I26" s="27" t="s">
-        <v>488</v>
+        <v>482</v>
       </c>
       <c r="J26" s="24" t="s">
+        <v>498</v>
+      </c>
+      <c r="K26" s="24" t="s">
+        <v>503</v>
+      </c>
+      <c r="L26" s="24" t="s">
         <v>504</v>
       </c>
-      <c r="K26" s="24" t="s">
-        <v>509</v>
-      </c>
-      <c r="L26" s="24" t="s">
-        <v>510</v>
-      </c>
       <c r="M26" s="24" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="N26" s="24" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="24" t="s">
-        <v>436</v>
+        <v>430</v>
       </c>
       <c r="B27" s="24" t="s">
-        <v>437</v>
+        <v>431</v>
       </c>
       <c r="C27" s="25">
         <v>53182.742412075226</v>
@@ -8464,33 +8461,33 @@
         <v>3</v>
       </c>
       <c r="G27" s="24" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="H27" s="26" t="s">
         <v>12</v>
       </c>
       <c r="I27" s="27" t="s">
-        <v>489</v>
+        <v>483</v>
       </c>
       <c r="J27" s="24" t="s">
+        <v>498</v>
+      </c>
+      <c r="K27" s="24" t="s">
+        <v>503</v>
+      </c>
+      <c r="L27" s="24" t="s">
         <v>504</v>
       </c>
-      <c r="K27" s="24" t="s">
-        <v>509</v>
-      </c>
-      <c r="L27" s="24" t="s">
-        <v>510</v>
-      </c>
       <c r="M27" s="24" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="N27" s="24" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="24" t="s">
-        <v>438</v>
+        <v>432</v>
       </c>
       <c r="B28" s="24" t="s">
         <v>6</v>
@@ -8499,7 +8496,7 @@
         <v>35393.799778929817</v>
       </c>
       <c r="D28" s="25" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="E28" s="24">
         <v>0</v>
@@ -8514,36 +8511,36 @@
         <v>122.662285</v>
       </c>
       <c r="I28" s="27" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="J28" s="24" t="s">
+        <v>498</v>
+      </c>
+      <c r="K28" s="24" t="s">
+        <v>503</v>
+      </c>
+      <c r="L28" s="24" t="s">
         <v>504</v>
       </c>
-      <c r="K28" s="24" t="s">
-        <v>509</v>
-      </c>
-      <c r="L28" s="24" t="s">
-        <v>510</v>
-      </c>
       <c r="M28" s="24" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="N28" s="24" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="24" t="s">
-        <v>439</v>
+        <v>433</v>
       </c>
       <c r="B29" s="24" t="s">
-        <v>440</v>
+        <v>434</v>
       </c>
       <c r="C29" s="25">
         <v>2375.3911489586781</v>
       </c>
       <c r="D29" s="25" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="E29" s="24">
         <v>0</v>
@@ -8552,42 +8549,42 @@
         <v>2</v>
       </c>
       <c r="G29" s="24" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="H29" s="26">
         <v>70.495289999999997</v>
       </c>
       <c r="I29" s="27" t="s">
-        <v>491</v>
+        <v>485</v>
       </c>
       <c r="J29" s="24" t="s">
+        <v>498</v>
+      </c>
+      <c r="K29" s="24" t="s">
+        <v>503</v>
+      </c>
+      <c r="L29" s="24" t="s">
         <v>504</v>
       </c>
-      <c r="K29" s="24" t="s">
-        <v>509</v>
-      </c>
-      <c r="L29" s="24" t="s">
-        <v>510</v>
-      </c>
       <c r="M29" s="24" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="N29" s="24" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="24" t="s">
-        <v>441</v>
+        <v>435</v>
       </c>
       <c r="B30" s="24" t="s">
-        <v>442</v>
+        <v>436</v>
       </c>
       <c r="C30" s="25">
         <v>6534.4815097404735</v>
       </c>
       <c r="D30" s="25" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
       <c r="E30" s="24">
         <v>0</v>
@@ -8596,36 +8593,36 @@
         <v>7</v>
       </c>
       <c r="G30" s="24" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="H30" s="26" t="s">
         <v>12</v>
       </c>
       <c r="I30" s="27" t="s">
-        <v>492</v>
+        <v>486</v>
       </c>
       <c r="J30" s="24" t="s">
+        <v>498</v>
+      </c>
+      <c r="K30" s="24" t="s">
+        <v>503</v>
+      </c>
+      <c r="L30" s="24" t="s">
         <v>504</v>
       </c>
-      <c r="K30" s="24" t="s">
-        <v>509</v>
-      </c>
-      <c r="L30" s="24" t="s">
-        <v>510</v>
-      </c>
       <c r="M30" s="24" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="N30" s="24" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="24" t="s">
-        <v>443</v>
+        <v>437</v>
       </c>
       <c r="B31" s="24" t="s">
-        <v>444</v>
+        <v>438</v>
       </c>
       <c r="C31" s="25">
         <v>17975.881159055345</v>
@@ -8646,30 +8643,30 @@
         <v>12</v>
       </c>
       <c r="I31" s="27" t="s">
-        <v>493</v>
+        <v>487</v>
       </c>
       <c r="J31" s="24" t="s">
+        <v>498</v>
+      </c>
+      <c r="K31" s="24" t="s">
+        <v>503</v>
+      </c>
+      <c r="L31" s="24" t="s">
         <v>504</v>
       </c>
-      <c r="K31" s="24" t="s">
-        <v>509</v>
-      </c>
-      <c r="L31" s="24" t="s">
-        <v>510</v>
-      </c>
       <c r="M31" s="24" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="N31" s="24" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="24" t="s">
-        <v>445</v>
+        <v>439</v>
       </c>
       <c r="B32" s="24" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
       <c r="C32" s="25">
         <v>1234.3228021367959</v>
@@ -8684,36 +8681,36 @@
         <v>2</v>
       </c>
       <c r="G32" s="24" t="s">
-        <v>409</v>
+        <v>403</v>
       </c>
       <c r="H32" s="26" t="s">
         <v>12</v>
       </c>
       <c r="I32" s="27" t="s">
-        <v>494</v>
+        <v>488</v>
       </c>
       <c r="J32" s="24" t="s">
+        <v>498</v>
+      </c>
+      <c r="K32" s="24" t="s">
+        <v>503</v>
+      </c>
+      <c r="L32" s="24" t="s">
         <v>504</v>
       </c>
-      <c r="K32" s="24" t="s">
-        <v>509</v>
-      </c>
-      <c r="L32" s="24" t="s">
-        <v>510</v>
-      </c>
       <c r="M32" s="24" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="N32" s="24" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
     </row>
     <row r="33" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="24" t="s">
-        <v>447</v>
+        <v>441</v>
       </c>
       <c r="B33" s="24" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="C33" s="25">
         <v>9001.3629494330653</v>
@@ -8728,36 +8725,36 @@
         <v>0</v>
       </c>
       <c r="G33" s="24" t="s">
-        <v>409</v>
+        <v>403</v>
       </c>
       <c r="H33" s="26" t="s">
         <v>12</v>
       </c>
       <c r="I33" s="27" t="s">
-        <v>495</v>
+        <v>489</v>
       </c>
       <c r="J33" s="24" t="s">
+        <v>498</v>
+      </c>
+      <c r="K33" s="24" t="s">
+        <v>503</v>
+      </c>
+      <c r="L33" s="24" t="s">
         <v>504</v>
       </c>
-      <c r="K33" s="24" t="s">
-        <v>509</v>
-      </c>
-      <c r="L33" s="24" t="s">
-        <v>510</v>
-      </c>
       <c r="M33" s="24" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="N33" s="24" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
     </row>
     <row r="34" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="24" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="B34" s="24" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="C34" s="25">
         <v>378.04871500147641</v>
@@ -8778,22 +8775,22 @@
         <v>12</v>
       </c>
       <c r="I34" s="27" t="s">
-        <v>495</v>
+        <v>489</v>
       </c>
       <c r="J34" s="24" t="s">
-        <v>506</v>
+        <v>500</v>
       </c>
       <c r="K34" s="24" t="s">
-        <v>509</v>
+        <v>503</v>
       </c>
       <c r="L34" s="24" t="s">
-        <v>510</v>
+        <v>504</v>
       </c>
       <c r="M34" s="24" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="N34" s="24" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
     </row>
     <row r="35" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -8801,7 +8798,7 @@
         <v>11</v>
       </c>
       <c r="B35" s="24" t="s">
-        <v>451</v>
+        <v>445</v>
       </c>
       <c r="C35" s="25">
         <v>544110.99319185445</v>
@@ -8816,42 +8813,42 @@
         <v>8</v>
       </c>
       <c r="G35" s="24" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
       <c r="H35" s="26">
         <v>68.122753000000003</v>
       </c>
       <c r="I35" s="27" t="s">
-        <v>496</v>
+        <v>490</v>
       </c>
       <c r="J35" s="24" t="s">
+        <v>498</v>
+      </c>
+      <c r="K35" s="24" t="s">
+        <v>503</v>
+      </c>
+      <c r="L35" s="24" t="s">
         <v>504</v>
       </c>
-      <c r="K35" s="24" t="s">
-        <v>509</v>
-      </c>
-      <c r="L35" s="24" t="s">
-        <v>510</v>
-      </c>
       <c r="M35" s="24" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="N35" s="24" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
     </row>
     <row r="36" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="24" t="s">
-        <v>452</v>
+        <v>446</v>
       </c>
       <c r="B36" s="24" t="s">
-        <v>453</v>
+        <v>447</v>
       </c>
       <c r="C36" s="25">
         <v>8842.3521510548053</v>
       </c>
       <c r="D36" s="25" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
       <c r="E36" s="24">
         <v>0</v>
@@ -8860,28 +8857,28 @@
         <v>20</v>
       </c>
       <c r="G36" s="24" t="s">
-        <v>409</v>
+        <v>403</v>
       </c>
       <c r="H36" s="26" t="s">
         <v>12</v>
       </c>
       <c r="I36" s="27" t="s">
-        <v>497</v>
+        <v>491</v>
       </c>
       <c r="J36" s="24" t="s">
+        <v>498</v>
+      </c>
+      <c r="K36" s="24" t="s">
+        <v>503</v>
+      </c>
+      <c r="L36" s="24" t="s">
         <v>504</v>
       </c>
-      <c r="K36" s="24" t="s">
-        <v>509</v>
-      </c>
-      <c r="L36" s="24" t="s">
-        <v>510</v>
-      </c>
       <c r="M36" s="24" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="N36" s="24" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
@@ -9062,7 +9059,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A08C373-50CB-424A-939A-38A53453958B}">
   <dimension ref="A1:R11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
@@ -9108,10 +9105,10 @@
     </row>
     <row r="2" spans="1:18" ht="51" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
-        <v>479</v>
+        <v>473</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>478</v>
+        <v>472</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>115</v>
@@ -9141,30 +9138,30 @@
         <v>117</v>
       </c>
       <c r="L2" s="17" t="s">
-        <v>604</v>
+        <v>598</v>
       </c>
       <c r="M2" s="17" t="s">
-        <v>544</v>
+        <v>538</v>
       </c>
       <c r="N2" s="17" t="s">
-        <v>545</v>
+        <v>539</v>
       </c>
       <c r="O2" s="17" t="s">
-        <v>546</v>
+        <v>540</v>
       </c>
       <c r="P2" s="17" t="s">
-        <v>547</v>
+        <v>541</v>
       </c>
       <c r="Q2" s="17" t="s">
-        <v>548</v>
+        <v>542</v>
       </c>
       <c r="R2" s="17" t="s">
-        <v>549</v>
+        <v>543</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="267.75" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
-        <v>522</v>
+        <v>516</v>
       </c>
       <c r="B3" s="16" t="s">
         <v>3</v>
@@ -9176,13 +9173,13 @@
         <v>34</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="F3" s="15" t="s">
         <v>118</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="H3" s="16" t="s">
         <v>119</v>
@@ -9191,28 +9188,28 @@
         <v>120</v>
       </c>
       <c r="J3" s="15" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="K3" s="16" t="s">
         <v>121</v>
       </c>
       <c r="M3" s="17" t="s">
+        <v>544</v>
+      </c>
+      <c r="N3" s="17" t="s">
+        <v>544</v>
+      </c>
+      <c r="O3" s="17" t="s">
+        <v>547</v>
+      </c>
+      <c r="P3" s="17" t="s">
         <v>550</v>
       </c>
-      <c r="N3" s="17" t="s">
-        <v>550</v>
-      </c>
-      <c r="O3" s="17" t="s">
-        <v>553</v>
-      </c>
-      <c r="P3" s="17" t="s">
-        <v>556</v>
-      </c>
       <c r="Q3" s="17" t="s">
-        <v>560</v>
+        <v>554</v>
       </c>
       <c r="R3" s="17" t="s">
-        <v>563</v>
+        <v>557</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="293.25" x14ac:dyDescent="0.25">
@@ -9223,54 +9220,54 @@
         <v>4</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="H4" s="16" t="s">
         <v>34</v>
       </c>
       <c r="I4" s="15" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="J4" s="16" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="K4" s="15" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="L4" s="17" t="s">
-        <v>564</v>
+        <v>558</v>
       </c>
       <c r="M4" s="17" t="s">
-        <v>550</v>
+        <v>544</v>
       </c>
       <c r="N4" s="17" t="s">
-        <v>550</v>
+        <v>544</v>
       </c>
       <c r="P4" s="17" t="s">
-        <v>567</v>
+        <v>561</v>
       </c>
       <c r="Q4" s="17" t="s">
-        <v>560</v>
+        <v>554</v>
       </c>
       <c r="R4" s="17" t="s">
-        <v>568</v>
+        <v>562</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="178.5" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
-        <v>523</v>
+        <v>517</v>
       </c>
       <c r="B5" s="16" t="s">
         <v>5</v>
@@ -9279,48 +9276,48 @@
         <v>12</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="H5" s="16" t="s">
         <v>34</v>
       </c>
       <c r="I5" s="15" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="J5" s="15" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="K5" s="16" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="M5" s="17" t="s">
-        <v>550</v>
+        <v>544</v>
       </c>
       <c r="N5" s="17" t="s">
-        <v>550</v>
+        <v>544</v>
       </c>
       <c r="P5" s="17" t="s">
-        <v>569</v>
+        <v>563</v>
       </c>
       <c r="Q5" s="17" t="s">
-        <v>560</v>
+        <v>554</v>
       </c>
       <c r="R5" s="17" t="s">
-        <v>572</v>
+        <v>566</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="153" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
-        <v>438</v>
+        <v>432</v>
       </c>
       <c r="B6" s="16" t="s">
         <v>6</v>
@@ -9329,107 +9326,107 @@
         <v>12</v>
       </c>
       <c r="D6" s="15" t="s">
+        <v>326</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>327</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>328</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>329</v>
+      </c>
+      <c r="H6" s="16" t="s">
+        <v>330</v>
+      </c>
+      <c r="I6" s="15" t="s">
+        <v>331</v>
+      </c>
+      <c r="J6" s="15" t="s">
         <v>332</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="K6" s="16" t="s">
         <v>333</v>
       </c>
-      <c r="F6" s="16" t="s">
-        <v>334</v>
-      </c>
-      <c r="G6" s="16" t="s">
-        <v>335</v>
-      </c>
-      <c r="H6" s="16" t="s">
-        <v>336</v>
-      </c>
-      <c r="I6" s="15" t="s">
-        <v>337</v>
-      </c>
-      <c r="J6" s="15" t="s">
-        <v>338</v>
-      </c>
-      <c r="K6" s="16" t="s">
-        <v>339</v>
-      </c>
       <c r="M6" s="17" t="s">
-        <v>550</v>
+        <v>544</v>
       </c>
       <c r="N6" s="17" t="s">
-        <v>550</v>
+        <v>544</v>
       </c>
       <c r="P6" s="17" t="s">
-        <v>573</v>
+        <v>567</v>
       </c>
       <c r="Q6" s="17" t="s">
-        <v>560</v>
+        <v>554</v>
       </c>
       <c r="R6" s="17" t="s">
-        <v>563</v>
+        <v>557</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="242.25" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
       <c r="B7" s="16" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="G7" s="15" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="H7" s="16" t="s">
         <v>34</v>
       </c>
       <c r="I7" s="15" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="J7" s="15" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="K7" s="16" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="L7" s="17" t="s">
-        <v>576</v>
+        <v>570</v>
       </c>
       <c r="M7" s="17" t="s">
-        <v>550</v>
+        <v>544</v>
       </c>
       <c r="N7" s="17" t="s">
-        <v>550</v>
+        <v>544</v>
       </c>
       <c r="P7" s="17" t="s">
         <v>67</v>
       </c>
       <c r="Q7" s="17" t="s">
-        <v>560</v>
+        <v>554</v>
       </c>
       <c r="R7" s="17" t="s">
-        <v>579</v>
+        <v>573</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="255" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
-        <v>408</v>
+        <v>402</v>
       </c>
       <c r="B8" s="16" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="D8" s="16" t="s">
         <v>12</v>
@@ -9438,34 +9435,34 @@
         <v>12</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="G8" s="15" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="H8" s="16" t="s">
         <v>34</v>
       </c>
       <c r="I8" s="15" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="J8" s="15" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="K8" s="16" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="L8" s="17" t="s">
-        <v>580</v>
+        <v>574</v>
       </c>
       <c r="P8" s="17" t="s">
-        <v>580</v>
+        <v>574</v>
       </c>
       <c r="Q8" s="17" t="s">
-        <v>560</v>
+        <v>554</v>
       </c>
       <c r="R8" s="17" t="s">
-        <v>583</v>
+        <v>577</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="165.75" x14ac:dyDescent="0.25">
@@ -9476,52 +9473,52 @@
         <v>9</v>
       </c>
       <c r="C9" s="16" t="s">
+        <v>347</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>348</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>349</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>350</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>351</v>
+      </c>
+      <c r="H9" s="16" t="s">
+        <v>352</v>
+      </c>
+      <c r="I9" s="15" t="s">
         <v>353</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="J9" s="16" t="s">
         <v>354</v>
       </c>
-      <c r="E9" s="16" t="s">
+      <c r="K9" s="16" t="s">
         <v>355</v>
       </c>
-      <c r="F9" s="15" t="s">
-        <v>356</v>
-      </c>
-      <c r="G9" s="16" t="s">
-        <v>357</v>
-      </c>
-      <c r="H9" s="16" t="s">
-        <v>358</v>
-      </c>
-      <c r="I9" s="15" t="s">
-        <v>359</v>
-      </c>
-      <c r="J9" s="16" t="s">
-        <v>360</v>
-      </c>
-      <c r="K9" s="16" t="s">
-        <v>361</v>
-      </c>
       <c r="L9" s="17" t="s">
-        <v>584</v>
+        <v>578</v>
       </c>
       <c r="M9" s="17" t="s">
-        <v>550</v>
+        <v>544</v>
       </c>
       <c r="N9" s="17" t="s">
-        <v>550</v>
+        <v>544</v>
       </c>
       <c r="O9" s="17" t="s">
-        <v>591</v>
+        <v>585</v>
       </c>
       <c r="P9" s="17" t="s">
-        <v>593</v>
+        <v>587</v>
       </c>
       <c r="Q9" s="17" t="s">
-        <v>560</v>
+        <v>554</v>
       </c>
       <c r="R9" s="17" t="s">
-        <v>585</v>
+        <v>579</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="76.5" x14ac:dyDescent="0.25">
@@ -9532,49 +9529,49 @@
         <v>10</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="E10" s="16" t="s">
         <v>12</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="H10" s="16" t="s">
         <v>34</v>
       </c>
       <c r="I10" s="15" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="J10" s="15" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="K10" s="16" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="L10" s="17" t="s">
-        <v>595</v>
+        <v>589</v>
       </c>
       <c r="M10" s="17" t="s">
-        <v>550</v>
+        <v>544</v>
       </c>
       <c r="N10" s="17" t="s">
-        <v>550</v>
+        <v>544</v>
       </c>
       <c r="P10" s="17" t="s">
-        <v>595</v>
+        <v>589</v>
       </c>
       <c r="Q10" s="17" t="s">
-        <v>560</v>
+        <v>554</v>
       </c>
       <c r="R10" s="17" t="s">
-        <v>595</v>
+        <v>589</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="114.75" x14ac:dyDescent="0.25">
@@ -9585,52 +9582,52 @@
         <v>11</v>
       </c>
       <c r="C11" s="16" t="s">
+        <v>363</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>364</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>365</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>366</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>367</v>
+      </c>
+      <c r="H11" s="16" t="s">
+        <v>368</v>
+      </c>
+      <c r="I11" s="15" t="s">
         <v>369</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="J11" s="15" t="s">
         <v>370</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="K11" s="16" t="s">
         <v>371</v>
       </c>
-      <c r="F11" s="15" t="s">
-        <v>372</v>
-      </c>
-      <c r="G11" s="16" t="s">
-        <v>373</v>
-      </c>
-      <c r="H11" s="16" t="s">
-        <v>374</v>
-      </c>
-      <c r="I11" s="15" t="s">
-        <v>375</v>
-      </c>
-      <c r="J11" s="15" t="s">
-        <v>376</v>
-      </c>
-      <c r="K11" s="16" t="s">
-        <v>377</v>
-      </c>
       <c r="L11" s="17" t="s">
-        <v>598</v>
+        <v>592</v>
       </c>
       <c r="M11" s="17" t="s">
-        <v>550</v>
+        <v>544</v>
       </c>
       <c r="N11" s="17" t="s">
-        <v>550</v>
+        <v>544</v>
       </c>
       <c r="O11" s="17" t="s">
-        <v>598</v>
+        <v>592</v>
       </c>
       <c r="P11" s="17" t="s">
-        <v>602</v>
+        <v>596</v>
       </c>
       <c r="Q11" s="17" t="s">
-        <v>560</v>
+        <v>554</v>
       </c>
       <c r="R11" s="17" t="s">
-        <v>560</v>
+        <v>554</v>
       </c>
     </row>
   </sheetData>
@@ -9671,7 +9668,7 @@
         <v>51</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>524</v>
+        <v>518</v>
       </c>
       <c r="C2" s="32" t="s">
         <v>83</v>
@@ -9695,7 +9692,7 @@
         <v>53</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>525</v>
+        <v>519</v>
       </c>
       <c r="C4" s="32" t="s">
         <v>85</v>
@@ -9734,7 +9731,7 @@
         <v>56</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>526</v>
+        <v>520</v>
       </c>
       <c r="C7" s="32" t="s">
         <v>88</v>
@@ -9747,7 +9744,7 @@
         <v>57</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>527</v>
+        <v>521</v>
       </c>
       <c r="C8" s="32" t="s">
         <v>89</v>
@@ -9760,7 +9757,7 @@
         <v>58</v>
       </c>
       <c r="B9" s="30" t="s">
-        <v>528</v>
+        <v>522</v>
       </c>
       <c r="C9" s="32" t="s">
         <v>90</v>
@@ -9773,7 +9770,7 @@
         <v>59</v>
       </c>
       <c r="B10" s="30" t="s">
-        <v>529</v>
+        <v>523</v>
       </c>
       <c r="C10" s="32" t="s">
         <v>91</v>
@@ -9825,7 +9822,7 @@
         <v>63</v>
       </c>
       <c r="B14" s="30" t="s">
-        <v>530</v>
+        <v>524</v>
       </c>
       <c r="C14" s="32" t="s">
         <v>95</v>
@@ -9864,7 +9861,7 @@
         <v>66</v>
       </c>
       <c r="B17" s="30" t="s">
-        <v>531</v>
+        <v>525</v>
       </c>
       <c r="C17" s="32" t="s">
         <v>98</v>
@@ -9913,10 +9910,10 @@
     </row>
     <row r="21" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="30" t="s">
-        <v>591</v>
+        <v>585</v>
       </c>
       <c r="B21" s="30" t="s">
-        <v>592</v>
+        <v>586</v>
       </c>
       <c r="C21" s="32" t="s">
         <v>102</v>
@@ -9939,10 +9936,10 @@
     </row>
     <row r="23" spans="1:6" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="30" t="s">
-        <v>597</v>
+        <v>591</v>
       </c>
       <c r="B23" s="30" t="s">
-        <v>599</v>
+        <v>593</v>
       </c>
       <c r="C23" s="32" t="s">
         <v>104</v>
@@ -9952,10 +9949,10 @@
     </row>
     <row r="24" spans="1:6" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="30" t="s">
-        <v>532</v>
+        <v>526</v>
       </c>
       <c r="B24" s="30" t="s">
-        <v>533</v>
+        <v>527</v>
       </c>
       <c r="C24" s="32" t="s">
         <v>105</v>
@@ -9965,13 +9962,13 @@
     </row>
     <row r="25" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A25" s="30" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="B25" s="30" t="s">
-        <v>534</v>
+        <v>528</v>
       </c>
       <c r="C25" s="32" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="D25" s="30"/>
       <c r="E25" s="30"/>
@@ -9979,13 +9976,13 @@
     </row>
     <row r="26" spans="1:6" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="30" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
       <c r="B26" s="30" t="s">
-        <v>535</v>
+        <v>529</v>
       </c>
       <c r="C26" s="32" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="D26" s="30"/>
       <c r="E26" s="30"/>
@@ -9993,208 +9990,208 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="24" t="s">
-        <v>504</v>
+        <v>498</v>
       </c>
       <c r="B27" s="24" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
       <c r="C27" s="24" t="s">
-        <v>505</v>
+        <v>499</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="30" t="s">
-        <v>506</v>
+        <v>500</v>
       </c>
       <c r="B28" s="24" t="s">
-        <v>537</v>
+        <v>531</v>
       </c>
       <c r="C28" s="24" t="s">
-        <v>507</v>
+        <v>501</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="30" t="s">
-        <v>509</v>
+        <v>503</v>
       </c>
       <c r="B29" s="24" t="s">
-        <v>538</v>
+        <v>532</v>
       </c>
       <c r="C29" s="24" t="s">
-        <v>508</v>
+        <v>502</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A30" s="30" t="s">
-        <v>510</v>
+        <v>504</v>
       </c>
       <c r="B30" s="24" t="s">
-        <v>511</v>
+        <v>505</v>
       </c>
       <c r="C30" s="24" t="s">
-        <v>512</v>
+        <v>506</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A31" s="30" t="s">
-        <v>513</v>
+        <v>507</v>
       </c>
       <c r="B31" s="24" t="s">
-        <v>514</v>
+        <v>508</v>
       </c>
       <c r="C31" s="24" t="s">
-        <v>515</v>
+        <v>509</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A32" s="30" t="s">
-        <v>516</v>
+        <v>510</v>
       </c>
       <c r="B32" s="24" t="s">
-        <v>517</v>
+        <v>511</v>
       </c>
       <c r="C32" s="24" t="s">
-        <v>518</v>
+        <v>512</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="30" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
       <c r="B33" s="24" t="s">
-        <v>539</v>
+        <v>533</v>
       </c>
       <c r="C33" s="24" t="s">
-        <v>520</v>
+        <v>514</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A34" s="30" t="s">
-        <v>550</v>
+        <v>544</v>
       </c>
       <c r="B34" s="24" t="s">
-        <v>551</v>
+        <v>545</v>
       </c>
       <c r="C34" s="24" t="s">
-        <v>552</v>
+        <v>546</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="24" t="s">
-        <v>553</v>
+        <v>547</v>
       </c>
       <c r="B35" s="24" t="s">
-        <v>554</v>
+        <v>548</v>
       </c>
       <c r="C35" s="24" t="s">
-        <v>555</v>
+        <v>549</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="30" t="s">
-        <v>557</v>
+        <v>551</v>
       </c>
       <c r="B36" s="24" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
       <c r="C36" s="24" t="s">
-        <v>558</v>
+        <v>552</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A37" s="30" t="s">
-        <v>560</v>
+        <v>554</v>
       </c>
       <c r="B37" s="24" t="s">
-        <v>561</v>
+        <v>555</v>
       </c>
       <c r="C37" s="24" t="s">
-        <v>562</v>
+        <v>556</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="30" t="s">
-        <v>564</v>
+        <v>558</v>
       </c>
       <c r="B38" s="24" t="s">
-        <v>565</v>
+        <v>559</v>
       </c>
       <c r="C38" s="24" t="s">
-        <v>566</v>
+        <v>560</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="24" t="s">
-        <v>569</v>
+        <v>563</v>
       </c>
       <c r="B39" s="24" t="s">
-        <v>570</v>
+        <v>564</v>
       </c>
       <c r="C39" s="24" t="s">
-        <v>571</v>
+        <v>565</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="30" t="s">
-        <v>573</v>
+        <v>567</v>
       </c>
       <c r="B40" s="24" t="s">
-        <v>574</v>
+        <v>568</v>
       </c>
       <c r="C40" s="24" t="s">
-        <v>575</v>
+        <v>569</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="30" t="s">
-        <v>576</v>
+        <v>570</v>
       </c>
       <c r="B41" s="24" t="s">
-        <v>577</v>
+        <v>571</v>
       </c>
       <c r="C41" s="24" t="s">
-        <v>578</v>
+        <v>572</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A42" s="30" t="s">
-        <v>580</v>
+        <v>574</v>
       </c>
       <c r="B42" s="24" t="s">
-        <v>581</v>
+        <v>575</v>
       </c>
       <c r="C42" s="24" t="s">
-        <v>582</v>
+        <v>576</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="30" t="s">
-        <v>584</v>
+        <v>578</v>
       </c>
       <c r="B43" s="24" t="s">
-        <v>587</v>
+        <v>581</v>
       </c>
       <c r="C43" s="33" t="s">
-        <v>586</v>
+        <v>580</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="30" t="s">
-        <v>588</v>
+        <v>582</v>
       </c>
       <c r="B44" s="24" t="s">
-        <v>589</v>
+        <v>583</v>
       </c>
       <c r="C44" s="24" t="s">
-        <v>590</v>
+        <v>584</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="30" t="s">
-        <v>595</v>
+        <v>589</v>
       </c>
       <c r="B45" s="24" t="s">
-        <v>596</v>
+        <v>590</v>
       </c>
       <c r="C45" s="24" t="s">
         <v>34</v>
@@ -10202,13 +10199,13 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="30" t="s">
-        <v>598</v>
+        <v>592</v>
       </c>
       <c r="B46" s="24" t="s">
-        <v>600</v>
+        <v>594</v>
       </c>
       <c r="C46" s="24" t="s">
-        <v>601</v>
+        <v>595</v>
       </c>
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.25">
@@ -10396,15 +10393,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100E2F0DF90B070FE43BFD707F72A4CD00B" ma:contentTypeVersion="15" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="8927d14e1bc908eae180c9caa4b5da89">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1bc94727-11e8-4443-b8f0-9215ff28e4bb" xmlns:ns3="cd34aed5-94da-4c30-bba3-37b78f4daae9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bb67c9392edae2d7a3a1d88d3e91258a" ns2:_="" ns3:_="">
     <xsd:import namespace="1bc94727-11e8-4443-b8f0-9215ff28e4bb"/>
@@ -10641,15 +10629,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22BF5C6F-88A2-47DA-9B5F-9FD29A58E304}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1143ECE1-9C35-446D-8A76-82388033D272}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10666,4 +10655,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22BF5C6F-88A2-47DA-9B5F-9FD29A58E304}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
import certification scheme formatting
</commit_message>
<xml_diff>
--- a/data/context_data.xlsx
+++ b/data/context_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m.haller\Documents\code\ptx-boa\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C18D647B-F47B-47A4-9ADF-E5D3A53F06E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A71EF7A0-9144-4C5D-90C7-83D39A3BC627}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D16C601B-E1D6-40C0-8CC1-80505BE1FBB6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{D16C601B-E1D6-40C0-8CC1-80505BE1FBB6}"/>
   </bookViews>
   <sheets>
     <sheet name="certification_schemes" sheetId="6" r:id="rId1"/>
@@ -1103,17 +1103,6 @@
 Is it possible to source it from the air (DAC) or from unavoidable emissions?</t>
   </si>
   <si>
-    <t xml:space="preserve">**If sourcing CO2 from the air (DAC)**, further questions regarding RES-E and land resources should be considered.
-- How are **additional energy demands of DAC** sourced (preferably from RES-E plants or excess heat)? 
-- Are there any **potential land conflicts** if deploying this technology?
-</t>
-  </si>
-  <si>
-    <t>**If sourcing CO2 from unavoidable process emissions or biogenic sources**: this should, preferably, only be a short term option.
-- What is the intended temporal scope of use of such CO2 sources? Are there **alternative sources in the long term**?
-- Are all established **sustainability criteria for biomass** met (e.g. related to risks of land use change and biodiversity)?</t>
-  </si>
-  <si>
     <t xml:space="preserve">Is the region affected by **water stress**? If yes, how is this issue addressed? </t>
   </si>
   <si>
@@ -1196,11 +1185,6 @@
   </si>
   <si>
     <t>(How) Can it be ensured that a **long-term demand for skilled labour** is generated and met with local workforce?</t>
-  </si>
-  <si>
-    <t>Where in the production chain do **health and safety risks** potentially occur? 
-- How can potential **risks be reduced to a minimum** and workers protected in the best possible way?
-- Are there mechanisms in place for **monitoring potential risks** as well as regular comprehensive audits?</t>
   </si>
   <si>
     <t>Does the supply country have a **national decarbonisation strategy (NDC)** which includes hydrogen and PtX production? (How) Does the planned PtX production fit into this?</t>
@@ -2172,6 +2156,21 @@
   </si>
   <si>
     <t>TÜV Süd CMS 70 (Green Hydrogen, Green Hydrogen+)</t>
+  </si>
+  <si>
+    <t>**If sourcing CO2 from the air (DAC)**, further questions regarding RES-E and land resources should be considered.
+  - How are **additional energy demands of DAC** sourced (preferably from RES-E plants or excess heat)? 
+  - Are there any **potential land conflicts** if deploying this technology?</t>
+  </si>
+  <si>
+    <t>**If sourcing CO2 from unavoidable process emissions or biogenic sources**: this should, preferably, only be a short term option.
+  - What is the intended temporal scope of use of such CO2 sources? Are there **alternative sources in the long term**?
+  - Are all established **sustainability criteria for biomass** met (e.g. related to risks of land use change and biodiversity)?</t>
+  </si>
+  <si>
+    <t>Where in the production chain do **health and safety risks** potentially occur? 
+  - How can potential **risks be reduced to a minimum** and workers protected in the best possible way?
+  - Are there mechanisms in place for **monitoring potential risks** as well as regular comprehensive audits?</t>
   </si>
 </sst>
 </file>
@@ -5237,7 +5236,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE04771-D0C8-4928-A647-849B136F2B55}">
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -5415,7 +5414,7 @@
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
       <c r="O4" s="2" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="P4" s="2"/>
     </row>
@@ -5459,7 +5458,7 @@
       </c>
       <c r="N5" s="2"/>
       <c r="O5" s="2" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="242.25" x14ac:dyDescent="0.25">
@@ -5544,7 +5543,7 @@
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
       <c r="O7" s="2" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="P7" s="2"/>
     </row>
@@ -5623,7 +5622,7 @@
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
       <c r="O9" s="2" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="P9" s="2"/>
     </row>
@@ -5831,7 +5830,7 @@
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
       <c r="O14" s="2" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="178.5" x14ac:dyDescent="0.25">
@@ -5880,7 +5879,7 @@
         <v>175</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>137</v>
@@ -5913,7 +5912,7 @@
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
       <c r="O16" s="2" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
     </row>
   </sheetData>
@@ -6538,8 +6537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A214DC92-F9FF-4B22-82D2-C12543A136EC}">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6565,7 +6564,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>130</v>
       </c>
@@ -6579,7 +6578,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>130</v>
       </c>
@@ -6593,7 +6592,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>130</v>
       </c>
@@ -6607,7 +6606,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>130</v>
       </c>
@@ -6621,7 +6620,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>130</v>
       </c>
@@ -6635,7 +6634,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
         <v>130</v>
       </c>
@@ -6649,7 +6648,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>130</v>
       </c>
@@ -6663,7 +6662,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
         <v>130</v>
       </c>
@@ -6677,7 +6676,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
         <v>130</v>
       </c>
@@ -6688,10 +6687,10 @@
         <v>133</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
         <v>130</v>
       </c>
@@ -6705,7 +6704,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
         <v>130</v>
       </c>
@@ -6719,7 +6718,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
         <v>130</v>
       </c>
@@ -6733,7 +6732,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
         <v>130</v>
       </c>
@@ -6744,10 +6743,10 @@
         <v>247</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
         <v>130</v>
       </c>
@@ -6758,10 +6757,10 @@
         <v>247</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
         <v>130</v>
       </c>
@@ -6772,10 +6771,10 @@
         <v>248</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
         <v>130</v>
       </c>
@@ -6786,10 +6785,10 @@
         <v>248</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
         <v>130</v>
       </c>
@@ -6800,10 +6799,10 @@
         <v>248</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
         <v>130</v>
       </c>
@@ -6814,10 +6813,10 @@
         <v>248</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
         <v>130</v>
       </c>
@@ -6828,10 +6827,10 @@
         <v>248</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
         <v>130</v>
       </c>
@@ -6842,10 +6841,10 @@
         <v>249</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
         <v>130</v>
       </c>
@@ -6856,10 +6855,10 @@
         <v>249</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
         <v>130</v>
       </c>
@@ -6870,10 +6869,10 @@
         <v>250</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="s">
         <v>130</v>
       </c>
@@ -6884,10 +6883,10 @@
         <v>250</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
         <v>251</v>
       </c>
@@ -6898,10 +6897,10 @@
         <v>252</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="9" t="s">
         <v>251</v>
       </c>
@@ -6912,10 +6911,10 @@
         <v>252</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
         <v>251</v>
       </c>
@@ -6926,10 +6925,10 @@
         <v>252</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="s">
         <v>251</v>
       </c>
@@ -6940,10 +6939,10 @@
         <v>252</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="9" t="s">
         <v>251</v>
       </c>
@@ -6954,10 +6953,10 @@
         <v>253</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
         <v>251</v>
       </c>
@@ -6968,10 +6967,10 @@
         <v>253</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
         <v>251</v>
       </c>
@@ -6982,10 +6981,10 @@
         <v>253</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="s">
         <v>251</v>
       </c>
@@ -6996,10 +6995,10 @@
         <v>253</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="s">
         <v>251</v>
       </c>
@@ -7010,10 +7009,10 @@
         <v>253</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="9" t="s">
         <v>251</v>
       </c>
@@ -7024,10 +7023,10 @@
         <v>253</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="9" t="s">
         <v>251</v>
       </c>
@@ -7038,10 +7037,10 @@
         <v>254</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="9" t="s">
         <v>251</v>
       </c>
@@ -7052,10 +7051,10 @@
         <v>254</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="9" t="s">
         <v>251</v>
       </c>
@@ -7066,10 +7065,10 @@
         <v>254</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="9" t="s">
         <v>255</v>
       </c>
@@ -7080,10 +7079,10 @@
         <v>256</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="9" t="s">
         <v>255</v>
       </c>
@@ -7094,10 +7093,10 @@
         <v>256</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="9" t="s">
         <v>255</v>
       </c>
@@ -7108,10 +7107,10 @@
         <v>256</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="9" t="s">
         <v>255</v>
       </c>
@@ -7122,10 +7121,10 @@
         <v>257</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="9" t="s">
         <v>255</v>
       </c>
@@ -7136,10 +7135,10 @@
         <v>257</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="9" t="s">
         <v>255</v>
       </c>
@@ -7150,10 +7149,10 @@
         <v>258</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>602</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="9" t="s">
         <v>255</v>
       </c>
@@ -7164,10 +7163,10 @@
         <v>258</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="9" t="s">
         <v>255</v>
       </c>
@@ -7178,10 +7177,10 @@
         <v>259</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="9" t="s">
         <v>260</v>
       </c>
@@ -7192,10 +7191,10 @@
         <v>261</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="9" t="s">
         <v>260</v>
       </c>
@@ -7206,10 +7205,10 @@
         <v>261</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="9" t="s">
         <v>260</v>
       </c>
@@ -7223,7 +7222,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="9" t="s">
         <v>260</v>
       </c>
@@ -7234,10 +7233,10 @@
         <v>263</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="9" t="s">
         <v>260</v>
       </c>
@@ -7248,10 +7247,10 @@
         <v>263</v>
       </c>
       <c r="D50" s="9" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="9" t="s">
         <v>260</v>
       </c>
@@ -7262,10 +7261,10 @@
         <v>263</v>
       </c>
       <c r="D51" s="9" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="9" t="s">
         <v>260</v>
       </c>
@@ -7276,10 +7275,10 @@
         <v>264</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="9" t="s">
         <v>260</v>
       </c>
@@ -7290,7 +7289,7 @@
         <v>264</v>
       </c>
       <c r="D53" s="9" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
   </sheetData>
@@ -7324,73 +7323,73 @@
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="34" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="D1" s="34"/>
       <c r="E1" s="34" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="F1" s="34"/>
       <c r="G1" s="2" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="C2" s="23" t="s">
+        <v>446</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>445</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>447</v>
+      </c>
+      <c r="F2" s="23" t="s">
+        <v>448</v>
+      </c>
+      <c r="G2" s="23" t="s">
         <v>449</v>
       </c>
-      <c r="D2" s="23" t="s">
-        <v>448</v>
-      </c>
-      <c r="E2" s="23" t="s">
+      <c r="H2" s="23" t="s">
         <v>450</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="I2" s="23" t="s">
         <v>451</v>
       </c>
-      <c r="G2" s="23" t="s">
-        <v>452</v>
-      </c>
-      <c r="H2" s="23" t="s">
-        <v>453</v>
-      </c>
-      <c r="I2" s="23" t="s">
-        <v>454</v>
-      </c>
       <c r="J2" s="28" t="s">
+        <v>490</v>
+      </c>
+      <c r="K2" s="28" t="s">
+        <v>491</v>
+      </c>
+      <c r="L2" s="28" t="s">
+        <v>492</v>
+      </c>
+      <c r="M2" s="28" t="s">
         <v>493</v>
       </c>
-      <c r="K2" s="28" t="s">
+      <c r="N2" s="28" t="s">
         <v>494</v>
-      </c>
-      <c r="L2" s="28" t="s">
-        <v>495</v>
-      </c>
-      <c r="M2" s="28" t="s">
-        <v>496</v>
-      </c>
-      <c r="N2" s="28" t="s">
-        <v>497</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C3" s="25">
         <v>102687.76054053067</v>
@@ -7405,36 +7404,36 @@
         <v>0</v>
       </c>
       <c r="G3" s="24" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H3" s="26" t="s">
         <v>12</v>
       </c>
       <c r="I3" s="27" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="J3" s="24" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="K3" s="24" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="L3" s="24" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="M3" s="24" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="N3" s="24" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="24" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C4" s="25">
         <v>28245.512550017502</v>
@@ -7449,36 +7448,36 @@
         <v>2</v>
       </c>
       <c r="G4" s="24" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H4" s="26" t="s">
         <v>12</v>
       </c>
       <c r="I4" s="27" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="J4" s="24" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="K4" s="24" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="L4" s="24" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="M4" s="24" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="N4" s="24" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="24" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="C5" s="25">
         <v>514994.41648738808</v>
@@ -7493,36 +7492,36 @@
         <v>5</v>
       </c>
       <c r="G5" s="24" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="H5" s="26" t="s">
         <v>12</v>
       </c>
       <c r="I5" s="27" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="J5" s="24" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="K5" s="24" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="L5" s="24" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="M5" s="24" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="N5" s="24" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="24" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="C6" s="25">
         <v>86869.842891781722</v>
@@ -7537,36 +7536,36 @@
         <v>19</v>
       </c>
       <c r="G6" s="24" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="H6" s="26" t="s">
         <v>12</v>
       </c>
       <c r="I6" s="27" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="J6" s="24" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="K6" s="24" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="L6" s="24" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="M6" s="24" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="N6" s="24" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="24" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="C7" s="25">
         <v>15833.086291840766</v>
@@ -7587,27 +7586,27 @@
         <v>159.50488000000001</v>
       </c>
       <c r="I7" s="27" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="J7" s="24" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="K7" s="24" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="L7" s="24" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="M7" s="24" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="N7" s="24" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="24" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="B8" s="24" t="s">
         <v>7</v>
@@ -7625,42 +7624,42 @@
         <v>93</v>
       </c>
       <c r="G8" s="24" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="H8" s="26" t="s">
         <v>12</v>
       </c>
       <c r="I8" s="27" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="J8" s="24" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="K8" s="24" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="L8" s="24" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="M8" s="24" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="N8" s="24" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="24" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="C9" s="25">
         <v>0</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="E9" s="24">
         <v>0</v>
@@ -7675,30 +7674,30 @@
         <v>214.441971</v>
       </c>
       <c r="I9" s="27" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="J9" s="24" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="K9" s="24" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="L9" s="24" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="M9" s="24" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="N9" s="24" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="24" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="C10" s="25">
         <v>3982.9900478920035</v>
@@ -7713,42 +7712,42 @@
         <v>3</v>
       </c>
       <c r="G10" s="24" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H10" s="26" t="s">
         <v>12</v>
       </c>
       <c r="I10" s="27" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="J10" s="24" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="K10" s="24" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="L10" s="24" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="M10" s="24" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="N10" s="24" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="24" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="C11" s="25">
         <v>2097.1640005327972</v>
       </c>
       <c r="D11" s="25" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="E11" s="24">
         <v>0</v>
@@ -7763,30 +7762,30 @@
         <v>80.084551000000005</v>
       </c>
       <c r="I11" s="27" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="J11" s="24" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="K11" s="24" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="L11" s="24" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="M11" s="24" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="N11" s="24" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="24" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="C12" s="25">
         <v>123653.93022264706</v>
@@ -7801,33 +7800,33 @@
         <v>1</v>
       </c>
       <c r="G12" s="24" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H12" s="26" t="s">
         <v>12</v>
       </c>
       <c r="I12" s="27" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="J12" s="24" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="K12" s="24" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="L12" s="24" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="M12" s="24" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="N12" s="24" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="24" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="B13" s="24" t="s">
         <v>8</v>
@@ -7845,36 +7844,36 @@
         <v>20</v>
       </c>
       <c r="G13" s="24" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="H13" s="26" t="s">
         <v>12</v>
       </c>
       <c r="I13" s="27" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="J13" s="24" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="K13" s="24" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="L13" s="24" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="M13" s="24" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="N13" s="24" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="24" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="C14" s="25">
         <v>13804.443716258276</v>
@@ -7895,30 +7894,30 @@
         <v>12</v>
       </c>
       <c r="I14" s="27" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="J14" s="24" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="K14" s="24" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="L14" s="24" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="M14" s="24" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="N14" s="24" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="24" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="B15" s="24" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="C15" s="25">
         <v>0</v>
@@ -7933,36 +7932,36 @@
         <v>1</v>
       </c>
       <c r="G15" s="24" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H15" s="26" t="s">
         <v>12</v>
       </c>
       <c r="I15" s="27" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="J15" s="24" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="K15" s="24" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="L15" s="24" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="M15" s="24" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="N15" s="24" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="24" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B16" s="24" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="C16" s="25">
         <v>176309.43933751195</v>
@@ -7977,36 +7976,36 @@
         <v>0</v>
       </c>
       <c r="G16" s="24" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="H16" s="26" t="s">
         <v>12</v>
       </c>
       <c r="I16" s="27" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="J16" s="24" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="K16" s="24" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="L16" s="24" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="M16" s="24" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="N16" s="24" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="24" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="B17" s="24" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="C17" s="25">
         <v>50841.820075831536</v>
@@ -8027,30 +8026,30 @@
         <v>12</v>
       </c>
       <c r="I17" s="27" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="J17" s="24" t="s">
+        <v>497</v>
+      </c>
+      <c r="K17" s="24" t="s">
         <v>500</v>
       </c>
-      <c r="K17" s="24" t="s">
-        <v>503</v>
-      </c>
       <c r="L17" s="24" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="M17" s="24" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="N17" s="24" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="24" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="B18" s="24" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="C18" s="25">
         <v>27966.147643374599</v>
@@ -8071,30 +8070,30 @@
         <v>12</v>
       </c>
       <c r="I18" s="27" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="J18" s="24" t="s">
+        <v>497</v>
+      </c>
+      <c r="K18" s="24" t="s">
         <v>500</v>
       </c>
-      <c r="K18" s="24" t="s">
-        <v>503</v>
-      </c>
       <c r="L18" s="24" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="M18" s="24" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="N18" s="24" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="24" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="B19" s="24" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="C19" s="25">
         <v>143817.34529670601</v>
@@ -8109,36 +8108,36 @@
         <v>4</v>
       </c>
       <c r="G19" s="24" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="H19" s="26" t="s">
         <v>12</v>
       </c>
       <c r="I19" s="27" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="J19" s="24" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="K19" s="24" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="L19" s="24" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="M19" s="24" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="N19" s="24" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="24" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="C20" s="25">
         <v>42147.136742444643</v>
@@ -8159,36 +8158,36 @@
         <v>12</v>
       </c>
       <c r="I20" s="27" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="J20" s="24" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="K20" s="24" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="L20" s="24" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="M20" s="24" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="N20" s="24" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="24" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="B21" s="24" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="C21" s="25">
         <v>99636.883371308024</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="E21" s="24">
         <v>0</v>
@@ -8197,42 +8196,42 @@
         <v>0</v>
       </c>
       <c r="G21" s="24" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H21" s="26" t="s">
         <v>12</v>
       </c>
       <c r="I21" s="27" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="J21" s="24" t="s">
+        <v>497</v>
+      </c>
+      <c r="K21" s="24" t="s">
         <v>500</v>
       </c>
-      <c r="K21" s="24" t="s">
-        <v>503</v>
-      </c>
       <c r="L21" s="24" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="M21" s="24" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="N21" s="24" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="24" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="B22" s="24" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="C22" s="25">
         <v>5256.6903781170731</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="E22" s="24">
         <v>6</v>
@@ -8241,36 +8240,36 @@
         <v>2</v>
       </c>
       <c r="G22" s="24" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="H22" s="26">
         <v>59.952992000000002</v>
       </c>
       <c r="I22" s="27" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="J22" s="24" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="K22" s="24" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="L22" s="24" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="M22" s="24" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="N22" s="24" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="24" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="B23" s="24" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="C23" s="25">
         <v>29291.660047894893</v>
@@ -8291,36 +8290,36 @@
         <v>12</v>
       </c>
       <c r="I23" s="27" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="J23" s="24" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="K23" s="24" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="L23" s="24" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="M23" s="24" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="N23" s="24" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="24" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="B24" s="24" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="C24" s="25">
         <v>7559.5180291508068</v>
       </c>
       <c r="D24" s="25" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="E24" s="24">
         <v>0</v>
@@ -8335,30 +8334,30 @@
         <v>129.84832399999999</v>
       </c>
       <c r="I24" s="27" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="J24" s="24" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="K24" s="24" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="L24" s="24" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="M24" s="24" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="N24" s="24" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="24" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="B25" s="24" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="C25" s="25">
         <v>192895.02833307866</v>
@@ -8373,36 +8372,36 @@
         <v>1</v>
       </c>
       <c r="G25" s="24" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="H25" s="26" t="s">
         <v>12</v>
       </c>
       <c r="I25" s="27" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="J25" s="24" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="K25" s="24" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="L25" s="24" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="M25" s="24" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="N25" s="24" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="24" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="B26" s="24" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="C26" s="25">
         <v>151622.74756959747</v>
@@ -8417,36 +8416,36 @@
         <v>0</v>
       </c>
       <c r="G26" s="24" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="H26" s="26" t="s">
         <v>12</v>
       </c>
       <c r="I26" s="27" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="J26" s="24" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="K26" s="24" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="L26" s="24" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="M26" s="24" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="N26" s="24" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="24" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="B27" s="24" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="C27" s="25">
         <v>53182.742412075226</v>
@@ -8461,33 +8460,33 @@
         <v>3</v>
       </c>
       <c r="G27" s="24" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="H27" s="26" t="s">
         <v>12</v>
       </c>
       <c r="I27" s="27" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="J27" s="24" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="K27" s="24" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="L27" s="24" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="M27" s="24" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="N27" s="24" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="24" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="B28" s="24" t="s">
         <v>6</v>
@@ -8496,7 +8495,7 @@
         <v>35393.799778929817</v>
       </c>
       <c r="D28" s="25" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="E28" s="24">
         <v>0</v>
@@ -8511,36 +8510,36 @@
         <v>122.662285</v>
       </c>
       <c r="I28" s="27" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="J28" s="24" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="K28" s="24" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="L28" s="24" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="M28" s="24" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="N28" s="24" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="24" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="B29" s="24" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="C29" s="25">
         <v>2375.3911489586781</v>
       </c>
       <c r="D29" s="25" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="E29" s="24">
         <v>0</v>
@@ -8549,42 +8548,42 @@
         <v>2</v>
       </c>
       <c r="G29" s="24" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H29" s="26">
         <v>70.495289999999997</v>
       </c>
       <c r="I29" s="27" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="J29" s="24" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="K29" s="24" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="L29" s="24" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="M29" s="24" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="N29" s="24" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="24" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="B30" s="24" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="C30" s="25">
         <v>6534.4815097404735</v>
       </c>
       <c r="D30" s="25" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="E30" s="24">
         <v>0</v>
@@ -8593,36 +8592,36 @@
         <v>7</v>
       </c>
       <c r="G30" s="24" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H30" s="26" t="s">
         <v>12</v>
       </c>
       <c r="I30" s="27" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="J30" s="24" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="K30" s="24" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="L30" s="24" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="M30" s="24" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="N30" s="24" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="24" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="B31" s="24" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="C31" s="25">
         <v>17975.881159055345</v>
@@ -8643,30 +8642,30 @@
         <v>12</v>
       </c>
       <c r="I31" s="27" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="J31" s="24" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="K31" s="24" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="L31" s="24" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="M31" s="24" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="N31" s="24" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="24" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="B32" s="24" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="C32" s="25">
         <v>1234.3228021367959</v>
@@ -8681,36 +8680,36 @@
         <v>2</v>
       </c>
       <c r="G32" s="24" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="H32" s="26" t="s">
         <v>12</v>
       </c>
       <c r="I32" s="27" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="J32" s="24" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="K32" s="24" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="L32" s="24" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="M32" s="24" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="N32" s="24" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
     </row>
     <row r="33" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="24" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="B33" s="24" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="C33" s="25">
         <v>9001.3629494330653</v>
@@ -8725,36 +8724,36 @@
         <v>0</v>
       </c>
       <c r="G33" s="24" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="H33" s="26" t="s">
         <v>12</v>
       </c>
       <c r="I33" s="27" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="J33" s="24" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="K33" s="24" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="L33" s="24" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="M33" s="24" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="N33" s="24" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
     </row>
     <row r="34" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="24" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="B34" s="24" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="C34" s="25">
         <v>378.04871500147641</v>
@@ -8775,22 +8774,22 @@
         <v>12</v>
       </c>
       <c r="I34" s="27" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="J34" s="24" t="s">
+        <v>497</v>
+      </c>
+      <c r="K34" s="24" t="s">
         <v>500</v>
       </c>
-      <c r="K34" s="24" t="s">
-        <v>503</v>
-      </c>
       <c r="L34" s="24" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="M34" s="24" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="N34" s="24" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
     </row>
     <row r="35" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -8798,7 +8797,7 @@
         <v>11</v>
       </c>
       <c r="B35" s="24" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="C35" s="25">
         <v>544110.99319185445</v>
@@ -8813,42 +8812,42 @@
         <v>8</v>
       </c>
       <c r="G35" s="24" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="H35" s="26">
         <v>68.122753000000003</v>
       </c>
       <c r="I35" s="27" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="J35" s="24" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="K35" s="24" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="L35" s="24" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="M35" s="24" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="N35" s="24" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
     </row>
     <row r="36" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="24" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="B36" s="24" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="C36" s="25">
         <v>8842.3521510548053</v>
       </c>
       <c r="D36" s="25" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="E36" s="24">
         <v>0</v>
@@ -8857,28 +8856,28 @@
         <v>20</v>
       </c>
       <c r="G36" s="24" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="H36" s="26" t="s">
         <v>12</v>
       </c>
       <c r="I36" s="27" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="J36" s="24" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="K36" s="24" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="L36" s="24" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="M36" s="24" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="N36" s="24" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
@@ -9105,10 +9104,10 @@
     </row>
     <row r="2" spans="1:18" ht="51" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>115</v>
@@ -9138,30 +9137,30 @@
         <v>117</v>
       </c>
       <c r="L2" s="17" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="M2" s="17" t="s">
+        <v>535</v>
+      </c>
+      <c r="N2" s="17" t="s">
+        <v>536</v>
+      </c>
+      <c r="O2" s="17" t="s">
+        <v>537</v>
+      </c>
+      <c r="P2" s="17" t="s">
         <v>538</v>
       </c>
-      <c r="N2" s="17" t="s">
+      <c r="Q2" s="17" t="s">
         <v>539</v>
       </c>
-      <c r="O2" s="17" t="s">
+      <c r="R2" s="17" t="s">
         <v>540</v>
-      </c>
-      <c r="P2" s="17" t="s">
-        <v>541</v>
-      </c>
-      <c r="Q2" s="17" t="s">
-        <v>542</v>
-      </c>
-      <c r="R2" s="17" t="s">
-        <v>543</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="267.75" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="B3" s="16" t="s">
         <v>3</v>
@@ -9173,13 +9172,13 @@
         <v>34</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="F3" s="15" t="s">
         <v>118</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="H3" s="16" t="s">
         <v>119</v>
@@ -9188,28 +9187,28 @@
         <v>120</v>
       </c>
       <c r="J3" s="15" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="K3" s="16" t="s">
         <v>121</v>
       </c>
       <c r="M3" s="17" t="s">
+        <v>541</v>
+      </c>
+      <c r="N3" s="17" t="s">
+        <v>541</v>
+      </c>
+      <c r="O3" s="17" t="s">
         <v>544</v>
       </c>
-      <c r="N3" s="17" t="s">
-        <v>544</v>
-      </c>
-      <c r="O3" s="17" t="s">
+      <c r="P3" s="17" t="s">
         <v>547</v>
       </c>
-      <c r="P3" s="17" t="s">
-        <v>550</v>
-      </c>
       <c r="Q3" s="17" t="s">
+        <v>551</v>
+      </c>
+      <c r="R3" s="17" t="s">
         <v>554</v>
-      </c>
-      <c r="R3" s="17" t="s">
-        <v>557</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="293.25" x14ac:dyDescent="0.25">
@@ -9220,54 +9219,54 @@
         <v>4</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="D4" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>309</v>
+      </c>
+      <c r="F4" s="15" t="s">
         <v>310</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="G4" s="15" t="s">
         <v>312</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>313</v>
-      </c>
-      <c r="G4" s="15" t="s">
-        <v>315</v>
       </c>
       <c r="H4" s="16" t="s">
         <v>34</v>
       </c>
       <c r="I4" s="15" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="J4" s="16" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="K4" s="15" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="L4" s="17" t="s">
+        <v>555</v>
+      </c>
+      <c r="M4" s="17" t="s">
+        <v>541</v>
+      </c>
+      <c r="N4" s="17" t="s">
+        <v>541</v>
+      </c>
+      <c r="P4" s="17" t="s">
         <v>558</v>
       </c>
-      <c r="M4" s="17" t="s">
-        <v>544</v>
-      </c>
-      <c r="N4" s="17" t="s">
-        <v>544</v>
-      </c>
-      <c r="P4" s="17" t="s">
-        <v>561</v>
-      </c>
       <c r="Q4" s="17" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="R4" s="17" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="178.5" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="B5" s="16" t="s">
         <v>5</v>
@@ -9276,48 +9275,48 @@
         <v>12</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="H5" s="16" t="s">
         <v>34</v>
       </c>
       <c r="I5" s="15" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="J5" s="15" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="K5" s="16" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="M5" s="17" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="N5" s="17" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="P5" s="17" t="s">
+        <v>560</v>
+      </c>
+      <c r="Q5" s="17" t="s">
+        <v>551</v>
+      </c>
+      <c r="R5" s="17" t="s">
         <v>563</v>
-      </c>
-      <c r="Q5" s="17" t="s">
-        <v>554</v>
-      </c>
-      <c r="R5" s="17" t="s">
-        <v>566</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="153" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="B6" s="16" t="s">
         <v>6</v>
@@ -9326,107 +9325,107 @@
         <v>12</v>
       </c>
       <c r="D6" s="15" t="s">
+        <v>323</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>324</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>325</v>
+      </c>
+      <c r="G6" s="16" t="s">
         <v>326</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="H6" s="16" t="s">
         <v>327</v>
       </c>
-      <c r="F6" s="16" t="s">
+      <c r="I6" s="15" t="s">
         <v>328</v>
       </c>
-      <c r="G6" s="16" t="s">
+      <c r="J6" s="15" t="s">
         <v>329</v>
       </c>
-      <c r="H6" s="16" t="s">
+      <c r="K6" s="16" t="s">
         <v>330</v>
       </c>
-      <c r="I6" s="15" t="s">
-        <v>331</v>
-      </c>
-      <c r="J6" s="15" t="s">
-        <v>332</v>
-      </c>
-      <c r="K6" s="16" t="s">
-        <v>333</v>
-      </c>
       <c r="M6" s="17" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="N6" s="17" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="P6" s="17" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="Q6" s="17" t="s">
+        <v>551</v>
+      </c>
+      <c r="R6" s="17" t="s">
         <v>554</v>
-      </c>
-      <c r="R6" s="17" t="s">
-        <v>557</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="242.25" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="B7" s="16" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="16" t="s">
+        <v>331</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>332</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>322</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>333</v>
+      </c>
+      <c r="G7" s="15" t="s">
         <v>334</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>335</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>325</v>
-      </c>
-      <c r="F7" s="16" t="s">
-        <v>336</v>
-      </c>
-      <c r="G7" s="15" t="s">
-        <v>337</v>
       </c>
       <c r="H7" s="16" t="s">
         <v>34</v>
       </c>
       <c r="I7" s="15" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="J7" s="15" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="K7" s="16" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="L7" s="17" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="M7" s="17" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="N7" s="17" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="P7" s="17" t="s">
         <v>67</v>
       </c>
       <c r="Q7" s="17" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="R7" s="17" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="255" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="B8" s="16" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="D8" s="16" t="s">
         <v>12</v>
@@ -9435,34 +9434,34 @@
         <v>12</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="G8" s="15" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="H8" s="16" t="s">
         <v>34</v>
       </c>
       <c r="I8" s="15" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="J8" s="15" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="K8" s="16" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="L8" s="17" t="s">
+        <v>571</v>
+      </c>
+      <c r="P8" s="17" t="s">
+        <v>571</v>
+      </c>
+      <c r="Q8" s="17" t="s">
+        <v>551</v>
+      </c>
+      <c r="R8" s="17" t="s">
         <v>574</v>
-      </c>
-      <c r="P8" s="17" t="s">
-        <v>574</v>
-      </c>
-      <c r="Q8" s="17" t="s">
-        <v>554</v>
-      </c>
-      <c r="R8" s="17" t="s">
-        <v>577</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="165.75" x14ac:dyDescent="0.25">
@@ -9473,52 +9472,52 @@
         <v>9</v>
       </c>
       <c r="C9" s="16" t="s">
+        <v>344</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>345</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>346</v>
+      </c>
+      <c r="F9" s="15" t="s">
         <v>347</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="G9" s="16" t="s">
         <v>348</v>
       </c>
-      <c r="E9" s="16" t="s">
+      <c r="H9" s="16" t="s">
         <v>349</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="I9" s="15" t="s">
         <v>350</v>
       </c>
-      <c r="G9" s="16" t="s">
+      <c r="J9" s="16" t="s">
         <v>351</v>
       </c>
-      <c r="H9" s="16" t="s">
+      <c r="K9" s="16" t="s">
         <v>352</v>
       </c>
-      <c r="I9" s="15" t="s">
-        <v>353</v>
-      </c>
-      <c r="J9" s="16" t="s">
-        <v>354</v>
-      </c>
-      <c r="K9" s="16" t="s">
-        <v>355</v>
-      </c>
       <c r="L9" s="17" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="M9" s="17" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="N9" s="17" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="O9" s="17" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="P9" s="17" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="Q9" s="17" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="R9" s="17" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="76.5" x14ac:dyDescent="0.25">
@@ -9529,49 +9528,49 @@
         <v>10</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="E10" s="16" t="s">
         <v>12</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="H10" s="16" t="s">
         <v>34</v>
       </c>
       <c r="I10" s="15" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="J10" s="15" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="K10" s="16" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="L10" s="17" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="M10" s="17" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="N10" s="17" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="P10" s="17" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="Q10" s="17" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="R10" s="17" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="114.75" x14ac:dyDescent="0.25">
@@ -9582,52 +9581,52 @@
         <v>11</v>
       </c>
       <c r="C11" s="16" t="s">
+        <v>360</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>361</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>362</v>
+      </c>
+      <c r="F11" s="15" t="s">
         <v>363</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="G11" s="16" t="s">
         <v>364</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="H11" s="16" t="s">
         <v>365</v>
       </c>
-      <c r="F11" s="15" t="s">
+      <c r="I11" s="15" t="s">
         <v>366</v>
       </c>
-      <c r="G11" s="16" t="s">
+      <c r="J11" s="15" t="s">
         <v>367</v>
       </c>
-      <c r="H11" s="16" t="s">
+      <c r="K11" s="16" t="s">
         <v>368</v>
       </c>
-      <c r="I11" s="15" t="s">
-        <v>369</v>
-      </c>
-      <c r="J11" s="15" t="s">
-        <v>370</v>
-      </c>
-      <c r="K11" s="16" t="s">
-        <v>371</v>
-      </c>
       <c r="L11" s="17" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="M11" s="17" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="N11" s="17" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="O11" s="17" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="P11" s="17" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="Q11" s="17" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="R11" s="17" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
     </row>
   </sheetData>
@@ -9668,7 +9667,7 @@
         <v>51</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="C2" s="32" t="s">
         <v>83</v>
@@ -9692,7 +9691,7 @@
         <v>53</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="C4" s="32" t="s">
         <v>85</v>
@@ -9731,7 +9730,7 @@
         <v>56</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="C7" s="32" t="s">
         <v>88</v>
@@ -9744,7 +9743,7 @@
         <v>57</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="C8" s="32" t="s">
         <v>89</v>
@@ -9757,7 +9756,7 @@
         <v>58</v>
       </c>
       <c r="B9" s="30" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="C9" s="32" t="s">
         <v>90</v>
@@ -9770,7 +9769,7 @@
         <v>59</v>
       </c>
       <c r="B10" s="30" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="C10" s="32" t="s">
         <v>91</v>
@@ -9822,7 +9821,7 @@
         <v>63</v>
       </c>
       <c r="B14" s="30" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="C14" s="32" t="s">
         <v>95</v>
@@ -9861,7 +9860,7 @@
         <v>66</v>
       </c>
       <c r="B17" s="30" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="C17" s="32" t="s">
         <v>98</v>
@@ -9910,10 +9909,10 @@
     </row>
     <row r="21" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="30" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="B21" s="30" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="C21" s="32" t="s">
         <v>102</v>
@@ -9936,10 +9935,10 @@
     </row>
     <row r="23" spans="1:6" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="30" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="B23" s="30" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="C23" s="32" t="s">
         <v>104</v>
@@ -9949,10 +9948,10 @@
     </row>
     <row r="24" spans="1:6" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="30" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="B24" s="30" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="C24" s="32" t="s">
         <v>105</v>
@@ -9962,13 +9961,13 @@
     </row>
     <row r="25" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A25" s="30" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="B25" s="30" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="C25" s="32" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="D25" s="30"/>
       <c r="E25" s="30"/>
@@ -9976,13 +9975,13 @@
     </row>
     <row r="26" spans="1:6" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="30" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="B26" s="30" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="C26" s="32" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="D26" s="30"/>
       <c r="E26" s="30"/>
@@ -9990,208 +9989,208 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="24" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="B27" s="24" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="C27" s="24" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="30" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="B28" s="24" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="C28" s="24" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="30" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="B29" s="24" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="C29" s="24" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A30" s="30" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="B30" s="24" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="C30" s="24" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A31" s="30" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="B31" s="24" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="C31" s="24" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A32" s="30" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="B32" s="24" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="C32" s="24" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="30" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="B33" s="24" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="C33" s="24" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A34" s="30" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="B34" s="24" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="C34" s="24" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="24" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="B35" s="24" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="C35" s="24" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="30" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="B36" s="24" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="C36" s="24" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A37" s="30" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="B37" s="24" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="C37" s="24" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="30" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="B38" s="24" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="C38" s="24" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="24" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="B39" s="24" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="C39" s="24" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="30" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="B40" s="24" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="C40" s="24" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="30" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="B41" s="24" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="C41" s="24" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A42" s="30" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="B42" s="24" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="C42" s="24" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="30" t="s">
+        <v>575</v>
+      </c>
+      <c r="B43" s="24" t="s">
         <v>578</v>
       </c>
-      <c r="B43" s="24" t="s">
-        <v>581</v>
-      </c>
       <c r="C43" s="33" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="30" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="B44" s="24" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="C44" s="24" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="30" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="B45" s="24" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="C45" s="24" t="s">
         <v>34</v>
@@ -10199,13 +10198,13 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="30" t="s">
+        <v>589</v>
+      </c>
+      <c r="B46" s="24" t="s">
+        <v>591</v>
+      </c>
+      <c r="C46" s="24" t="s">
         <v>592</v>
-      </c>
-      <c r="B46" s="24" t="s">
-        <v>594</v>
-      </c>
-      <c r="C46" s="24" t="s">
-        <v>595</v>
       </c>
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.25">
@@ -10393,6 +10392,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100E2F0DF90B070FE43BFD707F72A4CD00B" ma:contentTypeVersion="15" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="8927d14e1bc908eae180c9caa4b5da89">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1bc94727-11e8-4443-b8f0-9215ff28e4bb" xmlns:ns3="cd34aed5-94da-4c30-bba3-37b78f4daae9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bb67c9392edae2d7a3a1d88d3e91258a" ns2:_="" ns3:_="">
     <xsd:import namespace="1bc94727-11e8-4443-b8f0-9215ff28e4bb"/>
@@ -10629,16 +10637,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22BF5C6F-88A2-47DA-9B5F-9FD29A58E304}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1143ECE1-9C35-446D-8A76-82388033D272}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10655,12 +10662,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22BF5C6F-88A2-47DA-9B5F-9FD29A58E304}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
add supply country fact sheet
</commit_message>
<xml_diff>
--- a/data/context_data.xlsx
+++ b/data/context_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m.haller\Documents\code\ptx-boa\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3D78F26-87DB-4057-B70C-C60467C168ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76AD3648-8699-4454-975D-BA7B66D5F92F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{D16C601B-E1D6-40C0-8CC1-80505BE1FBB6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{D16C601B-E1D6-40C0-8CC1-80505BE1FBB6}"/>
   </bookViews>
   <sheets>
     <sheet name="certification_schemes" sheetId="6" r:id="rId1"/>
@@ -25,94 +25,94 @@
     <externalReference r:id="rId8"/>
   </externalReferences>
   <definedNames>
-    <definedName name="can_use_pipeline" localSheetId="3">INDEX([2]!chains[CAN_PIPELINE],supply!sel_chain_index)</definedName>
-    <definedName name="can_use_pipeline">INDEX([2]!chains[CAN_PIPELINE],sel_chain_index)</definedName>
-    <definedName name="chains_chain">[2]!chains[chain]</definedName>
-    <definedName name="compCostCountries_DELETE">[2]!Table23[Country code]</definedName>
-    <definedName name="context_data_carbonsource" localSheetId="3">[1]!Table33353637[#All]</definedName>
+    <definedName name="can_use_pipeline" localSheetId="3">INDEX([1]!chains[CAN_PIPELINE],supply!sel_chain_index)</definedName>
+    <definedName name="can_use_pipeline">INDEX([1]!chains[CAN_PIPELINE],sel_chain_index)</definedName>
+    <definedName name="chains_chain">[1]!chains[chain]</definedName>
+    <definedName name="compCostCountries_DELETE">[1]!Table23[Country code]</definedName>
+    <definedName name="context_data_carbonsource" localSheetId="3">[2]!Table33353637[#All]</definedName>
     <definedName name="context_data_carbonsource">#REF!</definedName>
-    <definedName name="context_data_infobox" localSheetId="3">[1]!Table32[#Data]</definedName>
+    <definedName name="context_data_infobox" localSheetId="3">[2]!Table32[#Data]</definedName>
     <definedName name="context_data_infobox">#REF!</definedName>
-    <definedName name="context_data_re" localSheetId="3">[1]!Table33[#All]</definedName>
+    <definedName name="context_data_re" localSheetId="3">[2]!Table33[#All]</definedName>
     <definedName name="context_data_re">#REF!</definedName>
-    <definedName name="context_data_transport_mode" localSheetId="3">[1]!Table3335[#All]</definedName>
+    <definedName name="context_data_transport_mode" localSheetId="3">[2]!Table3335[#All]</definedName>
     <definedName name="context_data_transport_mode">#REF!</definedName>
-    <definedName name="context_data_watersource" localSheetId="3">[1]!Table333536[#All]</definedName>
+    <definedName name="context_data_watersource" localSheetId="3">[2]!Table333536[#All]</definedName>
     <definedName name="context_data_watersource">#REF!</definedName>
-    <definedName name="conv_fact_to_mass">[2]_calc!$BM$6</definedName>
-    <definedName name="country_area">[2]!Table22[#All]</definedName>
-    <definedName name="country_country_code">[2]!country[target_country_code]</definedName>
-    <definedName name="country_country_name">[2]!country[target_country_name]</definedName>
-    <definedName name="country_energy_use">[2]!Table25[#All]</definedName>
-    <definedName name="country_pop">[2]!Table26[#All]</definedName>
-    <definedName name="country_pop_and_energy_use" localSheetId="3">[2]!Table26[#Data]</definedName>
-    <definedName name="country_pop_and_energy_use">[2]!Table26[#Data]</definedName>
-    <definedName name="default_scenarios">[2]!tab_default_scenario[default_scenario]</definedName>
-    <definedName name="dim_bool_bool">[2]!dim_bool[BOOL]</definedName>
-    <definedName name="flh_deriv">[2]_calc!$X$257:$X$335</definedName>
-    <definedName name="flh_ely">[2]_calc!$Q$257:$Q$335</definedName>
-    <definedName name="flh_region_code">[2]_calc!$B$257:$B$335</definedName>
-    <definedName name="flow_flow_code">[2]!flow[flow_code]</definedName>
-    <definedName name="flow_flow_name">[2]!flow[flow_name]</definedName>
-    <definedName name="flow_short_names">[2]_dims!$X$22:$Y$37</definedName>
-    <definedName name="input_scenarios">[2]!tabDatasetsInput[name]</definedName>
-    <definedName name="mapMaxValue">[2]_map!$G$3</definedName>
-    <definedName name="mapMinValue">[2]_map!$G$2</definedName>
-    <definedName name="output_scenario_name">[2]_todo_dev!$A$9</definedName>
-    <definedName name="output_scenario_names">[2]!output_scenarios[scenario]</definedName>
-    <definedName name="output_units">[2]!tabOutputUnit[output_unit]</definedName>
-    <definedName name="process_classes_process_class">[2]!process_classes[process_class]</definedName>
-    <definedName name="process_classes_process_class_name">[2]!process_classes[process_class_name]</definedName>
-    <definedName name="process_main_flow_code_out">[2]!process[main_flow_code_out]</definedName>
-    <definedName name="process_process_class">[2]!process[process_class]</definedName>
-    <definedName name="process_process_code">[2]!process[process_code]</definedName>
-    <definedName name="process_process_name">[2]!process[process_name]</definedName>
-    <definedName name="process_res_gen_name">[2]!process_res_gen[process_name]</definedName>
-    <definedName name="process_res_gen_process_code">[2]!process_res_gen[process_code]</definedName>
-    <definedName name="process_res_gen_process_name">[2]!process_res_gen[process_name]</definedName>
-    <definedName name="region_region_code">[2]!region[source_region_code]</definedName>
-    <definedName name="region_region_name">[2]!region[region_name]</definedName>
-    <definedName name="regions_by_cost">[2]!Table21[#All]</definedName>
-    <definedName name="release_date">[2]_release!$B$2</definedName>
-    <definedName name="release_version">[2]_release!$B$1</definedName>
-    <definedName name="saved_outputs">[2]!tabDatasetsOutput[name]</definedName>
-    <definedName name="secondary_process_CO2_G">[2]!tabSelCo2[name]</definedName>
-    <definedName name="secondary_process_H2O_L">[2]!tabSelWater[name]</definedName>
-    <definedName name="sel_chain">[2]b_dashboard!$D$23</definedName>
-    <definedName name="sel_chain_deriv_proc_code">[2]_calc!$X$2</definedName>
-    <definedName name="sel_chain_ely_proc_code">[2]_calc!$Q$2</definedName>
-    <definedName name="sel_chain_flow_out">[2]_calc!$BM$5</definedName>
-    <definedName name="sel_chain_index" localSheetId="3">MATCH(sel_chain,[2]!chains[chain],)</definedName>
-    <definedName name="sel_chain_index">MATCH(sel_chain,[2]!chains[chain],)</definedName>
-    <definedName name="sel_chain_range" localSheetId="3">OFFSET([2]!chains[[#Headers],[chain]],supply!sel_chain_index,1,1,COUNTA([2]!chains[#Headers])-1)</definedName>
-    <definedName name="sel_chain_range">OFFSET([2]!chains[[#Headers],[chain]],sel_chain_index,1,1,COUNTA([2]!chains[#Headers])-1)</definedName>
-    <definedName name="sel_chain_range_word" localSheetId="3">OFFSET([2]!chains[[#Headers],[chain]],sel_chain_index_world,1,1,COUNTA([2]!chains[#Headers])-1)</definedName>
-    <definedName name="sel_chain_range_word">OFFSET([2]!chains[[#Headers],[chain]],sel_chain_index_world,1,1,COUNTA([2]!chains[#Headers])-1)</definedName>
-    <definedName name="sel_choices_transport" localSheetId="3">OFFSET([2]!choicesTransport[none],0,supply!sel_pipeline_possible*2+sel_ship_possible,supply!sel_pipeline_possible+sel_ship_possible)</definedName>
-    <definedName name="sel_choices_transport">OFFSET([2]!choicesTransport[none],0,sel_pipeline_possible*2+sel_ship_possible,sel_pipeline_possible+sel_ship_possible)</definedName>
+    <definedName name="conv_fact_to_mass">[1]_calc!$BM$6</definedName>
+    <definedName name="country_area">[1]!Table22[#All]</definedName>
+    <definedName name="country_country_code">[1]!country[target_country_code]</definedName>
+    <definedName name="country_country_name">[1]!country[target_country_name]</definedName>
+    <definedName name="country_energy_use">[1]!Table25[#All]</definedName>
+    <definedName name="country_pop">[1]!Table26[#All]</definedName>
+    <definedName name="country_pop_and_energy_use" localSheetId="3">[1]!Table26[#Data]</definedName>
+    <definedName name="country_pop_and_energy_use">[1]!Table26[#Data]</definedName>
+    <definedName name="default_scenarios">[1]!tab_default_scenario[default_scenario]</definedName>
+    <definedName name="dim_bool_bool">[1]!dim_bool[BOOL]</definedName>
+    <definedName name="flh_deriv">[1]_calc!$X$257:$X$335</definedName>
+    <definedName name="flh_ely">[1]_calc!$Q$257:$Q$335</definedName>
+    <definedName name="flh_region_code">[1]_calc!$B$257:$B$335</definedName>
+    <definedName name="flow_flow_code">[1]!flow[flow_code]</definedName>
+    <definedName name="flow_flow_name">[1]!flow[flow_name]</definedName>
+    <definedName name="flow_short_names">[1]_dims!$X$22:$Y$37</definedName>
+    <definedName name="input_scenarios">[1]!tabDatasetsInput[name]</definedName>
+    <definedName name="mapMaxValue">[1]_map!$G$3</definedName>
+    <definedName name="mapMinValue">[1]_map!$G$2</definedName>
+    <definedName name="output_scenario_name">[1]_todo_dev!$A$9</definedName>
+    <definedName name="output_scenario_names">[1]!output_scenarios[scenario]</definedName>
+    <definedName name="output_units">[1]!tabOutputUnit[output_unit]</definedName>
+    <definedName name="process_classes_process_class">[1]!process_classes[process_class]</definedName>
+    <definedName name="process_classes_process_class_name">[1]!process_classes[process_class_name]</definedName>
+    <definedName name="process_main_flow_code_out">[1]!process[main_flow_code_out]</definedName>
+    <definedName name="process_process_class">[1]!process[process_class]</definedName>
+    <definedName name="process_process_code">[1]!process[process_code]</definedName>
+    <definedName name="process_process_name">[1]!process[process_name]</definedName>
+    <definedName name="process_res_gen_name">[1]!process_res_gen[process_name]</definedName>
+    <definedName name="process_res_gen_process_code">[1]!process_res_gen[process_code]</definedName>
+    <definedName name="process_res_gen_process_name">[1]!process_res_gen[process_name]</definedName>
+    <definedName name="region_region_code">[1]!region[source_region_code]</definedName>
+    <definedName name="region_region_name">[1]!region[region_name]</definedName>
+    <definedName name="regions_by_cost">[1]!Table21[#All]</definedName>
+    <definedName name="release_date">[1]_release!$B$2</definedName>
+    <definedName name="release_version">[1]_release!$B$1</definedName>
+    <definedName name="saved_outputs">[1]!tabDatasetsOutput[name]</definedName>
+    <definedName name="secondary_process_CO2_G">[1]!tabSelCo2[name]</definedName>
+    <definedName name="secondary_process_H2O_L">[1]!tabSelWater[name]</definedName>
+    <definedName name="sel_chain">[1]b_dashboard!$D$23</definedName>
+    <definedName name="sel_chain_deriv_proc_code">[1]_calc!$X$2</definedName>
+    <definedName name="sel_chain_ely_proc_code">[1]_calc!$Q$2</definedName>
+    <definedName name="sel_chain_flow_out">[1]_calc!$BM$5</definedName>
+    <definedName name="sel_chain_index" localSheetId="3">MATCH(sel_chain,[1]!chains[chain],)</definedName>
+    <definedName name="sel_chain_index">MATCH(sel_chain,[1]!chains[chain],)</definedName>
+    <definedName name="sel_chain_range" localSheetId="3">OFFSET([1]!chains[[#Headers],[chain]],supply!sel_chain_index,1,1,COUNTA([1]!chains[#Headers])-1)</definedName>
+    <definedName name="sel_chain_range">OFFSET([1]!chains[[#Headers],[chain]],sel_chain_index,1,1,COUNTA([1]!chains[#Headers])-1)</definedName>
+    <definedName name="sel_chain_range_word" localSheetId="3">OFFSET([1]!chains[[#Headers],[chain]],sel_chain_index_world,1,1,COUNTA([1]!chains[#Headers])-1)</definedName>
+    <definedName name="sel_chain_range_word">OFFSET([1]!chains[[#Headers],[chain]],sel_chain_index_world,1,1,COUNTA([1]!chains[#Headers])-1)</definedName>
+    <definedName name="sel_choices_transport" localSheetId="3">OFFSET([1]!choicesTransport[none],0,supply!sel_pipeline_possible*2+sel_ship_possible,supply!sel_pipeline_possible+sel_ship_possible)</definedName>
+    <definedName name="sel_choices_transport">OFFSET([1]!choicesTransport[none],0,sel_pipeline_possible*2+sel_ship_possible,sel_pipeline_possible+sel_ship_possible)</definedName>
     <definedName name="sel_country_code" localSheetId="3">IF(sel_country_name="","",INDEX(country_country_code,MATCH(sel_country_name,country_country_name,0),1))</definedName>
     <definedName name="sel_country_code">IF(sel_country_name="","",INDEX(country_country_code,MATCH(sel_country_name,country_country_name,0),1))</definedName>
-    <definedName name="sel_country_name">[2]b_dashboard!$D$22</definedName>
-    <definedName name="sel_pipeline_possible" localSheetId="3">AND(INDEX([2]_calc!$AQ$14:$AQ$92,MATCH(_xlfn.SINGLE(supply!sel_region_code),[2]_calc!$B$14:$B$92,0))&gt;0,_xlfn.SINGLE(supply!can_use_pipeline)=TRUE)</definedName>
-    <definedName name="sel_pipeline_possible">AND(INDEX([2]_calc!$AQ$14:$AQ$92,MATCH(_xlfn.SINGLE(sel_region_code),[2]_calc!$B$14:$B$92,0))&gt;0,_xlfn.SINGLE(can_use_pipeline)=TRUE)</definedName>
-    <definedName name="sel_region_code" localSheetId="3">IF(sel_region_name="","",INDEX([2]!region[source_region_code],MATCH(sel_region_name,[2]!region[region_name],0),1))</definedName>
-    <definedName name="sel_region_code">IF(sel_region_name="","",INDEX([2]!region[source_region_code],MATCH(sel_region_name,[2]!region[region_name],0),1))</definedName>
+    <definedName name="sel_country_name">[1]b_dashboard!$D$22</definedName>
+    <definedName name="sel_pipeline_possible" localSheetId="3">AND(INDEX([1]_calc!$AQ$14:$AQ$92,MATCH(_xlfn.SINGLE(supply!sel_region_code),[1]_calc!$B$14:$B$92,0))&gt;0,_xlfn.SINGLE(supply!can_use_pipeline)=TRUE)</definedName>
+    <definedName name="sel_pipeline_possible">AND(INDEX([1]_calc!$AQ$14:$AQ$92,MATCH(_xlfn.SINGLE(sel_region_code),[1]_calc!$B$14:$B$92,0))&gt;0,_xlfn.SINGLE(can_use_pipeline)=TRUE)</definedName>
+    <definedName name="sel_region_code" localSheetId="3">IF(sel_region_name="","",INDEX([1]!region[source_region_code],MATCH(sel_region_name,[1]!region[region_name],0),1))</definedName>
+    <definedName name="sel_region_code">IF(sel_region_name="","",INDEX([1]!region[source_region_code],MATCH(sel_region_name,[1]!region[region_name],0),1))</definedName>
     <definedName name="sel_region_country_code" localSheetId="3">IF(supply!sel_region_code="","",LEFT(supply!sel_region_code,3))</definedName>
     <definedName name="sel_region_country_code">IF(sel_region_code="","",LEFT(sel_region_code,3))</definedName>
-    <definedName name="sel_region_name">[2]b_dashboard!$D$21</definedName>
-    <definedName name="sel_res_gen" localSheetId="3">IF(sel_res_gen_name="","",INDEX([2]!process[#Data],MATCH(sel_res_gen_name,[2]!process[process_name],0),1))</definedName>
-    <definedName name="sel_res_gen">IF(sel_res_gen_name="","",INDEX([2]!process[#Data],MATCH(sel_res_gen_name,[2]!process[process_name],0),1))</definedName>
-    <definedName name="sel_res_gen_name">[2]b_dashboard!$D$24</definedName>
-    <definedName name="sel_scenario">[2]b_dashboard!$D$25</definedName>
-    <definedName name="sel_secproc_co2">[2]b_dashboard!$D$30</definedName>
-    <definedName name="sel_secproc_water">[2]b_dashboard!$D$31</definedName>
-    <definedName name="sel_ship_own_fuel">[2]b_dashboard!$D$33</definedName>
+    <definedName name="sel_region_name">[1]b_dashboard!$D$21</definedName>
+    <definedName name="sel_res_gen" localSheetId="3">IF(sel_res_gen_name="","",INDEX([1]!process[#Data],MATCH(sel_res_gen_name,[1]!process[process_name],0),1))</definedName>
+    <definedName name="sel_res_gen">IF(sel_res_gen_name="","",INDEX([1]!process[#Data],MATCH(sel_res_gen_name,[1]!process[process_name],0),1))</definedName>
+    <definedName name="sel_res_gen_name">[1]b_dashboard!$D$24</definedName>
+    <definedName name="sel_scenario">[1]b_dashboard!$D$25</definedName>
+    <definedName name="sel_secproc_co2">[1]b_dashboard!$D$30</definedName>
+    <definedName name="sel_secproc_water">[1]b_dashboard!$D$31</definedName>
+    <definedName name="sel_ship_own_fuel">[1]b_dashboard!$D$33</definedName>
     <definedName name="sel_ship_possible">TRUE</definedName>
-    <definedName name="sel_transport">[2]b_dashboard!$D$32</definedName>
-    <definedName name="selOutputUnit">[2]b_dashboard!$D$34</definedName>
-    <definedName name="selOutputUnit2">[2]_dims!$CA$2</definedName>
-    <definedName name="tabDatasets_name">[2]!tabDatasetsInput[name]</definedName>
-    <definedName name="target_countries">[2]!country[target_country_code]</definedName>
+    <definedName name="sel_transport">[1]b_dashboard!$D$32</definedName>
+    <definedName name="selOutputUnit">[1]b_dashboard!$D$34</definedName>
+    <definedName name="selOutputUnit2">[1]_dims!$CA$2</definedName>
+    <definedName name="tabDatasets_name">[1]!tabDatasetsInput[name]</definedName>
+    <definedName name="target_countries">[1]!country[target_country_code]</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -3026,37 +3026,6 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="Sheet1"/>
-      <sheetName val="context_cs_type"/>
-      <sheetName val="context_cs_scope"/>
-      <sheetName val="context_cs_countries"/>
-      <sheetName val="_context_data_infobox"/>
-      <sheetName val="certification_schemes"/>
-      <sheetName val="demand_countries"/>
-      <sheetName val="literature"/>
-      <sheetName val="sustainability"/>
-      <sheetName val="context_data"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
       <sheetName val="b_disclaimer"/>
       <sheetName val="b_Info"/>
       <sheetName val="b_dashboard"/>
@@ -3107,6 +3076,7 @@
       <sheetName val="_scenario_2030_medium"/>
       <sheetName val="_scenario_2040_high"/>
       <sheetName val="_scenario_2030_high"/>
+      <sheetName val="ptxboa_v19 - Kopie"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
@@ -4892,6 +4862,38 @@
       <sheetData sheetId="47"/>
       <sheetData sheetId="48"/>
       <sheetData sheetId="49"/>
+      <sheetData sheetId="50" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet1"/>
+      <sheetName val="context_cs_type"/>
+      <sheetName val="context_cs_scope"/>
+      <sheetName val="context_cs_countries"/>
+      <sheetName val="_context_data_infobox"/>
+      <sheetName val="certification_schemes"/>
+      <sheetName val="demand_countries"/>
+      <sheetName val="literature"/>
+      <sheetName val="sustainability"/>
+      <sheetName val="context_data"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -7303,8 +7305,8 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:N43"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -9639,7 +9641,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F35DBB3-2A80-4CA5-AC9F-BFE408866ADC}">
   <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
@@ -10389,6 +10391,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100E2F0DF90B070FE43BFD707F72A4CD00B" ma:contentTypeVersion="15" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="8927d14e1bc908eae180c9caa4b5da89">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1bc94727-11e8-4443-b8f0-9215ff28e4bb" xmlns:ns3="cd34aed5-94da-4c30-bba3-37b78f4daae9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bb67c9392edae2d7a3a1d88d3e91258a" ns2:_="" ns3:_="">
     <xsd:import namespace="1bc94727-11e8-4443-b8f0-9215ff28e4bb"/>
@@ -10625,16 +10636,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22BF5C6F-88A2-47DA-9B5F-9FD29A58E304}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1143ECE1-9C35-446D-8A76-82388033D272}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10651,12 +10661,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22BF5C6F-88A2-47DA-9B5F-9FD29A58E304}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
remove ``load_context_data`` from api - was only used for infobox - data has been integrated in ``data_context_data.xsx`` - import is done via ``import_context_data.xlsx``
</commit_message>
<xml_diff>
--- a/data/context_data.xlsx
+++ b/data/context_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m.haller\Documents\code\ptx-boa\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76AD3648-8699-4454-975D-BA7B66D5F92F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FAED2CA-60E9-4929-B29A-7B9F1505800A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{D16C601B-E1D6-40C0-8CC1-80505BE1FBB6}"/>
   </bookViews>
@@ -16,104 +16,11 @@
     <sheet name="certification_schemes" sheetId="6" r:id="rId1"/>
     <sheet name="certification_schemes_countries" sheetId="10" r:id="rId2"/>
     <sheet name="sustainability" sheetId="9" r:id="rId3"/>
-    <sheet name="supply" sheetId="11" r:id="rId4"/>
-    <sheet name="demand_countries" sheetId="8" r:id="rId5"/>
-    <sheet name="literature" sheetId="7" r:id="rId6"/>
+    <sheet name="infobox" sheetId="12" r:id="rId4"/>
+    <sheet name="supply" sheetId="11" r:id="rId5"/>
+    <sheet name="demand_countries" sheetId="8" r:id="rId6"/>
+    <sheet name="literature" sheetId="7" r:id="rId7"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId7"/>
-    <externalReference r:id="rId8"/>
-  </externalReferences>
-  <definedNames>
-    <definedName name="can_use_pipeline" localSheetId="3">INDEX([1]!chains[CAN_PIPELINE],supply!sel_chain_index)</definedName>
-    <definedName name="can_use_pipeline">INDEX([1]!chains[CAN_PIPELINE],sel_chain_index)</definedName>
-    <definedName name="chains_chain">[1]!chains[chain]</definedName>
-    <definedName name="compCostCountries_DELETE">[1]!Table23[Country code]</definedName>
-    <definedName name="context_data_carbonsource" localSheetId="3">[2]!Table33353637[#All]</definedName>
-    <definedName name="context_data_carbonsource">#REF!</definedName>
-    <definedName name="context_data_infobox" localSheetId="3">[2]!Table32[#Data]</definedName>
-    <definedName name="context_data_infobox">#REF!</definedName>
-    <definedName name="context_data_re" localSheetId="3">[2]!Table33[#All]</definedName>
-    <definedName name="context_data_re">#REF!</definedName>
-    <definedName name="context_data_transport_mode" localSheetId="3">[2]!Table3335[#All]</definedName>
-    <definedName name="context_data_transport_mode">#REF!</definedName>
-    <definedName name="context_data_watersource" localSheetId="3">[2]!Table333536[#All]</definedName>
-    <definedName name="context_data_watersource">#REF!</definedName>
-    <definedName name="conv_fact_to_mass">[1]_calc!$BM$6</definedName>
-    <definedName name="country_area">[1]!Table22[#All]</definedName>
-    <definedName name="country_country_code">[1]!country[target_country_code]</definedName>
-    <definedName name="country_country_name">[1]!country[target_country_name]</definedName>
-    <definedName name="country_energy_use">[1]!Table25[#All]</definedName>
-    <definedName name="country_pop">[1]!Table26[#All]</definedName>
-    <definedName name="country_pop_and_energy_use" localSheetId="3">[1]!Table26[#Data]</definedName>
-    <definedName name="country_pop_and_energy_use">[1]!Table26[#Data]</definedName>
-    <definedName name="default_scenarios">[1]!tab_default_scenario[default_scenario]</definedName>
-    <definedName name="dim_bool_bool">[1]!dim_bool[BOOL]</definedName>
-    <definedName name="flh_deriv">[1]_calc!$X$257:$X$335</definedName>
-    <definedName name="flh_ely">[1]_calc!$Q$257:$Q$335</definedName>
-    <definedName name="flh_region_code">[1]_calc!$B$257:$B$335</definedName>
-    <definedName name="flow_flow_code">[1]!flow[flow_code]</definedName>
-    <definedName name="flow_flow_name">[1]!flow[flow_name]</definedName>
-    <definedName name="flow_short_names">[1]_dims!$X$22:$Y$37</definedName>
-    <definedName name="input_scenarios">[1]!tabDatasetsInput[name]</definedName>
-    <definedName name="mapMaxValue">[1]_map!$G$3</definedName>
-    <definedName name="mapMinValue">[1]_map!$G$2</definedName>
-    <definedName name="output_scenario_name">[1]_todo_dev!$A$9</definedName>
-    <definedName name="output_scenario_names">[1]!output_scenarios[scenario]</definedName>
-    <definedName name="output_units">[1]!tabOutputUnit[output_unit]</definedName>
-    <definedName name="process_classes_process_class">[1]!process_classes[process_class]</definedName>
-    <definedName name="process_classes_process_class_name">[1]!process_classes[process_class_name]</definedName>
-    <definedName name="process_main_flow_code_out">[1]!process[main_flow_code_out]</definedName>
-    <definedName name="process_process_class">[1]!process[process_class]</definedName>
-    <definedName name="process_process_code">[1]!process[process_code]</definedName>
-    <definedName name="process_process_name">[1]!process[process_name]</definedName>
-    <definedName name="process_res_gen_name">[1]!process_res_gen[process_name]</definedName>
-    <definedName name="process_res_gen_process_code">[1]!process_res_gen[process_code]</definedName>
-    <definedName name="process_res_gen_process_name">[1]!process_res_gen[process_name]</definedName>
-    <definedName name="region_region_code">[1]!region[source_region_code]</definedName>
-    <definedName name="region_region_name">[1]!region[region_name]</definedName>
-    <definedName name="regions_by_cost">[1]!Table21[#All]</definedName>
-    <definedName name="release_date">[1]_release!$B$2</definedName>
-    <definedName name="release_version">[1]_release!$B$1</definedName>
-    <definedName name="saved_outputs">[1]!tabDatasetsOutput[name]</definedName>
-    <definedName name="secondary_process_CO2_G">[1]!tabSelCo2[name]</definedName>
-    <definedName name="secondary_process_H2O_L">[1]!tabSelWater[name]</definedName>
-    <definedName name="sel_chain">[1]b_dashboard!$D$23</definedName>
-    <definedName name="sel_chain_deriv_proc_code">[1]_calc!$X$2</definedName>
-    <definedName name="sel_chain_ely_proc_code">[1]_calc!$Q$2</definedName>
-    <definedName name="sel_chain_flow_out">[1]_calc!$BM$5</definedName>
-    <definedName name="sel_chain_index" localSheetId="3">MATCH(sel_chain,[1]!chains[chain],)</definedName>
-    <definedName name="sel_chain_index">MATCH(sel_chain,[1]!chains[chain],)</definedName>
-    <definedName name="sel_chain_range" localSheetId="3">OFFSET([1]!chains[[#Headers],[chain]],supply!sel_chain_index,1,1,COUNTA([1]!chains[#Headers])-1)</definedName>
-    <definedName name="sel_chain_range">OFFSET([1]!chains[[#Headers],[chain]],sel_chain_index,1,1,COUNTA([1]!chains[#Headers])-1)</definedName>
-    <definedName name="sel_chain_range_word" localSheetId="3">OFFSET([1]!chains[[#Headers],[chain]],sel_chain_index_world,1,1,COUNTA([1]!chains[#Headers])-1)</definedName>
-    <definedName name="sel_chain_range_word">OFFSET([1]!chains[[#Headers],[chain]],sel_chain_index_world,1,1,COUNTA([1]!chains[#Headers])-1)</definedName>
-    <definedName name="sel_choices_transport" localSheetId="3">OFFSET([1]!choicesTransport[none],0,supply!sel_pipeline_possible*2+sel_ship_possible,supply!sel_pipeline_possible+sel_ship_possible)</definedName>
-    <definedName name="sel_choices_transport">OFFSET([1]!choicesTransport[none],0,sel_pipeline_possible*2+sel_ship_possible,sel_pipeline_possible+sel_ship_possible)</definedName>
-    <definedName name="sel_country_code" localSheetId="3">IF(sel_country_name="","",INDEX(country_country_code,MATCH(sel_country_name,country_country_name,0),1))</definedName>
-    <definedName name="sel_country_code">IF(sel_country_name="","",INDEX(country_country_code,MATCH(sel_country_name,country_country_name,0),1))</definedName>
-    <definedName name="sel_country_name">[1]b_dashboard!$D$22</definedName>
-    <definedName name="sel_pipeline_possible" localSheetId="3">AND(INDEX([1]_calc!$AQ$14:$AQ$92,MATCH(_xlfn.SINGLE(supply!sel_region_code),[1]_calc!$B$14:$B$92,0))&gt;0,_xlfn.SINGLE(supply!can_use_pipeline)=TRUE)</definedName>
-    <definedName name="sel_pipeline_possible">AND(INDEX([1]_calc!$AQ$14:$AQ$92,MATCH(_xlfn.SINGLE(sel_region_code),[1]_calc!$B$14:$B$92,0))&gt;0,_xlfn.SINGLE(can_use_pipeline)=TRUE)</definedName>
-    <definedName name="sel_region_code" localSheetId="3">IF(sel_region_name="","",INDEX([1]!region[source_region_code],MATCH(sel_region_name,[1]!region[region_name],0),1))</definedName>
-    <definedName name="sel_region_code">IF(sel_region_name="","",INDEX([1]!region[source_region_code],MATCH(sel_region_name,[1]!region[region_name],0),1))</definedName>
-    <definedName name="sel_region_country_code" localSheetId="3">IF(supply!sel_region_code="","",LEFT(supply!sel_region_code,3))</definedName>
-    <definedName name="sel_region_country_code">IF(sel_region_code="","",LEFT(sel_region_code,3))</definedName>
-    <definedName name="sel_region_name">[1]b_dashboard!$D$21</definedName>
-    <definedName name="sel_res_gen" localSheetId="3">IF(sel_res_gen_name="","",INDEX([1]!process[#Data],MATCH(sel_res_gen_name,[1]!process[process_name],0),1))</definedName>
-    <definedName name="sel_res_gen">IF(sel_res_gen_name="","",INDEX([1]!process[#Data],MATCH(sel_res_gen_name,[1]!process[process_name],0),1))</definedName>
-    <definedName name="sel_res_gen_name">[1]b_dashboard!$D$24</definedName>
-    <definedName name="sel_scenario">[1]b_dashboard!$D$25</definedName>
-    <definedName name="sel_secproc_co2">[1]b_dashboard!$D$30</definedName>
-    <definedName name="sel_secproc_water">[1]b_dashboard!$D$31</definedName>
-    <definedName name="sel_ship_own_fuel">[1]b_dashboard!$D$33</definedName>
-    <definedName name="sel_ship_possible">TRUE</definedName>
-    <definedName name="sel_transport">[1]b_dashboard!$D$32</definedName>
-    <definedName name="selOutputUnit">[1]b_dashboard!$D$34</definedName>
-    <definedName name="selOutputUnit2">[1]_dims!$CA$2</definedName>
-    <definedName name="tabDatasets_name">[1]!tabDatasetsInput[name]</definedName>
-    <definedName name="target_countries">[1]!country[target_country_code]</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -191,6 +98,53 @@
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
+    <author>tc={7C326BBD-CADA-414E-8630-DB89B2783121}</author>
+    <author>tc={9396247F-F92D-4843-8B4A-446356C13809}</author>
+    <author>tc={28CB0F6E-75D7-4DD3-8285-1765A8E1BC92}</author>
+    <author>tc={BCC66E9D-D639-4CC4-926D-7484C4028444}</author>
+  </authors>
+  <commentList>
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{7C326BBD-CADA-414E-8630-DB89B2783121}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Diese Zeile mit Infos zur Verlinkung in Bubble/Point Chart nutzen</t>
+      </text>
+    </comment>
+    <comment ref="B7" authorId="1" shapeId="0" xr:uid="{9396247F-F92D-4843-8B4A-446356C13809}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    only referring to renewable H2
+Reply:
+    new targets as stated in the RePowerPlan EU</t>
+      </text>
+    </comment>
+    <comment ref="E7" authorId="2" shapeId="0" xr:uid="{28CB0F6E-75D7-4DD3-8285-1765A8E1BC92}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    53.000 km by 2040</t>
+      </text>
+    </comment>
+    <comment ref="E10" authorId="3" shapeId="0" xr:uid="{BCC66E9D-D639-4CC4-926D-7484C4028444}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    non-renewable</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
     <author>tc={41EB567B-49B3-4249-A497-693C9780E7FB}</author>
     <author>tc={C876D122-024F-4AEB-B1DC-30DFDDAC00DC}</author>
   </authors>
@@ -217,7 +171,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1153" uniqueCount="605">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1241" uniqueCount="659">
   <si>
     <t>topic</t>
   </si>
@@ -2172,12 +2126,178 @@
   - How can potential **risks be reduced to a minimum** and workers protected in the best possible way?
   - Are there mechanisms in place for **monitoring potential risks** as well as regular comprehensive audits?</t>
   </si>
+  <si>
+    <t>Target Country InfoBox:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RE generation: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carbon source: </t>
+  </si>
+  <si>
+    <t>Water source:</t>
+  </si>
+  <si>
+    <t>Mode of transportation:</t>
+  </si>
+  <si>
+    <t>key_info_1</t>
+  </si>
+  <si>
+    <t>key_info_2</t>
+  </si>
+  <si>
+    <t>key_info_3</t>
+  </si>
+  <si>
+    <t>key_info_4</t>
+  </si>
+  <si>
+    <t>selection</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>Port of Rotterdam functions as a central import hub to the European market</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Home of the first declared H2 valley in Europe </t>
+  </si>
+  <si>
+    <t>PV tilted</t>
+  </si>
+  <si>
+    <t>To secure that existing RES-E plants are not withdrawn from existing capacities, electricity should be sourced from new, additional RES-E plants. (How) Can you ensure this additionality of electricity supply?</t>
+  </si>
+  <si>
+    <t>DAC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How are additional energy demands of DAC sourced (preferably from RES-E plants or excess heat)? Are there any potential land conflicts if deploying this technology? </t>
+  </si>
+  <si>
+    <t>Water desalination</t>
+  </si>
+  <si>
+    <t>How is brine disposal managed? Can chemicals be reduced to a minimum? How are additional energy requirements of desalination plants sourced?</t>
+  </si>
+  <si>
+    <t>Ship</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If you have only one option (ship) displayed in the dropdown menu, a pipeline option to your selected target country does not seem feasible. This might impact your competitiveness towards this country. </t>
+  </si>
+  <si>
+    <t>Both importing and exporting country for H2 &amp; derivatives</t>
+  </si>
+  <si>
+    <t>Considerable domestic installed electrolyser capacity foreseen by 2030 (4 GW)</t>
+  </si>
+  <si>
+    <t>Plans to connect to France &amp; Germany via Europe's first offshore green H2 pipeline (H2Med)</t>
+  </si>
+  <si>
+    <t>PV tracking</t>
+  </si>
+  <si>
+    <t>Specific costs</t>
+  </si>
+  <si>
+    <t>CO2 sourcing should not delay the decarbonisation of economic sectors. Is it possible to source it from the air or from unavoidable emissions (e.g. cement industry)?</t>
+  </si>
+  <si>
+    <t>Is the region affected by water stress? If yes, how is this issue addressed? Could additional water demand lead to rising water costs to the local public?</t>
+  </si>
+  <si>
+    <t>Pipeline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Updated National Hydrogen Strategy in preparation </t>
+  </si>
+  <si>
+    <t>Part of project to build Europe's first offshore pipeline for green H2 from Spain (H2Med)</t>
+  </si>
+  <si>
+    <t>Wind-PV-Hybrid</t>
+  </si>
+  <si>
+    <t>2,8-3,3 Mt</t>
+  </si>
+  <si>
+    <t>High reliance on H2 imports projected</t>
+  </si>
+  <si>
+    <t>LNG import infrastructure in development 
+(8 terminals in development)</t>
+  </si>
+  <si>
+    <t>Plans to connect to Spain &amp; Portugal via France with Europe's first offshore green H2 pipeline (H2Med)</t>
+  </si>
+  <si>
+    <t>Wind Offshore</t>
+  </si>
+  <si>
+    <t>EU</t>
+  </si>
+  <si>
+    <t>20 Mt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Large domestic electrolyser capacities foreseen by 2030 (40 GW) </t>
+  </si>
+  <si>
+    <t>Half of the hydrogen demand covered with domestic capacities by 2030 (only 10 Mt imports)</t>
+  </si>
+  <si>
+    <t>Large-scale H2 pipeline infrastructure planned (European H2 Backbone)</t>
+  </si>
+  <si>
+    <t>Wind Onshore</t>
+  </si>
+  <si>
+    <t>Released the first H2 strategy worldwide in 2017  (Basic Hydrogen Strategy)</t>
+  </si>
+  <si>
+    <t>Well-developed LNG import infrastructure 
+(45 terminals operating)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Imports of blue and green H2 from overseas planned from 2030 on </t>
+  </si>
+  <si>
+    <t>Goals for share of green H2 in 2030 at 50% &amp; in 2040 at 70%</t>
+  </si>
+  <si>
+    <t>High cost-competitiveness in alkaline electrolysis technology</t>
+  </si>
+  <si>
+    <t>Well-developed LNG import infrastructure 
+(32 terminals operating)</t>
+  </si>
+  <si>
+    <t>Considerable domestic production capacities of green H2 foreseen by 2030 (5 Mt p/a)</t>
+  </si>
+  <si>
+    <t>80% of H2 demand expected to be green by 2050</t>
+  </si>
+  <si>
+    <t>Goal to become largely independent from H2 imports by 2030-2035</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Large-scale H2 pipeline infrastructure already in place (~ 2.600 km) </t>
+  </si>
+  <si>
+    <t>Extensive LNG export infrastructure 
+(36 terminals operating)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2213,8 +2333,43 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2239,8 +2394,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF66CCFF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -2263,12 +2424,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2366,12 +2547,108 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="91">
+  <dxfs count="100">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF4472C4"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF4472C4"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color rgb="FF4472C4"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color rgb="FF4472C4"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FF000000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FF000000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FF000000"/>
+      </font>
+      <border>
+        <top style="double">
+          <color rgb="FF4472C4"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF4472C4"/>
+          <bgColor rgb="FF4472C4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color rgb="FF4472C4"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF4472C4"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF4472C4"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF4472C4"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -3010,7 +3287,19 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="TableStyleLight9 2" pivot="0" count="9" xr9:uid="{CB3F1850-4632-49A9-A1EC-1C038F9E06CB}">
+      <tableStyleElement type="wholeTable" dxfId="8"/>
+      <tableStyleElement type="headerRow" dxfId="7"/>
+      <tableStyleElement type="totalRow" dxfId="6"/>
+      <tableStyleElement type="firstColumn" dxfId="5"/>
+      <tableStyleElement type="lastColumn" dxfId="4"/>
+      <tableStyleElement type="firstRowStripe" dxfId="3"/>
+      <tableStyleElement type="secondRowStripe" dxfId="2"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="1"/>
+      <tableStyleElement type="secondColumnStripe" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -3022,1886 +3311,10 @@
 </styleSheet>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="b_disclaimer"/>
-      <sheetName val="b_Info"/>
-      <sheetName val="b_dashboard"/>
-      <sheetName val="_release"/>
-      <sheetName val="_todo_dev"/>
-      <sheetName val="_dims"/>
-      <sheetName val="_input"/>
-      <sheetName val="_data_storage"/>
-      <sheetName val="_data_flh"/>
-      <sheetName val="_calc"/>
-      <sheetName val="_pivot_output"/>
-      <sheetName val="_colors"/>
-      <sheetName val="_map"/>
-      <sheetName val="_output"/>
-      <sheetName val="m_CompareScenarios"/>
-      <sheetName val="m_CompareTargetCountries"/>
-      <sheetName val="m_CompareRE"/>
-      <sheetName val="m_CompareChains"/>
-      <sheetName val="_user_scenario_changes"/>
-      <sheetName val="b_MarketScanning"/>
-      <sheetName val="_MarketScanning_2"/>
-      <sheetName val="b_CostComponents"/>
-      <sheetName val="b_CompareCosts"/>
-      <sheetName val="b_CompareInputData"/>
-      <sheetName val="r_RegDataMAR"/>
-      <sheetName val="r_RegDataARG"/>
-      <sheetName val="r_RegDataZAF"/>
-      <sheetName val="b_context_demand"/>
-      <sheetName val="b_context_supply"/>
-      <sheetName val="b_context_certification"/>
-      <sheetName val="b_context_sustainability"/>
-      <sheetName val="_country_size"/>
-      <sheetName val="cd_rank_countries"/>
-      <sheetName val="e_view_data_processes"/>
-      <sheetName val="e_view_data_transport"/>
-      <sheetName val="e_view_data_chain"/>
-      <sheetName val="_view_data_regions"/>
-      <sheetName val="a_edit_data_speccost"/>
-      <sheetName val="a_edit_data_process"/>
-      <sheetName val="_dev_map"/>
-      <sheetName val="_agora_colors"/>
-      <sheetName val="_outputs"/>
-      <sheetName val="_results"/>
-      <sheetName val="_index_storage"/>
-      <sheetName val="_scenario_2040_medium"/>
-      <sheetName val="_scenario_2030_low"/>
-      <sheetName val="_scenario_2040_low"/>
-      <sheetName val="_scenario_2030_medium"/>
-      <sheetName val="_scenario_2040_high"/>
-      <sheetName val="_scenario_2030_high"/>
-      <sheetName val="ptxboa_v19 - Kopie"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2">
-        <row r="21">
-          <cell r="D21" t="str">
-            <v>South Africa</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="D22" t="str">
-            <v>Spain</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="D23" t="str">
-            <v>Methane (AEL)</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="D24" t="str">
-            <v>Wind-PV-Hybrid</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="D25" t="str">
-            <v>2030 (medium)</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="D30" t="str">
-            <v>Specific costs</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="D31" t="str">
-            <v>Water desalination</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="D32" t="str">
-            <v>Ship</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="D33" t="b">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="D34" t="str">
-            <v>USD/MWh</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="3">
-        <row r="1">
-          <cell r="B1" t="str">
-            <v>1.0.9</v>
-          </cell>
-        </row>
-        <row r="2">
-          <cell r="B2">
-            <v>45205</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="4">
-        <row r="9">
-          <cell r="A9" t="str">
-            <v>FT e-fuels (SEOC)</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="5">
-        <row r="2">
-          <cell r="CA2" t="str">
-            <v>USD/MWh CH4</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="X22" t="str">
-            <v>BFUEL-L</v>
-          </cell>
-          <cell r="Y22" t="str">
-            <v>bunker fuel</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="X23" t="str">
-            <v>CH3OH-L</v>
-          </cell>
-          <cell r="Y23" t="str">
-            <v>CH3OH</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="X24" t="str">
-            <v>CH4-G</v>
-          </cell>
-          <cell r="Y24" t="str">
-            <v>CH4</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="X25" t="str">
-            <v>CH4-L</v>
-          </cell>
-          <cell r="Y25" t="str">
-            <v>CH4</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="X26" t="str">
-            <v>CHX-L</v>
-          </cell>
-          <cell r="Y26" t="str">
-            <v>FT e-fuels</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="X27" t="str">
-            <v>CO2-G</v>
-          </cell>
-          <cell r="Y27" t="str">
-            <v>CO2</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="X28" t="str">
-            <v>C-S</v>
-          </cell>
-          <cell r="Y28" t="str">
-            <v>C</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="X29" t="str">
-            <v>DRI-S</v>
-          </cell>
-          <cell r="Y29" t="str">
-            <v>Green iron</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="X30" t="str">
-            <v>EL</v>
-          </cell>
-          <cell r="Y30" t="str">
-            <v>electricity</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="X31" t="str">
-            <v>H2-G</v>
-          </cell>
-          <cell r="Y31" t="str">
-            <v>H2</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="X32" t="str">
-            <v>H2-L</v>
-          </cell>
-          <cell r="Y32" t="str">
-            <v>H2</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="X33" t="str">
-            <v>H2O-L</v>
-          </cell>
-          <cell r="Y33" t="str">
-            <v>H2O</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="X34" t="str">
-            <v>HEAT</v>
-          </cell>
-          <cell r="Y34" t="str">
-            <v>heat</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="X35" t="str">
-            <v>LOHC-L</v>
-          </cell>
-          <cell r="Y35" t="str">
-            <v>H2 (LOHC)</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="X36" t="str">
-            <v>N2-G</v>
-          </cell>
-          <cell r="Y36" t="str">
-            <v>N2</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="X37" t="str">
-            <v>NH3-L</v>
-          </cell>
-          <cell r="Y37" t="str">
-            <v>NH3</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9">
-        <row r="2">
-          <cell r="Q2" t="str">
-            <v>AEL-EL</v>
-          </cell>
-          <cell r="X2" t="str">
-            <v>CH4SYN</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="BM5" t="str">
-            <v>CH4-G</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="BM6">
-            <v>1000</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="B14" t="str">
-            <v>ARE</v>
-          </cell>
-          <cell r="AQ14">
-            <v>6000</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="B15" t="str">
-            <v>ARG</v>
-          </cell>
-          <cell r="AQ15">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="B16" t="str">
-            <v>ARG-BA</v>
-          </cell>
-          <cell r="AQ16">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="B17" t="str">
-            <v>ARG-CAT</v>
-          </cell>
-          <cell r="AQ17">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="B18" t="str">
-            <v>ARG-CBA</v>
-          </cell>
-          <cell r="AQ18">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="B19" t="str">
-            <v>ARG-CHA</v>
-          </cell>
-          <cell r="AQ19">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="B20" t="str">
-            <v>ARG-CHU</v>
-          </cell>
-          <cell r="AQ20">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="B21" t="str">
-            <v>ARG-COR</v>
-          </cell>
-          <cell r="AQ21">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="B22" t="str">
-            <v>ARG-CRB</v>
-          </cell>
-          <cell r="AQ22">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="B23" t="str">
-            <v>ARG-CRU</v>
-          </cell>
-          <cell r="AQ23">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="B24" t="str">
-            <v>ARG-EST</v>
-          </cell>
-          <cell r="AQ24">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="B25" t="str">
-            <v>ARG-FOR</v>
-          </cell>
-          <cell r="AQ25">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="B26" t="str">
-            <v>ARG-FUE</v>
-          </cell>
-          <cell r="AQ26">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="B27" t="str">
-            <v>ARG-JUJ</v>
-          </cell>
-          <cell r="AQ27">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="B28" t="str">
-            <v>ARG-LAR</v>
-          </cell>
-          <cell r="AQ28">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="B29" t="str">
-            <v>ARG-MEN</v>
-          </cell>
-          <cell r="AQ29">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="B30" t="str">
-            <v>ARG-MIS</v>
-          </cell>
-          <cell r="AQ30">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="B31" t="str">
-            <v>ARG-NEG</v>
-          </cell>
-          <cell r="AQ31">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="B32" t="str">
-            <v>ARG-NEU</v>
-          </cell>
-          <cell r="AQ32">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="B33" t="str">
-            <v>ARG-PAM</v>
-          </cell>
-          <cell r="AQ33">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="B34" t="str">
-            <v>ARG-RIO</v>
-          </cell>
-          <cell r="AQ34">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="B35" t="str">
-            <v>ARG-SAF</v>
-          </cell>
-          <cell r="AQ35">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="B36" t="str">
-            <v>ARG-SAJ</v>
-          </cell>
-          <cell r="AQ36">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="B37" t="str">
-            <v>ARG-SAL</v>
-          </cell>
-          <cell r="AQ37">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="B38" t="str">
-            <v>ARG-SAT</v>
-          </cell>
-          <cell r="AQ38">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="B39" t="str">
-            <v>ARG-TUC</v>
-          </cell>
-          <cell r="AQ39">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="40">
-          <cell r="B40" t="str">
-            <v>AUS</v>
-          </cell>
-          <cell r="AQ40">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="B41" t="str">
-            <v>BRA</v>
-          </cell>
-          <cell r="AQ41">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="B42" t="str">
-            <v>CHL</v>
-          </cell>
-          <cell r="AQ42">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="43">
-          <cell r="B43" t="str">
-            <v>CHN</v>
-          </cell>
-          <cell r="AQ43">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="44">
-          <cell r="B44" t="str">
-            <v>COL</v>
-          </cell>
-          <cell r="AQ44">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="45">
-          <cell r="B45" t="str">
-            <v>CRI</v>
-          </cell>
-          <cell r="AQ45">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="46">
-          <cell r="B46" t="str">
-            <v>DNK</v>
-          </cell>
-          <cell r="AQ46">
-            <v>2000</v>
-          </cell>
-        </row>
-        <row r="47">
-          <cell r="B47" t="str">
-            <v>DZA</v>
-          </cell>
-          <cell r="AQ47">
-            <v>1000</v>
-          </cell>
-        </row>
-        <row r="48">
-          <cell r="B48" t="str">
-            <v>EGY</v>
-          </cell>
-          <cell r="AQ48">
-            <v>4500</v>
-          </cell>
-        </row>
-        <row r="49">
-          <cell r="B49" t="str">
-            <v>ESP</v>
-          </cell>
-          <cell r="AQ49">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="50">
-          <cell r="B50" t="str">
-            <v>IDN</v>
-          </cell>
-          <cell r="AQ50">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="51">
-          <cell r="B51" t="str">
-            <v>IND</v>
-          </cell>
-          <cell r="AQ51">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="52">
-          <cell r="B52" t="str">
-            <v>JOR</v>
-          </cell>
-          <cell r="AQ52">
-            <v>4000</v>
-          </cell>
-        </row>
-        <row r="53">
-          <cell r="B53" t="str">
-            <v>KAZ</v>
-          </cell>
-          <cell r="AQ53">
-            <v>5000</v>
-          </cell>
-        </row>
-        <row r="54">
-          <cell r="B54" t="str">
-            <v>KEN</v>
-          </cell>
-          <cell r="AQ54">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="55">
-          <cell r="B55" t="str">
-            <v>MAR</v>
-          </cell>
-          <cell r="AQ55">
-            <v>250</v>
-          </cell>
-        </row>
-        <row r="56">
-          <cell r="B56" t="str">
-            <v>MAR-BEN</v>
-          </cell>
-          <cell r="AQ56">
-            <v>250</v>
-          </cell>
-        </row>
-        <row r="57">
-          <cell r="B57" t="str">
-            <v>MAR-CAS</v>
-          </cell>
-          <cell r="AQ57">
-            <v>250</v>
-          </cell>
-        </row>
-        <row r="58">
-          <cell r="B58" t="str">
-            <v>MAR-DAK</v>
-          </cell>
-          <cell r="AQ58">
-            <v>250</v>
-          </cell>
-        </row>
-        <row r="59">
-          <cell r="B59" t="str">
-            <v>MAR-DRA</v>
-          </cell>
-          <cell r="AQ59">
-            <v>250</v>
-          </cell>
-        </row>
-        <row r="60">
-          <cell r="B60" t="str">
-            <v>MAR-FES</v>
-          </cell>
-          <cell r="AQ60">
-            <v>250</v>
-          </cell>
-        </row>
-        <row r="61">
-          <cell r="B61" t="str">
-            <v>MAR-GUE</v>
-          </cell>
-          <cell r="AQ61">
-            <v>250</v>
-          </cell>
-        </row>
-        <row r="62">
-          <cell r="B62" t="str">
-            <v>MAR-LAA</v>
-          </cell>
-          <cell r="AQ62">
-            <v>250</v>
-          </cell>
-        </row>
-        <row r="63">
-          <cell r="B63" t="str">
-            <v>MAR-LOR</v>
-          </cell>
-          <cell r="AQ63">
-            <v>250</v>
-          </cell>
-        </row>
-        <row r="64">
-          <cell r="B64" t="str">
-            <v>MAR-MAR</v>
-          </cell>
-          <cell r="AQ64">
-            <v>250</v>
-          </cell>
-        </row>
-        <row r="65">
-          <cell r="B65" t="str">
-            <v>MAR-RAB</v>
-          </cell>
-          <cell r="AQ65">
-            <v>250</v>
-          </cell>
-        </row>
-        <row r="66">
-          <cell r="B66" t="str">
-            <v>MAR-SOU</v>
-          </cell>
-          <cell r="AQ66">
-            <v>250</v>
-          </cell>
-        </row>
-        <row r="67">
-          <cell r="B67" t="str">
-            <v>MAR-TAN</v>
-          </cell>
-          <cell r="AQ67">
-            <v>250</v>
-          </cell>
-        </row>
-        <row r="68">
-          <cell r="B68" t="str">
-            <v>MEX</v>
-          </cell>
-          <cell r="AQ68">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="69">
-          <cell r="B69" t="str">
-            <v>MRT</v>
-          </cell>
-          <cell r="AQ69">
-            <v>3000</v>
-          </cell>
-        </row>
-        <row r="70">
-          <cell r="B70" t="str">
-            <v>NAM</v>
-          </cell>
-          <cell r="AQ70">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="71">
-          <cell r="B71" t="str">
-            <v>NOR</v>
-          </cell>
-          <cell r="AQ71">
-            <v>2000</v>
-          </cell>
-        </row>
-        <row r="72">
-          <cell r="B72" t="str">
-            <v>PER</v>
-          </cell>
-          <cell r="AQ72">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="73">
-          <cell r="B73" t="str">
-            <v>PRT</v>
-          </cell>
-          <cell r="AQ73">
-            <v>250</v>
-          </cell>
-        </row>
-        <row r="74">
-          <cell r="B74" t="str">
-            <v>RUS</v>
-          </cell>
-          <cell r="AQ74">
-            <v>5000</v>
-          </cell>
-        </row>
-        <row r="75">
-          <cell r="B75" t="str">
-            <v>SAU</v>
-          </cell>
-          <cell r="AQ75">
-            <v>5000</v>
-          </cell>
-        </row>
-        <row r="76">
-          <cell r="B76" t="str">
-            <v>SWE</v>
-          </cell>
-          <cell r="AQ76">
-            <v>3000</v>
-          </cell>
-        </row>
-        <row r="77">
-          <cell r="B77" t="str">
-            <v>THA</v>
-          </cell>
-          <cell r="AQ77">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="78">
-          <cell r="B78" t="str">
-            <v>TUN</v>
-          </cell>
-          <cell r="AQ78">
-            <v>1500</v>
-          </cell>
-        </row>
-        <row r="79">
-          <cell r="B79" t="str">
-            <v>UKR</v>
-          </cell>
-          <cell r="AQ79">
-            <v>3000</v>
-          </cell>
-        </row>
-        <row r="80">
-          <cell r="B80" t="str">
-            <v>URY</v>
-          </cell>
-          <cell r="AQ80">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="81">
-          <cell r="B81" t="str">
-            <v>USA</v>
-          </cell>
-          <cell r="AQ81">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="82">
-          <cell r="B82" t="str">
-            <v>VNM</v>
-          </cell>
-          <cell r="AQ82">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="83">
-          <cell r="B83" t="str">
-            <v>ZAF</v>
-          </cell>
-          <cell r="AQ83">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="84">
-          <cell r="B84" t="str">
-            <v>ZAF-EC</v>
-          </cell>
-          <cell r="AQ84">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="85">
-          <cell r="B85" t="str">
-            <v>ZAF-FRS</v>
-          </cell>
-          <cell r="AQ85">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="86">
-          <cell r="B86" t="str">
-            <v>ZAF-GAU</v>
-          </cell>
-          <cell r="AQ86">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="87">
-          <cell r="B87" t="str">
-            <v>ZAF-KWA</v>
-          </cell>
-          <cell r="AQ87">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="88">
-          <cell r="B88" t="str">
-            <v>ZAF-LIM</v>
-          </cell>
-          <cell r="AQ88">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="89">
-          <cell r="B89" t="str">
-            <v>ZAF-MPU</v>
-          </cell>
-          <cell r="AQ89">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="90">
-          <cell r="B90" t="str">
-            <v>ZAF-NC</v>
-          </cell>
-          <cell r="AQ90">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="91">
-          <cell r="B91" t="str">
-            <v>ZAF-NW</v>
-          </cell>
-          <cell r="AQ91">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="92">
-          <cell r="B92" t="str">
-            <v>ZAF-WC</v>
-          </cell>
-          <cell r="AQ92">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="257">
-          <cell r="B257" t="str">
-            <v>ARE</v>
-          </cell>
-          <cell r="Q257">
-            <v>2960.5180413305925</v>
-          </cell>
-          <cell r="X257">
-            <v>7438.2448855443708</v>
-          </cell>
-        </row>
-        <row r="258">
-          <cell r="B258" t="str">
-            <v>ARG</v>
-          </cell>
-          <cell r="Q258">
-            <v>6151.7249999999995</v>
-          </cell>
-          <cell r="X258">
-            <v>6652.8499999999995</v>
-          </cell>
-        </row>
-        <row r="259">
-          <cell r="B259" t="str">
-            <v>ARG-BA</v>
-          </cell>
-          <cell r="Q259">
-            <v>4938.9666441569962</v>
-          </cell>
-          <cell r="X259">
-            <v>6606.7151892591291</v>
-          </cell>
-        </row>
-        <row r="260">
-          <cell r="B260" t="str">
-            <v>ARG-CAT</v>
-          </cell>
-          <cell r="Q260">
-            <v>4783.096568140877</v>
-          </cell>
-          <cell r="X260">
-            <v>6664.7838090518426</v>
-          </cell>
-        </row>
-        <row r="261">
-          <cell r="B261" t="str">
-            <v>ARG-CBA</v>
-          </cell>
-          <cell r="Q261">
-            <v>4756.5176239964449</v>
-          </cell>
-          <cell r="X261">
-            <v>6674.6856621942961</v>
-          </cell>
-        </row>
-        <row r="262">
-          <cell r="B262" t="str">
-            <v>ARG-CHA</v>
-          </cell>
-          <cell r="Q262">
-            <v>4215.8821233282515</v>
-          </cell>
-          <cell r="X262">
-            <v>6876.0967228490554</v>
-          </cell>
-        </row>
-        <row r="263">
-          <cell r="B263" t="str">
-            <v>ARG-CHU</v>
-          </cell>
-          <cell r="Q263">
-            <v>6701.2899251803447</v>
-          </cell>
-          <cell r="X263">
-            <v>6070.8938761280278</v>
-          </cell>
-        </row>
-        <row r="264">
-          <cell r="B264" t="str">
-            <v>ARG-COR</v>
-          </cell>
-          <cell r="Q264">
-            <v>4147.3122928125722</v>
-          </cell>
-          <cell r="X264">
-            <v>6901.6420713805719</v>
-          </cell>
-        </row>
-        <row r="265">
-          <cell r="B265" t="str">
-            <v>ARG-CRB</v>
-          </cell>
-          <cell r="Q265">
-            <v>3855.8308972693135</v>
-          </cell>
-          <cell r="X265">
-            <v>7010.2320122278488</v>
-          </cell>
-        </row>
-        <row r="266">
-          <cell r="B266" t="str">
-            <v>ARG-CRU</v>
-          </cell>
-          <cell r="Q266">
-            <v>6675.7458807710309</v>
-          </cell>
-          <cell r="X266">
-            <v>6051.0028757190294</v>
-          </cell>
-        </row>
-        <row r="267">
-          <cell r="B267" t="str">
-            <v>ARG-EST</v>
-          </cell>
-          <cell r="Q267">
-            <v>4866.4641374412286</v>
-          </cell>
-          <cell r="X267">
-            <v>6633.7256367042255</v>
-          </cell>
-        </row>
-        <row r="268">
-          <cell r="B268" t="str">
-            <v>ARG-FOR</v>
-          </cell>
-          <cell r="Q268">
-            <v>4940.7839119875825</v>
-          </cell>
-          <cell r="X268">
-            <v>6606.038175188095</v>
-          </cell>
-        </row>
-        <row r="269">
-          <cell r="B269" t="str">
-            <v>ARG-FUE</v>
-          </cell>
-          <cell r="Q269">
-            <v>4210.5090764948363</v>
-          </cell>
-          <cell r="X269">
-            <v>6878.0984246616972</v>
-          </cell>
-        </row>
-        <row r="270">
-          <cell r="B270" t="str">
-            <v>ARG-JUJ</v>
-          </cell>
-          <cell r="Q270">
-            <v>5421.6591629855902</v>
-          </cell>
-          <cell r="X270">
-            <v>6426.8904976374597</v>
-          </cell>
-        </row>
-        <row r="271">
-          <cell r="B271" t="str">
-            <v>ARG-LAR</v>
-          </cell>
-          <cell r="Q271">
-            <v>4997.2323565432998</v>
-          </cell>
-          <cell r="X271">
-            <v>6585.0085885697063</v>
-          </cell>
-        </row>
-        <row r="272">
-          <cell r="B272" t="str">
-            <v>ARG-MEN</v>
-          </cell>
-          <cell r="Q272">
-            <v>4559.3857641699005</v>
-          </cell>
-          <cell r="X272">
-            <v>6748.1261538516828</v>
-          </cell>
-        </row>
-        <row r="273">
-          <cell r="B273" t="str">
-            <v>ARG-MIS</v>
-          </cell>
-          <cell r="Q273">
-            <v>3039.5525975482356</v>
-          </cell>
-          <cell r="X273">
-            <v>7400.4329586376434</v>
-          </cell>
-        </row>
-        <row r="274">
-          <cell r="B274" t="str">
-            <v>ARG-NEG</v>
-          </cell>
-          <cell r="Q274">
-            <v>6067.6295194113209</v>
-          </cell>
-          <cell r="X274">
-            <v>6186.2374615744629</v>
-          </cell>
-        </row>
-        <row r="275">
-          <cell r="B275" t="str">
-            <v>ARG-NEU</v>
-          </cell>
-          <cell r="Q275">
-            <v>5188.3207839838806</v>
-          </cell>
-          <cell r="X275">
-            <v>6513.8195475206276</v>
-          </cell>
-        </row>
-        <row r="276">
-          <cell r="B276" t="str">
-            <v>ARG-PAM</v>
-          </cell>
-          <cell r="Q276">
-            <v>5176.6277743733881</v>
-          </cell>
-          <cell r="X276">
-            <v>6518.1757199602562</v>
-          </cell>
-        </row>
-        <row r="277">
-          <cell r="B277" t="str">
-            <v>ARG-RIO</v>
-          </cell>
-          <cell r="Q277">
-            <v>4195.903946113056</v>
-          </cell>
-          <cell r="X277">
-            <v>6883.5394931774708</v>
-          </cell>
-        </row>
-        <row r="278">
-          <cell r="B278" t="str">
-            <v>ARG-SAF</v>
-          </cell>
-          <cell r="Q278">
-            <v>4322.4378447101881</v>
-          </cell>
-          <cell r="X278">
-            <v>6836.3999200385779</v>
-          </cell>
-        </row>
-        <row r="279">
-          <cell r="B279" t="str">
-            <v>ARG-SAJ</v>
-          </cell>
-          <cell r="Q279">
-            <v>4046.4046324904407</v>
-          </cell>
-          <cell r="X279">
-            <v>6939.2347171993379</v>
-          </cell>
-        </row>
-        <row r="280">
-          <cell r="B280" t="str">
-            <v>ARG-SAL</v>
-          </cell>
-          <cell r="Q280">
-            <v>5073.1083019062844</v>
-          </cell>
-          <cell r="X280">
-            <v>6556.7413833735009</v>
-          </cell>
-        </row>
-        <row r="281">
-          <cell r="B281" t="str">
-            <v>ARG-SAT</v>
-          </cell>
-          <cell r="Q281">
-            <v>4696.714478504442</v>
-          </cell>
-          <cell r="X281">
-            <v>6696.9650259229984</v>
-          </cell>
-        </row>
-        <row r="282">
-          <cell r="B282" t="str">
-            <v>ARG-TUC</v>
-          </cell>
-          <cell r="Q282">
-            <v>3387.0596672414049</v>
-          </cell>
-          <cell r="X282">
-            <v>7234.1776831271982</v>
-          </cell>
-        </row>
-        <row r="283">
-          <cell r="B283" t="str">
-            <v>AUS</v>
-          </cell>
-          <cell r="Q283">
-            <v>5418.3249999999998</v>
-          </cell>
-          <cell r="X283">
-            <v>6490.875</v>
-          </cell>
-        </row>
-        <row r="284">
-          <cell r="B284" t="str">
-            <v>BRA</v>
-          </cell>
-          <cell r="Q284">
-            <v>5857.2249999999995</v>
-          </cell>
-          <cell r="X284">
-            <v>6261.45</v>
-          </cell>
-        </row>
-        <row r="285">
-          <cell r="B285" t="str">
-            <v>CHL</v>
-          </cell>
-          <cell r="Q285">
-            <v>3331.1749999999997</v>
-          </cell>
-          <cell r="X285">
-            <v>7342.0749999999998</v>
-          </cell>
-        </row>
-        <row r="286">
-          <cell r="B286" t="str">
-            <v>CHN</v>
-          </cell>
-          <cell r="Q286">
-            <v>5229.1174979378948</v>
-          </cell>
-          <cell r="X286">
-            <v>6498.6209351125426</v>
-          </cell>
-        </row>
-        <row r="287">
-          <cell r="B287" t="str">
-            <v>COL</v>
-          </cell>
-          <cell r="Q287">
-            <v>5618.4202621198119</v>
-          </cell>
-          <cell r="X287">
-            <v>6353.5881310277209</v>
-          </cell>
-        </row>
-        <row r="288">
-          <cell r="B288" t="str">
-            <v>CRI</v>
-          </cell>
-          <cell r="Q288">
-            <v>3250.4390566726183</v>
-          </cell>
-          <cell r="X288">
-            <v>7299.5400864606718</v>
-          </cell>
-        </row>
-        <row r="289">
-          <cell r="B289" t="str">
-            <v>DNK</v>
-          </cell>
-          <cell r="Q289">
-            <v>5245.367546572651</v>
-          </cell>
-          <cell r="X289">
-            <v>6492.5670605016949</v>
-          </cell>
-        </row>
-        <row r="290">
-          <cell r="B290" t="str">
-            <v>DZA</v>
-          </cell>
-          <cell r="Q290">
-            <v>2807.25</v>
-          </cell>
-          <cell r="X290">
-            <v>7494.55</v>
-          </cell>
-        </row>
-        <row r="291">
-          <cell r="B291" t="str">
-            <v>EGY</v>
-          </cell>
-          <cell r="Q291">
-            <v>3931.5749999999998</v>
-          </cell>
-          <cell r="X291">
-            <v>7378.65</v>
-          </cell>
-        </row>
-        <row r="292">
-          <cell r="B292" t="str">
-            <v>ESP</v>
-          </cell>
-          <cell r="Q292">
-            <v>5820.5891472656131</v>
-          </cell>
-          <cell r="X292">
-            <v>6278.2711206976928</v>
-          </cell>
-        </row>
-        <row r="293">
-          <cell r="B293" t="str">
-            <v>IDN</v>
-          </cell>
-          <cell r="Q293">
-            <v>2371.4702152796694</v>
-          </cell>
-          <cell r="X293">
-            <v>7720.058745318197</v>
-          </cell>
-        </row>
-        <row r="294">
-          <cell r="B294" t="str">
-            <v>IND</v>
-          </cell>
-          <cell r="Q294">
-            <v>5350.4</v>
-          </cell>
-          <cell r="X294">
-            <v>6241.5</v>
-          </cell>
-        </row>
-        <row r="295">
-          <cell r="B295" t="str">
-            <v>JOR</v>
-          </cell>
-          <cell r="Q295">
-            <v>2863.2999999999997</v>
-          </cell>
-          <cell r="X295">
-            <v>7697.85</v>
-          </cell>
-        </row>
-        <row r="296">
-          <cell r="B296" t="str">
-            <v>KAZ</v>
-          </cell>
-          <cell r="Q296">
-            <v>5358.7477420968016</v>
-          </cell>
-          <cell r="X296">
-            <v>6450.3278338701857</v>
-          </cell>
-        </row>
-        <row r="297">
-          <cell r="B297" t="str">
-            <v>KEN</v>
-          </cell>
-          <cell r="Q297">
-            <v>4452.6499999999996</v>
-          </cell>
-          <cell r="X297">
-            <v>4526.75</v>
-          </cell>
-        </row>
-        <row r="298">
-          <cell r="B298" t="str">
-            <v>MAR</v>
-          </cell>
-          <cell r="Q298">
-            <v>4500.1499999999996</v>
-          </cell>
-          <cell r="X298">
-            <v>6762.0999999999995</v>
-          </cell>
-        </row>
-        <row r="299">
-          <cell r="B299" t="str">
-            <v>MAR-BEN</v>
-          </cell>
-          <cell r="Q299">
-            <v>3185.0625782775878</v>
-          </cell>
-          <cell r="X299">
-            <v>7330.8176787038046</v>
-          </cell>
-        </row>
-        <row r="300">
-          <cell r="B300" t="str">
-            <v>MAR-CAS</v>
-          </cell>
-          <cell r="Q300">
-            <v>3916.1073137762983</v>
-          </cell>
-          <cell r="X300">
-            <v>6987.7763337418173</v>
-          </cell>
-        </row>
-        <row r="301">
-          <cell r="B301" t="str">
-            <v>MAR-DAK</v>
-          </cell>
-          <cell r="Q301">
-            <v>6642.4372020361143</v>
-          </cell>
-          <cell r="X301">
-            <v>6025.0655992359871</v>
-          </cell>
-        </row>
-        <row r="302">
-          <cell r="B302" t="str">
-            <v>MAR-DRA</v>
-          </cell>
-          <cell r="Q302">
-            <v>4324.9126494107632</v>
-          </cell>
-          <cell r="X302">
-            <v>6835.4779438845144</v>
-          </cell>
-        </row>
-        <row r="303">
-          <cell r="B303" t="str">
-            <v>MAR-FES</v>
-          </cell>
-          <cell r="Q303">
-            <v>3508.8408490347183</v>
-          </cell>
-          <cell r="X303">
-            <v>7175.9147995866961</v>
-          </cell>
-        </row>
-        <row r="304">
-          <cell r="B304" t="str">
-            <v>MAR-GUE</v>
-          </cell>
-          <cell r="Q304">
-            <v>5023.520232710207</v>
-          </cell>
-          <cell r="X304">
-            <v>6575.2151713512776</v>
-          </cell>
-        </row>
-        <row r="305">
-          <cell r="B305" t="str">
-            <v>MAR-LAA</v>
-          </cell>
-          <cell r="Q305">
-            <v>6009.3271997728652</v>
-          </cell>
-          <cell r="X305">
-            <v>6207.9577001131847</v>
-          </cell>
-        </row>
-        <row r="306">
-          <cell r="B306" t="str">
-            <v>MAR-LOR</v>
-          </cell>
-          <cell r="Q306">
-            <v>4767.8737749117199</v>
-          </cell>
-          <cell r="X306">
-            <v>6670.4549847822991</v>
-          </cell>
-        </row>
-        <row r="307">
-          <cell r="B307" t="str">
-            <v>MAR-MAR</v>
-          </cell>
-          <cell r="Q307">
-            <v>3395.7118969829239</v>
-          </cell>
-          <cell r="X307">
-            <v>7230.0382598897795</v>
-          </cell>
-        </row>
-        <row r="308">
-          <cell r="B308" t="str">
-            <v>MAR-RAB</v>
-          </cell>
-          <cell r="Q308">
-            <v>3274.9918607071504</v>
-          </cell>
-          <cell r="X308">
-            <v>7287.793467311546</v>
-          </cell>
-        </row>
-        <row r="309">
-          <cell r="B309" t="str">
-            <v>MAR-SOU</v>
-          </cell>
-          <cell r="Q309">
-            <v>4369.7035281559165</v>
-          </cell>
-          <cell r="X309">
-            <v>6818.7913252947801</v>
-          </cell>
-        </row>
-        <row r="310">
-          <cell r="B310" t="str">
-            <v>MAR-TAN</v>
-          </cell>
-          <cell r="Q310">
-            <v>4399.0894115770197</v>
-          </cell>
-          <cell r="X310">
-            <v>6807.8437609176608</v>
-          </cell>
-        </row>
-        <row r="311">
-          <cell r="B311" t="str">
-            <v>MEX</v>
-          </cell>
-          <cell r="Q311">
-            <v>3896.9</v>
-          </cell>
-          <cell r="X311">
-            <v>6779.2</v>
-          </cell>
-        </row>
-        <row r="312">
-          <cell r="B312" t="str">
-            <v>MRT</v>
-          </cell>
-          <cell r="Q312">
-            <v>6696.5499999999993</v>
-          </cell>
-          <cell r="X312">
-            <v>6807.7</v>
-          </cell>
-        </row>
-        <row r="313">
-          <cell r="B313" t="str">
-            <v>NAM</v>
-          </cell>
-          <cell r="Q313">
-            <v>7160.0484857561869</v>
-          </cell>
-          <cell r="X313">
-            <v>6428.126527693531</v>
-          </cell>
-        </row>
-        <row r="314">
-          <cell r="B314" t="str">
-            <v>NOR</v>
-          </cell>
-          <cell r="Q314">
-            <v>4951.2964731880929</v>
-          </cell>
-          <cell r="X314">
-            <v>6602.1217729189584</v>
-          </cell>
-        </row>
-        <row r="315">
-          <cell r="B315" t="str">
-            <v>PER</v>
-          </cell>
-          <cell r="Q315">
-            <v>2852.85</v>
-          </cell>
-          <cell r="X315">
-            <v>7790.95</v>
-          </cell>
-        </row>
-        <row r="316">
-          <cell r="B316" t="str">
-            <v>PRT</v>
-          </cell>
-          <cell r="Q316">
-            <v>5831.8845796358564</v>
-          </cell>
-          <cell r="X316">
-            <v>6274.0630636769592</v>
-          </cell>
-        </row>
-        <row r="317">
-          <cell r="B317" t="str">
-            <v>RUS</v>
-          </cell>
-          <cell r="Q317">
-            <v>3261.35</v>
-          </cell>
-          <cell r="X317">
-            <v>6156.95</v>
-          </cell>
-        </row>
-        <row r="318">
-          <cell r="B318" t="str">
-            <v>SAU</v>
-          </cell>
-          <cell r="Q318">
-            <v>3220.9749999999999</v>
-          </cell>
-          <cell r="X318">
-            <v>7620.4250000000002</v>
-          </cell>
-        </row>
-        <row r="319">
-          <cell r="B319" t="str">
-            <v>SWE</v>
-          </cell>
-          <cell r="Q319">
-            <v>3632.7836923185168</v>
-          </cell>
-          <cell r="X319">
-            <v>7116.6177280885831</v>
-          </cell>
-        </row>
-        <row r="320">
-          <cell r="B320" t="str">
-            <v>THA</v>
-          </cell>
-          <cell r="Q320">
-            <v>3391.0600884010501</v>
-          </cell>
-          <cell r="X320">
-            <v>7232.2637907777807</v>
-          </cell>
-        </row>
-        <row r="321">
-          <cell r="B321" t="str">
-            <v>TUN</v>
-          </cell>
-          <cell r="Q321">
-            <v>3097</v>
-          </cell>
-          <cell r="X321">
-            <v>7260.85</v>
-          </cell>
-        </row>
-        <row r="322">
-          <cell r="B322" t="str">
-            <v>UKR</v>
-          </cell>
-          <cell r="Q322">
-            <v>5028.3766144519759</v>
-          </cell>
-          <cell r="X322">
-            <v>6573.405950542905</v>
-          </cell>
-        </row>
-        <row r="323">
-          <cell r="B323" t="str">
-            <v>URY</v>
-          </cell>
-          <cell r="Q323">
-            <v>5653.9250000000002</v>
-          </cell>
-          <cell r="X323">
-            <v>6463.3249999999998</v>
-          </cell>
-        </row>
-        <row r="324">
-          <cell r="B324" t="str">
-            <v>USA</v>
-          </cell>
-          <cell r="Q324">
-            <v>5744.1750000000002</v>
-          </cell>
-          <cell r="X324">
-            <v>6282.3499999999995</v>
-          </cell>
-        </row>
-        <row r="325">
-          <cell r="B325" t="str">
-            <v>VNM</v>
-          </cell>
-          <cell r="Q325">
-            <v>4638.4593410818907</v>
-          </cell>
-          <cell r="X325">
-            <v>6718.6676869623916</v>
-          </cell>
-        </row>
-        <row r="326">
-          <cell r="B326" t="str">
-            <v>ZAF</v>
-          </cell>
-          <cell r="Q326">
-            <v>3452.2999999999997</v>
-          </cell>
-          <cell r="X326">
-            <v>6924.0749999999998</v>
-          </cell>
-        </row>
-        <row r="327">
-          <cell r="B327" t="str">
-            <v>ZAF-EC</v>
-          </cell>
-          <cell r="Q327">
-            <v>5357.2785258864797</v>
-          </cell>
-          <cell r="X327">
-            <v>6450.8751830451602</v>
-          </cell>
-        </row>
-        <row r="328">
-          <cell r="B328" t="str">
-            <v>ZAF-FRS</v>
-          </cell>
-          <cell r="Q328">
-            <v>4304.2466634919829</v>
-          </cell>
-          <cell r="X328">
-            <v>6843.1769539166589</v>
-          </cell>
-        </row>
-        <row r="329">
-          <cell r="B329" t="str">
-            <v>ZAF-GAU</v>
-          </cell>
-          <cell r="Q329">
-            <v>3569.33905</v>
-          </cell>
-          <cell r="X329">
-            <v>7146.9710860724654</v>
-          </cell>
-        </row>
-        <row r="330">
-          <cell r="B330" t="str">
-            <v>ZAF-KWA</v>
-          </cell>
-          <cell r="Q330">
-            <v>4112.4581361528417</v>
-          </cell>
-          <cell r="X330">
-            <v>6914.626813692882</v>
-          </cell>
-        </row>
-        <row r="331">
-          <cell r="B331" t="str">
-            <v>ZAF-LIM</v>
-          </cell>
-          <cell r="Q331">
-            <v>4069.701505998692</v>
-          </cell>
-          <cell r="X331">
-            <v>6930.5555831109605</v>
-          </cell>
-        </row>
-        <row r="332">
-          <cell r="B332" t="str">
-            <v>ZAF-MPU</v>
-          </cell>
-          <cell r="Q332">
-            <v>4069.701505998692</v>
-          </cell>
-          <cell r="X332">
-            <v>6930.5555831109605</v>
-          </cell>
-        </row>
-        <row r="333">
-          <cell r="B333" t="str">
-            <v>ZAF-NC</v>
-          </cell>
-          <cell r="Q333">
-            <v>5310.6168836425632</v>
-          </cell>
-          <cell r="X333">
-            <v>6468.2587452504249</v>
-          </cell>
-        </row>
-        <row r="334">
-          <cell r="B334" t="str">
-            <v>ZAF-NW</v>
-          </cell>
-          <cell r="Q334">
-            <v>4347.7064455119726</v>
-          </cell>
-          <cell r="X334">
-            <v>6826.9862287762417</v>
-          </cell>
-        </row>
-        <row r="335">
-          <cell r="B335" t="str">
-            <v>ZAF-WC</v>
-          </cell>
-          <cell r="Q335">
-            <v>4701.7138736611696</v>
-          </cell>
-          <cell r="X335">
-            <v>6695.1025261798168</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12">
-        <row r="2">
-          <cell r="G2">
-            <v>87.367502532414022</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="G3">
-            <v>232.52591244984052</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
-      <sheetData sheetId="23"/>
-      <sheetData sheetId="24"/>
-      <sheetData sheetId="25"/>
-      <sheetData sheetId="26"/>
-      <sheetData sheetId="27"/>
-      <sheetData sheetId="28"/>
-      <sheetData sheetId="29"/>
-      <sheetData sheetId="30"/>
-      <sheetData sheetId="31"/>
-      <sheetData sheetId="32"/>
-      <sheetData sheetId="33"/>
-      <sheetData sheetId="34"/>
-      <sheetData sheetId="35"/>
-      <sheetData sheetId="36"/>
-      <sheetData sheetId="37"/>
-      <sheetData sheetId="38"/>
-      <sheetData sheetId="39"/>
-      <sheetData sheetId="40"/>
-      <sheetData sheetId="41"/>
-      <sheetData sheetId="42"/>
-      <sheetData sheetId="43"/>
-      <sheetData sheetId="44"/>
-      <sheetData sheetId="45"/>
-      <sheetData sheetId="46"/>
-      <sheetData sheetId="47"/>
-      <sheetData sheetId="48"/>
-      <sheetData sheetId="49"/>
-      <sheetData sheetId="50" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sheet1"/>
-      <sheetName val="context_cs_type"/>
-      <sheetName val="context_cs_scope"/>
-      <sheetName val="context_cs_countries"/>
-      <sheetName val="_context_data_infobox"/>
-      <sheetName val="certification_schemes"/>
-      <sheetName val="demand_countries"/>
-      <sheetName val="literature"/>
-      <sheetName val="sustainability"/>
-      <sheetName val="context_data"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <person displayName="Markus Haller" id="{DD827897-2D45-4275-8857-9F8104ECFC4F}" userId="S::m.haller@oeko.de::d316836f-ce4c-41ea-b145-e0651e70b405" providerId="AD"/>
+  <person displayName="Susanne Krieger" id="{E166FC0D-584A-4ACA-8C42-8483F27018E4}" userId="S::s.krieger@oeko.de::b8ba3234-4142-4144-a218-6f55425c3a71" providerId="AD"/>
 </personList>
 </file>
 
@@ -5224,6 +3637,26 @@
 
 <file path=xl/threadedComments/threadedComment3.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="B2" dT="2023-01-16T16:39:34.50" personId="{E166FC0D-584A-4ACA-8C42-8483F27018E4}" id="{7C326BBD-CADA-414E-8630-DB89B2783121}">
+    <text>Diese Zeile mit Infos zur Verlinkung in Bubble/Point Chart nutzen</text>
+  </threadedComment>
+  <threadedComment ref="B7" dT="2023-01-17T08:12:13.78" personId="{E166FC0D-584A-4ACA-8C42-8483F27018E4}" id="{9396247F-F92D-4843-8B4A-446356C13809}">
+    <text>only referring to renewable H2</text>
+  </threadedComment>
+  <threadedComment ref="B7" dT="2023-01-30T13:17:37.70" personId="{E166FC0D-584A-4ACA-8C42-8483F27018E4}" id="{6F7FBF85-2A53-41A4-8EC9-6107E14456F7}" parentId="{9396247F-F92D-4843-8B4A-446356C13809}">
+    <text>new targets as stated in the RePowerPlan EU</text>
+  </threadedComment>
+  <threadedComment ref="E7" dT="2023-01-19T14:28:45.63" personId="{E166FC0D-584A-4ACA-8C42-8483F27018E4}" id="{28CB0F6E-75D7-4DD3-8285-1765A8E1BC92}">
+    <text>53.000 km by 2040</text>
+  </threadedComment>
+  <threadedComment ref="E10" dT="2023-01-23T13:41:53.26" personId="{E166FC0D-584A-4ACA-8C42-8483F27018E4}" id="{BCC66E9D-D639-4CC4-926D-7484C4028444}">
+    <text>non-renewable</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment4.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <threadedComment ref="F2" dT="2023-09-26T15:08:10.64" personId="{DD827897-2D45-4275-8857-9F8104ECFC4F}" id="{41EB567B-49B3-4249-A497-693C9780E7FB}">
     <text>Ich würde vorschlagen, wie hier auch bei allen anderen 
 Spalten die zugehörigen Links direkt in den Markup-Text reinzuschreiben.</text>
@@ -5919,290 +4352,290 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="J4">
-    <cfRule type="cellIs" dxfId="90" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="71" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="89" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="72" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O4">
-    <cfRule type="cellIs" dxfId="88" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="69" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="87" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="70" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5">
-    <cfRule type="cellIs" dxfId="86" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="67" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="85" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="68" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L5">
-    <cfRule type="cellIs" dxfId="84" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="65" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="83" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="66" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M5">
-    <cfRule type="cellIs" dxfId="82" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="63" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="64" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6">
-    <cfRule type="cellIs" dxfId="80" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="61" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="79" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="62" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6">
-    <cfRule type="cellIs" dxfId="78" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="59" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="77" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="60" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L6">
-    <cfRule type="cellIs" dxfId="76" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="57" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="58" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M6">
-    <cfRule type="cellIs" dxfId="74" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="55" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="56" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N6">
-    <cfRule type="cellIs" dxfId="72" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="53" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="71" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="54" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7">
-    <cfRule type="cellIs" dxfId="70" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="51" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="52" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K7">
-    <cfRule type="cellIs" dxfId="68" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="49" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="50" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K8">
-    <cfRule type="cellIs" dxfId="66" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="47" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="48" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K9">
-    <cfRule type="cellIs" dxfId="64" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="45" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="46" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L9">
-    <cfRule type="cellIs" dxfId="62" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="43" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="44" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O9">
-    <cfRule type="cellIs" dxfId="60" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="41" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="42" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K10">
-    <cfRule type="cellIs" dxfId="58" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="39" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="40" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L10">
-    <cfRule type="cellIs" dxfId="56" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="37" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="38" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11">
-    <cfRule type="cellIs" dxfId="54" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="35" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="36" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11">
-    <cfRule type="cellIs" dxfId="52" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="33" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="34" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O11">
-    <cfRule type="cellIs" dxfId="50" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="31" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="32" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12">
-    <cfRule type="cellIs" dxfId="48" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="29" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="30" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N12">
-    <cfRule type="cellIs" dxfId="46" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="27" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="28" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O12">
-    <cfRule type="cellIs" dxfId="44" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="25" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="26" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J13">
-    <cfRule type="cellIs" dxfId="42" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="23" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="24" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13">
-    <cfRule type="cellIs" dxfId="40" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="21" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="22" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L13">
-    <cfRule type="cellIs" dxfId="38" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="19" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="20" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M13">
-    <cfRule type="cellIs" dxfId="36" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="17" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="18" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N13">
-    <cfRule type="cellIs" dxfId="34" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="15" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="16" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O13">
-    <cfRule type="cellIs" dxfId="32" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="13" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="14" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J14">
-    <cfRule type="cellIs" dxfId="30" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="11" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="12" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J15">
-    <cfRule type="cellIs" dxfId="28" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="9" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="10" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15">
-    <cfRule type="cellIs" dxfId="26" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="7" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="8" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J16">
-    <cfRule type="cellIs" dxfId="24" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="5" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="6" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K16">
-    <cfRule type="cellIs" dxfId="22" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="3" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="4" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O16">
-    <cfRule type="cellIs" dxfId="20" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="1" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="2" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7301,11 +5734,346 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34582045-E811-49CA-82B8-AB81ED823DC3}">
+  <dimension ref="A1:R12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="37" customWidth="1"/>
+    <col min="2" max="6" width="30" style="37" customWidth="1"/>
+    <col min="7" max="7" width="4.42578125" style="37" customWidth="1"/>
+    <col min="8" max="8" width="30" style="37" customWidth="1"/>
+    <col min="9" max="9" width="52.5703125" style="37" customWidth="1"/>
+    <col min="10" max="10" width="5.140625" style="37" customWidth="1"/>
+    <col min="11" max="11" width="30" style="37" customWidth="1"/>
+    <col min="12" max="12" width="52.5703125" style="37" customWidth="1"/>
+    <col min="13" max="13" width="5.140625" style="37" customWidth="1"/>
+    <col min="14" max="14" width="30" style="37" customWidth="1"/>
+    <col min="15" max="15" width="52.5703125" style="37" customWidth="1"/>
+    <col min="16" max="16" width="5.140625" style="37" customWidth="1"/>
+    <col min="17" max="17" width="30" style="37" customWidth="1"/>
+    <col min="18" max="18" width="52.5703125" style="37" customWidth="1"/>
+    <col min="19" max="19" width="5.140625" style="37" customWidth="1"/>
+    <col min="20" max="16384" width="8.85546875" style="37"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="36" t="s">
+        <v>605</v>
+      </c>
+      <c r="H1" s="36" t="s">
+        <v>606</v>
+      </c>
+      <c r="K1" s="36" t="s">
+        <v>607</v>
+      </c>
+      <c r="N1" s="36" t="s">
+        <v>608</v>
+      </c>
+      <c r="Q1" s="36" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="38" t="s">
+        <v>469</v>
+      </c>
+      <c r="B2" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="38" t="s">
+        <v>610</v>
+      </c>
+      <c r="D2" s="38" t="s">
+        <v>611</v>
+      </c>
+      <c r="E2" s="38" t="s">
+        <v>612</v>
+      </c>
+      <c r="F2" s="38" t="s">
+        <v>613</v>
+      </c>
+      <c r="H2" s="37" t="s">
+        <v>614</v>
+      </c>
+      <c r="I2" s="37" t="s">
+        <v>615</v>
+      </c>
+      <c r="K2" s="37" t="s">
+        <v>614</v>
+      </c>
+      <c r="L2" s="37" t="s">
+        <v>615</v>
+      </c>
+      <c r="N2" s="37" t="s">
+        <v>614</v>
+      </c>
+      <c r="O2" s="37" t="s">
+        <v>615</v>
+      </c>
+      <c r="Q2" s="37" t="s">
+        <v>614</v>
+      </c>
+      <c r="R2" s="37" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>616</v>
+      </c>
+      <c r="D3" s="39" t="s">
+        <v>617</v>
+      </c>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="H3" s="40" t="s">
+        <v>618</v>
+      </c>
+      <c r="I3" s="41" t="s">
+        <v>619</v>
+      </c>
+      <c r="K3" s="40" t="s">
+        <v>620</v>
+      </c>
+      <c r="L3" s="41" t="s">
+        <v>621</v>
+      </c>
+      <c r="N3" s="40" t="s">
+        <v>622</v>
+      </c>
+      <c r="O3" s="41" t="s">
+        <v>623</v>
+      </c>
+      <c r="Q3" s="40" t="s">
+        <v>624</v>
+      </c>
+      <c r="R3" s="41" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="39" t="s">
+        <v>626</v>
+      </c>
+      <c r="D4" s="39" t="s">
+        <v>627</v>
+      </c>
+      <c r="E4" s="39" t="s">
+        <v>628</v>
+      </c>
+      <c r="F4" s="39"/>
+      <c r="H4" s="40" t="s">
+        <v>629</v>
+      </c>
+      <c r="I4" s="41" t="s">
+        <v>619</v>
+      </c>
+      <c r="K4" s="40" t="s">
+        <v>630</v>
+      </c>
+      <c r="L4" s="41" t="s">
+        <v>631</v>
+      </c>
+      <c r="N4" s="40" t="s">
+        <v>630</v>
+      </c>
+      <c r="O4" s="41" t="s">
+        <v>632</v>
+      </c>
+      <c r="Q4" s="40" t="s">
+        <v>633</v>
+      </c>
+      <c r="R4" s="41"/>
+    </row>
+    <row r="5" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="39" t="s">
+        <v>634</v>
+      </c>
+      <c r="D5" s="39" t="s">
+        <v>635</v>
+      </c>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="H5" s="40" t="s">
+        <v>636</v>
+      </c>
+      <c r="I5" s="41" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="39" t="s">
+        <v>637</v>
+      </c>
+      <c r="C6" s="39" t="s">
+        <v>638</v>
+      </c>
+      <c r="D6" s="39" t="s">
+        <v>639</v>
+      </c>
+      <c r="E6" s="42" t="s">
+        <v>640</v>
+      </c>
+      <c r="F6" s="39"/>
+      <c r="H6" s="40" t="s">
+        <v>641</v>
+      </c>
+      <c r="I6" s="41" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="39" t="s">
+        <v>642</v>
+      </c>
+      <c r="B7" s="39" t="s">
+        <v>643</v>
+      </c>
+      <c r="C7" s="39" t="s">
+        <v>644</v>
+      </c>
+      <c r="D7" s="39" t="s">
+        <v>645</v>
+      </c>
+      <c r="E7" s="39" t="s">
+        <v>646</v>
+      </c>
+      <c r="F7" s="39"/>
+      <c r="H7" s="43" t="s">
+        <v>647</v>
+      </c>
+      <c r="I7" s="41" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="39" t="s">
+        <v>344</v>
+      </c>
+      <c r="C8" s="39" t="s">
+        <v>638</v>
+      </c>
+      <c r="D8" s="39" t="s">
+        <v>648</v>
+      </c>
+      <c r="E8" s="39" t="s">
+        <v>649</v>
+      </c>
+      <c r="F8" s="39"/>
+    </row>
+    <row r="9" spans="1:18" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="39" t="s">
+        <v>353</v>
+      </c>
+      <c r="C9" s="39" t="s">
+        <v>650</v>
+      </c>
+      <c r="D9" s="39" t="s">
+        <v>651</v>
+      </c>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
+    </row>
+    <row r="10" spans="1:18" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="39" t="s">
+        <v>331</v>
+      </c>
+      <c r="C10" s="39" t="s">
+        <v>626</v>
+      </c>
+      <c r="D10" s="39" t="s">
+        <v>652</v>
+      </c>
+      <c r="E10" s="39" t="s">
+        <v>653</v>
+      </c>
+      <c r="F10" s="39"/>
+    </row>
+    <row r="11" spans="1:18" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="39" t="s">
+        <v>338</v>
+      </c>
+      <c r="C11" s="39" t="s">
+        <v>626</v>
+      </c>
+      <c r="D11" s="39" t="s">
+        <v>654</v>
+      </c>
+      <c r="E11" s="39" t="s">
+        <v>655</v>
+      </c>
+      <c r="F11" s="39"/>
+    </row>
+    <row r="12" spans="1:18" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="39" t="s">
+        <v>360</v>
+      </c>
+      <c r="C12" s="39" t="s">
+        <v>626</v>
+      </c>
+      <c r="D12" s="39" t="s">
+        <v>656</v>
+      </c>
+      <c r="E12" s="39" t="s">
+        <v>657</v>
+      </c>
+      <c r="F12" s="39" t="s">
+        <v>658</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66EF205A-9961-4EC2-AED6-DBC55BECEA90}">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:N43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
@@ -9002,16 +7770,16 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G36">
-    <cfRule type="cellIs" dxfId="18" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="1" operator="equal">
       <formula>"very high"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="2" operator="equal">
       <formula>"high"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="3" operator="equal">
       <formula>"medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="4" operator="equal">
       <formula>"low"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9056,7 +7824,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A08C373-50CB-424A-939A-38A53453958B}">
   <dimension ref="A1:R11"/>
   <sheetViews>
@@ -9637,7 +8405,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F35DBB3-2A80-4CA5-AC9F-BFE408866ADC}">
   <dimension ref="A1:H58"/>
   <sheetViews>
@@ -10251,7 +9019,7 @@
     <mergeCell ref="H53:H54"/>
   </mergeCells>
   <conditionalFormatting sqref="A2:A15 A17:A23 A40:A46">
-    <cfRule type="expression" dxfId="14" priority="31">
+    <cfRule type="expression" dxfId="23" priority="31">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
     <cfRule type="expression" priority="32">
@@ -10259,7 +9027,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21:B23 B2:B15 B17:B19">
-    <cfRule type="expression" dxfId="13" priority="29">
+    <cfRule type="expression" dxfId="22" priority="29">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
     <cfRule type="expression" priority="30">
@@ -10267,7 +9035,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20">
-    <cfRule type="expression" dxfId="12" priority="27">
+    <cfRule type="expression" dxfId="21" priority="27">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
     <cfRule type="expression" priority="28">
@@ -10275,7 +9043,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17:C23 C2:C15">
-    <cfRule type="expression" dxfId="11" priority="25">
+    <cfRule type="expression" dxfId="20" priority="25">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
     <cfRule type="expression" priority="26">
@@ -10283,7 +9051,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3">
-    <cfRule type="expression" dxfId="10" priority="23">
+    <cfRule type="expression" dxfId="19" priority="23">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
     <cfRule type="expression" priority="24">
@@ -10291,7 +9059,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13:C15">
-    <cfRule type="expression" dxfId="9" priority="21">
+    <cfRule type="expression" dxfId="18" priority="21">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
     <cfRule type="expression" priority="22">
@@ -10299,7 +9067,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12">
-    <cfRule type="expression" dxfId="8" priority="19">
+    <cfRule type="expression" dxfId="17" priority="19">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
     <cfRule type="expression" priority="20">
@@ -10307,7 +9075,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24">
-    <cfRule type="expression" dxfId="7" priority="17">
+    <cfRule type="expression" dxfId="16" priority="17">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
     <cfRule type="expression" priority="18">
@@ -10315,7 +9083,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16">
-    <cfRule type="expression" dxfId="6" priority="15">
+    <cfRule type="expression" dxfId="15" priority="15">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
     <cfRule type="expression" priority="16">
@@ -10323,7 +9091,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="expression" dxfId="5" priority="13">
+    <cfRule type="expression" dxfId="14" priority="13">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
     <cfRule type="expression" priority="14">
@@ -10331,7 +9099,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6">
-    <cfRule type="expression" dxfId="4" priority="11">
+    <cfRule type="expression" dxfId="13" priority="11">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
     <cfRule type="expression" priority="12">
@@ -10339,7 +9107,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7">
-    <cfRule type="expression" dxfId="3" priority="9">
+    <cfRule type="expression" dxfId="12" priority="9">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
     <cfRule type="expression" priority="10">
@@ -10347,7 +9115,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25:A26 D25:D26 A28:A34 A36:A38">
-    <cfRule type="expression" dxfId="2" priority="7">
+    <cfRule type="expression" dxfId="11" priority="7">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
     <cfRule type="expression" priority="8">
@@ -10355,7 +9123,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25:B26 E25:E26">
-    <cfRule type="expression" dxfId="1" priority="5">
+    <cfRule type="expression" dxfId="10" priority="5">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
     <cfRule type="expression" priority="6">
@@ -10363,7 +9131,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:C26 F25:F26">
-    <cfRule type="expression" dxfId="0" priority="3">
+    <cfRule type="expression" dxfId="9" priority="3">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
     <cfRule type="expression" priority="4">
@@ -10391,15 +9159,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100E2F0DF90B070FE43BFD707F72A4CD00B" ma:contentTypeVersion="15" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="8927d14e1bc908eae180c9caa4b5da89">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1bc94727-11e8-4443-b8f0-9215ff28e4bb" xmlns:ns3="cd34aed5-94da-4c30-bba3-37b78f4daae9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bb67c9392edae2d7a3a1d88d3e91258a" ns2:_="" ns3:_="">
     <xsd:import namespace="1bc94727-11e8-4443-b8f0-9215ff28e4bb"/>
@@ -10636,15 +9395,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22BF5C6F-88A2-47DA-9B5F-9FD29A58E304}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1143ECE1-9C35-446D-8A76-82388033D272}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10661,4 +9421,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22BF5C6F-88A2-47DA-9B5F-9FD29A58E304}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fix column header type in excel file
</commit_message>
<xml_diff>
--- a/data/context_data.xlsx
+++ b/data/context_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://oekoinstev.sharepoint.com/sites/AgoraPtXTool/Freigegebene Dokumente/General/Daten/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m.haller\Documents\code\ptx-boa\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1864" documentId="13_ncr:1_{57048A87-158B-4EA5-9C6F-1E45CE5AC6D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{415F37F5-53BC-47BE-A83E-1229B867DAF5}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF164CDB-E5CE-47F1-9C1C-00B2DC943F9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1785" windowWidth="29040" windowHeight="17640" xr2:uid="{D16C601B-E1D6-40C0-8CC1-80505BE1FBB6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{D16C601B-E1D6-40C0-8CC1-80505BE1FBB6}"/>
   </bookViews>
   <sheets>
     <sheet name="certification_schemes" sheetId="6" r:id="rId1"/>
@@ -143,25 +143,25 @@
   <commentList>
     <comment ref="B1" authorId="0" shapeId="0" xr:uid="{2A667BCC-C7D3-4992-946E-E2C855F210A9}">
       <text>
-        <t>[Kommentarthread]
-Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
-Kommentar:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     Original Spaltenüberschriften zur Orientierung</t>
       </text>
     </comment>
     <comment ref="B2" authorId="1" shapeId="0" xr:uid="{A9F65885-4E49-415C-91A1-1173FAD6E194}">
       <text>
-        <t>[Kommentarthread]
-Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
-Kommentar:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     finale Spaltenüberschriften</t>
       </text>
     </comment>
     <comment ref="J3" authorId="2" shapeId="0" xr:uid="{992A6B03-D2E4-4C1E-A3AD-D20F03F53B7A}">
       <text>
-        <t>[Kommentarthread]
-Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
-Kommentar:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     Whatever benchmarks mean in this context - IRENA / RMI: no threshold; NOW: threshold 76.1 gCO2eq/MJ</t>
       </text>
     </comment>
@@ -178,17 +178,17 @@
   <commentList>
     <comment ref="D2" authorId="0" shapeId="0" xr:uid="{EE4818DC-680A-43E1-BAF8-70110032BAE7}">
       <text>
-        <t>[Kommentarthread]
-Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
-Kommentar:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     Diese Fragen kommen sowohl bei Guardrails als auch bei Goals vor, würde ich also hier zweimal eintragen</t>
       </text>
     </comment>
     <comment ref="D5" authorId="1" shapeId="0" xr:uid="{2081EC17-A2D5-4172-AC61-548734349701}">
       <text>
-        <t>[Kommentarthread]
-Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
-Kommentar:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     Diese Fragen kommen sowohl bei Guardrails als auch bei Goals vor, würde ich also hier zweimal eintragen</t>
       </text>
     </comment>
@@ -205,17 +205,17 @@
   <commentList>
     <comment ref="G1" authorId="0" shapeId="0" xr:uid="{BC4C7A2D-BA6F-4F3F-A00B-273363E7C0FF}">
       <text>
-        <t>[Kommentarthread]
-Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
-Kommentar:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     Check - Updates bei CCS Institute</t>
       </text>
     </comment>
     <comment ref="I1" authorId="1" shapeId="0" xr:uid="{1B1D3AC6-D276-4403-9A19-F31E7F4ECC15}">
       <text>
-        <t>[Kommentarthread]
-Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
-Kommentar:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     Needs to be done</t>
       </text>
     </comment>
@@ -233,28 +233,28 @@
   <commentList>
     <comment ref="F2" authorId="0" shapeId="0" xr:uid="{41EB567B-49B3-4249-A497-693C9780E7FB}">
       <text>
-        <t>[Kommentarthread]
-Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
-Kommentar:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     Ich würde vorschlagen, wie hier auch bei allen anderen 
 Spalten die zugehörigen Links direkt in den Markup-Text reinzuschreiben.</t>
       </text>
     </comment>
     <comment ref="H2" authorId="1" shapeId="0" xr:uid="{C876D122-024F-4AEB-B1DC-30DFDDAC00DC}">
       <text>
-        <t>[Kommentarthread]
-Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
-Kommentar:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     Eine Liste der Certification schemes brauchen wir hier nicht, die Info haben wir schon bei den schemes</t>
       </text>
     </comment>
     <comment ref="C4" authorId="2" shapeId="0" xr:uid="{CB3F7516-C126-4E96-8DE2-098FB533FCD9}">
       <text>
-        <t>[Kommentarthread]
-Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
-Kommentar:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     2.9 - 3.9 Mt
-Antwort:
+Reply:
     Achtung: andere Einheit</t>
       </text>
     </comment>
@@ -1440,9 +1440,6 @@
   </si>
   <si>
     <t>Fraunhofer IEE (2022): Global PtX Atlas.</t>
-  </si>
-  <si>
-    <t>source__h2_demand_2030</t>
   </si>
   <si>
     <t>source_targeted_sectors_main</t>
@@ -2432,6 +2429,9 @@
   </si>
   <si>
     <t>not yet [Link](https://www.vietnam.vn/en/viet-nam-se-day-manh-san-xuat-nang-luong-hydrogen/)</t>
+  </si>
+  <si>
+    <t>source_h2_demand_2030</t>
   </si>
 </sst>
 </file>
@@ -2679,9 +2679,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -2691,10 +2688,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="76">
     <dxf>
@@ -5127,7 +5127,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -5479,11 +5479,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE04771-D0C8-4928-A647-849B136F2B55}">
   <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="2"/>
     <col min="2" max="7" width="34" style="1" customWidth="1"/>
@@ -5551,7 +5551,7 @@
         <v>35</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>34</v>
@@ -5583,31 +5583,31 @@
         <v>16</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="H3" s="33" t="s">
+        <v>462</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="J3" s="40" t="s">
+        <v>466</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>465</v>
-      </c>
-      <c r="H3" s="33" t="s">
-        <v>463</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>460</v>
-      </c>
-      <c r="J3" s="40" t="s">
-        <v>467</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>466</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>105</v>
@@ -5617,7 +5617,7 @@
       </c>
       <c r="N3" s="1"/>
       <c r="O3" s="1" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="191.25" x14ac:dyDescent="0.25">
@@ -5625,13 +5625,13 @@
         <v>125</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="C4" s="40" t="s">
         <v>472</v>
       </c>
-      <c r="C4" s="40" t="s">
+      <c r="D4" s="1" t="s">
         <v>473</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>474</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>106</v>
@@ -5643,20 +5643,20 @@
         <v>108</v>
       </c>
       <c r="H4" s="33" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>107</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="P4" s="1"/>
     </row>
@@ -5671,38 +5671,38 @@
         <v>104</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="H5" s="33" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>109</v>
       </c>
       <c r="J5" s="41" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="O5" s="1" t="s">
         <v>549</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>545</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>546</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>550</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="331.5" x14ac:dyDescent="0.25">
@@ -5713,43 +5713,43 @@
         <v>126</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>553</v>
+      </c>
+      <c r="F6" s="36" t="s">
         <v>520</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>519</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>554</v>
-      </c>
-      <c r="F6" s="36" t="s">
+      <c r="G6" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="H6" s="33" t="s">
         <v>521</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>503</v>
-      </c>
-      <c r="H6" s="33" t="s">
-        <v>522</v>
-      </c>
       <c r="I6" s="36" t="s">
+        <v>526</v>
+      </c>
+      <c r="J6" s="36" t="s">
+        <v>525</v>
+      </c>
+      <c r="K6" s="1" t="s">
         <v>527</v>
       </c>
-      <c r="J6" s="36" t="s">
-        <v>526</v>
-      </c>
-      <c r="K6" s="1" t="s">
+      <c r="L6" s="1" t="s">
         <v>528</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="M6" s="1" t="s">
         <v>529</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="N6" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="N6" s="1" t="s">
+      <c r="O6" s="1" t="s">
         <v>531</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>532</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5757,28 +5757,28 @@
         <v>128</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>104</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>556</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>557</v>
-      </c>
       <c r="F7" s="36" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="I7" s="40" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>121</v>
@@ -5790,44 +5790,44 @@
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="P7" s="1"/>
     </row>
     <row r="8" spans="1:16" ht="280.5" x14ac:dyDescent="0.25">
       <c r="A8" s="39" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>579</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>587</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>588</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>580</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>588</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>589</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>581</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G8" s="1" t="s">
+        <v>581</v>
+      </c>
+      <c r="I8" s="1" t="s">
         <v>582</v>
       </c>
-      <c r="I8" s="1" t="s">
-        <v>583</v>
-      </c>
       <c r="J8" s="1" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5838,36 +5838,36 @@
         <v>42</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>112</v>
       </c>
       <c r="F9" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>565</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>566</v>
-      </c>
       <c r="H9" s="4" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>109</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="P9" s="1"/>
     </row>
@@ -5879,36 +5879,36 @@
         <v>14</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>493</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>494</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>499</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>495</v>
-      </c>
       <c r="H10" s="4" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>114</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="P10" s="1"/>
     </row>
@@ -5920,28 +5920,28 @@
         <v>43</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>475</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>476</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>477</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>478</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="H11" s="33" t="s">
         <v>479</v>
       </c>
-      <c r="H11" s="33" t="s">
+      <c r="I11" s="1" t="s">
         <v>480</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="J11" s="4" t="s">
         <v>481</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>482</v>
       </c>
       <c r="K11" s="4" t="s">
         <v>122</v>
@@ -5950,7 +5950,7 @@
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
       <c r="O11" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P11" s="1"/>
     </row>
@@ -5962,43 +5962,43 @@
         <v>132</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>118</v>
       </c>
       <c r="F12" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="H12" s="33" t="s">
         <v>486</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>485</v>
-      </c>
-      <c r="H12" s="33" t="s">
-        <v>487</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>114</v>
       </c>
       <c r="J12" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="K12" s="1" t="s">
         <v>488</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>489</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>119</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="N12" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="O12" s="1" t="s">
         <v>490</v>
-      </c>
-      <c r="O12" s="1" t="s">
-        <v>491</v>
       </c>
       <c r="P12" s="1"/>
     </row>
@@ -6010,32 +6010,32 @@
         <v>120</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>517</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>518</v>
-      </c>
       <c r="E13" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>509</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="H13" s="1" t="s">
         <v>510</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>511</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>107</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="382.5" x14ac:dyDescent="0.25">
@@ -6043,43 +6043,43 @@
         <v>133</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>109</v>
       </c>
       <c r="J14" s="1" t="s">
+        <v>596</v>
+      </c>
+      <c r="K14" s="1" t="s">
         <v>597</v>
       </c>
-      <c r="K14" s="1" t="s">
-        <v>598</v>
-      </c>
       <c r="L14" s="1" t="s">
+        <v>602</v>
+      </c>
+      <c r="M14" s="1" t="s">
         <v>603</v>
       </c>
-      <c r="M14" s="1" t="s">
-        <v>604</v>
-      </c>
       <c r="N14" s="1" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="265.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6087,40 +6087,40 @@
         <v>116</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D15" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>600</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>505</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>601</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>501</v>
-      </c>
-      <c r="G15" s="1" t="s">
+      <c r="H15" s="4" t="s">
+        <v>499</v>
+      </c>
+      <c r="I15" s="1" t="s">
         <v>506</v>
       </c>
-      <c r="H15" s="4" t="s">
-        <v>500</v>
-      </c>
-      <c r="I15" s="1" t="s">
+      <c r="J15" s="1" t="s">
+        <v>595</v>
+      </c>
+      <c r="K15" s="1" t="s">
         <v>507</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>596</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>508</v>
       </c>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
   </sheetData>
@@ -6394,7 +6394,7 @@
       <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.28515625" style="7" customWidth="1"/>
     <col min="2" max="2" width="13.140625" style="7" customWidth="1"/>
@@ -7160,7 +7160,7 @@
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.42578125" style="2" customWidth="1"/>
     <col min="2" max="2" width="18.7109375" style="2" customWidth="1"/>
@@ -7177,19 +7177,19 @@
     <row r="1" spans="1:14" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="44" t="s">
+      <c r="C1" s="47" t="s">
         <v>320</v>
       </c>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44" t="s">
+      <c r="D1" s="47"/>
+      <c r="E1" s="47" t="s">
         <v>242</v>
       </c>
-      <c r="F1" s="44"/>
+      <c r="F1" s="47"/>
       <c r="G1" s="1" t="s">
         <v>243</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>334</v>
@@ -7218,7 +7218,7 @@
         <v>318</v>
       </c>
       <c r="H2" s="19" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="I2" s="19" t="s">
         <v>319</v>
@@ -7265,7 +7265,7 @@
         <v>12</v>
       </c>
       <c r="I3" s="23" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="J3" s="20" t="s">
         <v>340</v>
@@ -7277,7 +7277,7 @@
         <v>346</v>
       </c>
       <c r="M3" s="20" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="N3" s="20" t="s">
         <v>50</v>
@@ -7309,7 +7309,7 @@
         <v>12</v>
       </c>
       <c r="I4" s="23" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="J4" s="20" t="s">
         <v>340</v>
@@ -7353,7 +7353,7 @@
         <v>12</v>
       </c>
       <c r="I5" s="23" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="J5" s="20" t="s">
         <v>340</v>
@@ -7397,7 +7397,7 @@
         <v>12</v>
       </c>
       <c r="I6" s="23" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="J6" s="20" t="s">
         <v>340</v>
@@ -7485,7 +7485,7 @@
         <v>12</v>
       </c>
       <c r="I8" s="23" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="J8" s="20" t="s">
         <v>340</v>
@@ -7529,7 +7529,7 @@
         <v>214.441971</v>
       </c>
       <c r="I9" s="23" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="J9" s="20" t="s">
         <v>340</v>
@@ -7617,7 +7617,7 @@
         <v>80.084551000000005</v>
       </c>
       <c r="I11" s="23" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="J11" s="20" t="s">
         <v>340</v>
@@ -7661,7 +7661,7 @@
         <v>12</v>
       </c>
       <c r="I12" s="23" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="J12" s="20" t="s">
         <v>340</v>
@@ -7705,7 +7705,7 @@
         <v>12</v>
       </c>
       <c r="I13" s="23" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="J13" s="20" t="s">
         <v>340</v>
@@ -7749,7 +7749,7 @@
         <v>12</v>
       </c>
       <c r="I14" s="23" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="J14" s="20" t="s">
         <v>340</v>
@@ -7793,7 +7793,7 @@
         <v>12</v>
       </c>
       <c r="I15" s="23" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="J15" s="20" t="s">
         <v>340</v>
@@ -7837,7 +7837,7 @@
         <v>12</v>
       </c>
       <c r="I16" s="23" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="J16" s="20" t="s">
         <v>340</v>
@@ -7881,7 +7881,7 @@
         <v>12</v>
       </c>
       <c r="I17" s="23" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="J17" s="20" t="s">
         <v>342</v>
@@ -7969,7 +7969,7 @@
         <v>12</v>
       </c>
       <c r="I19" s="23" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="J19" s="20" t="s">
         <v>340</v>
@@ -8057,7 +8057,7 @@
         <v>12</v>
       </c>
       <c r="I21" s="23" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="J21" s="20" t="s">
         <v>342</v>
@@ -8145,7 +8145,7 @@
         <v>12</v>
       </c>
       <c r="I23" s="23" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="J23" s="20" t="s">
         <v>340</v>
@@ -8409,7 +8409,7 @@
         <v>70.495289999999997</v>
       </c>
       <c r="I29" s="23" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="J29" s="20" t="s">
         <v>340</v>
@@ -8497,7 +8497,7 @@
         <v>12</v>
       </c>
       <c r="I31" s="23" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="J31" s="20" t="s">
         <v>340</v>
@@ -8541,7 +8541,7 @@
         <v>12</v>
       </c>
       <c r="I32" s="23" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="J32" s="20" t="s">
         <v>340</v>
@@ -8585,7 +8585,7 @@
         <v>12</v>
       </c>
       <c r="I33" s="23" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="J33" s="20" t="s">
         <v>340</v>
@@ -8629,7 +8629,7 @@
         <v>12</v>
       </c>
       <c r="I34" s="23" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="J34" s="20" t="s">
         <v>342</v>
@@ -8673,7 +8673,7 @@
         <v>68.122753000000003</v>
       </c>
       <c r="I35" s="23" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="J35" s="20" t="s">
         <v>340</v>
@@ -8717,7 +8717,7 @@
         <v>12</v>
       </c>
       <c r="I36" s="23" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="J36" s="20" t="s">
         <v>340</v>
@@ -8914,12 +8914,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A08C373-50CB-424A-939A-38A53453958B}">
   <dimension ref="A1:R11"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="13"/>
     <col min="2" max="2" width="13.140625" style="13" bestFit="1" customWidth="1"/>
@@ -8994,25 +8994,25 @@
         <v>90</v>
       </c>
       <c r="L2" s="13" t="s">
+        <v>652</v>
+      </c>
+      <c r="M2" s="13" t="s">
         <v>368</v>
       </c>
-      <c r="M2" s="13" t="s">
+      <c r="N2" s="13" t="s">
         <v>369</v>
       </c>
-      <c r="N2" s="13" t="s">
+      <c r="O2" s="13" t="s">
         <v>370</v>
       </c>
-      <c r="O2" s="13" t="s">
+      <c r="P2" s="13" t="s">
         <v>371</v>
       </c>
-      <c r="P2" s="13" t="s">
+      <c r="Q2" s="13" t="s">
         <v>372</v>
       </c>
-      <c r="Q2" s="13" t="s">
+      <c r="R2" s="13" t="s">
         <v>373</v>
-      </c>
-      <c r="R2" s="13" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="382.5" x14ac:dyDescent="0.25">
@@ -9032,35 +9032,35 @@
         <v>203</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="H3" s="32"/>
       <c r="I3" s="11" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="J3" s="11" t="s">
         <v>201</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="M3" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="N3" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="P3" s="13" t="s">
+        <v>416</v>
+      </c>
+      <c r="Q3" s="13" t="s">
+        <v>383</v>
+      </c>
+      <c r="R3" s="13" t="s">
         <v>417</v>
-      </c>
-      <c r="Q3" s="13" t="s">
-        <v>384</v>
-      </c>
-      <c r="R3" s="13" t="s">
-        <v>418</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="369.75" x14ac:dyDescent="0.25">
@@ -9071,7 +9071,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>202</v>
@@ -9089,31 +9089,31 @@
         <v>30</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="J4" s="11" t="s">
         <v>207</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="L4" s="13" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="M4" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="N4" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="P4" s="13" t="s">
+        <v>413</v>
+      </c>
+      <c r="Q4" s="13" t="s">
+        <v>383</v>
+      </c>
+      <c r="R4" s="13" t="s">
         <v>414</v>
-      </c>
-      <c r="Q4" s="13" t="s">
-        <v>384</v>
-      </c>
-      <c r="R4" s="13" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="140.25" x14ac:dyDescent="0.25">
@@ -9139,31 +9139,31 @@
         <v>210</v>
       </c>
       <c r="H5" s="11" t="s">
+        <v>420</v>
+      </c>
+      <c r="I5" s="11" t="s">
         <v>421</v>
-      </c>
-      <c r="I5" s="11" t="s">
-        <v>422</v>
       </c>
       <c r="J5" s="11" t="s">
         <v>211</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="M5" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="N5" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="P5" s="13" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="Q5" s="13" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="R5" s="13" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="255" x14ac:dyDescent="0.25">
@@ -9186,37 +9186,37 @@
         <v>214</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="H6" s="12" t="s">
         <v>215</v>
       </c>
       <c r="I6" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="J6" s="11" t="s">
         <v>216</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="M6" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="N6" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="O6" s="13" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="P6" s="13" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="Q6" s="13" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="R6" s="13" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="369.75" x14ac:dyDescent="0.25">
@@ -9236,7 +9236,7 @@
         <v>12</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G7" s="11" t="s">
         <v>219</v>
@@ -9245,31 +9245,31 @@
         <v>30</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="J7" s="11" t="s">
         <v>220</v>
       </c>
       <c r="K7" s="11" t="s">
+        <v>436</v>
+      </c>
+      <c r="L7" s="13" t="s">
+        <v>395</v>
+      </c>
+      <c r="M7" s="13" t="s">
+        <v>374</v>
+      </c>
+      <c r="N7" s="13" t="s">
+        <v>374</v>
+      </c>
+      <c r="P7" s="13" t="s">
+        <v>435</v>
+      </c>
+      <c r="Q7" s="13" t="s">
+        <v>383</v>
+      </c>
+      <c r="R7" s="13" t="s">
         <v>437</v>
-      </c>
-      <c r="L7" s="13" t="s">
-        <v>396</v>
-      </c>
-      <c r="M7" s="13" t="s">
-        <v>375</v>
-      </c>
-      <c r="N7" s="13" t="s">
-        <v>375</v>
-      </c>
-      <c r="P7" s="13" t="s">
-        <v>436</v>
-      </c>
-      <c r="Q7" s="13" t="s">
-        <v>384</v>
-      </c>
-      <c r="R7" s="13" t="s">
-        <v>438</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="409.5" x14ac:dyDescent="0.25">
@@ -9283,40 +9283,40 @@
         <v>233</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="E8" s="12" t="s">
         <v>12</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="H8" s="12" t="s">
         <v>30</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="J8" s="11" t="s">
         <v>221</v>
       </c>
       <c r="K8" s="11" t="s">
+        <v>443</v>
+      </c>
+      <c r="L8" s="13" t="s">
+        <v>441</v>
+      </c>
+      <c r="P8" s="13" t="s">
+        <v>440</v>
+      </c>
+      <c r="Q8" s="13" t="s">
+        <v>383</v>
+      </c>
+      <c r="R8" s="13" t="s">
         <v>444</v>
-      </c>
-      <c r="L8" s="13" t="s">
-        <v>442</v>
-      </c>
-      <c r="P8" s="13" t="s">
-        <v>441</v>
-      </c>
-      <c r="Q8" s="13" t="s">
-        <v>384</v>
-      </c>
-      <c r="R8" s="13" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="229.5" x14ac:dyDescent="0.25">
@@ -9336,16 +9336,16 @@
         <v>224</v>
       </c>
       <c r="F9" s="11" t="s">
+        <v>445</v>
+      </c>
+      <c r="G9" s="12" t="s">
         <v>446</v>
       </c>
-      <c r="G9" s="12" t="s">
-        <v>447</v>
-      </c>
       <c r="H9" s="11" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="J9" s="11" t="s">
         <v>225</v>
@@ -9354,25 +9354,25 @@
         <v>226</v>
       </c>
       <c r="L9" s="13" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="M9" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="N9" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="O9" s="13" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="P9" s="13" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="Q9" s="13" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="R9" s="13" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="76.5" x14ac:dyDescent="0.25">
@@ -9392,13 +9392,13 @@
         <v>12</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="G10" s="11" t="s">
         <v>229</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="I10" s="11" t="s">
         <v>230</v>
@@ -9410,25 +9410,25 @@
         <v>232</v>
       </c>
       <c r="L10" s="13" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="M10" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="N10" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="O10" s="13" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="P10" s="13" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="Q10" s="13" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="R10" s="13" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="127.5" x14ac:dyDescent="0.25">
@@ -9442,13 +9442,13 @@
         <v>233</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="G11" s="12" t="s">
         <v>234</v>
@@ -9466,25 +9466,25 @@
         <v>237</v>
       </c>
       <c r="L11" s="13" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="M11" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="N11" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="O11" s="13" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="P11" s="13" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="Q11" s="13" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="R11" s="13" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
   </sheetData>
@@ -9502,7 +9502,7 @@
       <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="38.28515625" style="20" customWidth="1"/>
     <col min="2" max="2" width="65.140625" style="20" customWidth="1"/>
@@ -9523,35 +9523,35 @@
     </row>
     <row r="2" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
+        <v>539</v>
+      </c>
+      <c r="B2" s="20" t="s">
         <v>540</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="C2" s="31" t="s">
         <v>541</v>
-      </c>
-      <c r="C2" s="31" t="s">
-        <v>542</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
+        <v>386</v>
+      </c>
+      <c r="B3" s="20" t="s">
         <v>387</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="C3" s="31" t="s">
         <v>388</v>
-      </c>
-      <c r="C3" s="31" t="s">
-        <v>389</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
+        <v>468</v>
+      </c>
+      <c r="B4" s="26" t="s">
         <v>469</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="C4" s="42" t="s">
         <v>470</v>
-      </c>
-      <c r="C4" s="42" t="s">
-        <v>471</v>
       </c>
       <c r="D4" s="26"/>
       <c r="E4" s="26"/>
@@ -9569,37 +9569,37 @@
     </row>
     <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
+        <v>405</v>
+      </c>
+      <c r="B6" s="20" t="s">
         <v>406</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="C6" s="31" t="s">
         <v>407</v>
-      </c>
-      <c r="C6" s="31" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="C7" s="42" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="D7" s="26"/>
       <c r="E7" s="26"/>
     </row>
     <row r="8" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="C8" s="31" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -9620,23 +9620,23 @@
         <v>46</v>
       </c>
       <c r="B10" s="26" t="s">
+        <v>616</v>
+      </c>
+      <c r="C10" s="42" t="s">
         <v>617</v>
-      </c>
-      <c r="C10" s="42" t="s">
-        <v>618</v>
       </c>
       <c r="D10" s="26"/>
       <c r="E10" s="26"/>
     </row>
     <row r="11" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="C11" s="38" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="D11" s="25"/>
       <c r="E11" s="25"/>
@@ -9679,13 +9679,13 @@
     </row>
     <row r="15" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
+        <v>550</v>
+      </c>
+      <c r="B15" s="20" t="s">
         <v>551</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="C15" s="31" t="s">
         <v>552</v>
-      </c>
-      <c r="C15" s="31" t="s">
-        <v>553</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15" x14ac:dyDescent="0.25">
@@ -9701,32 +9701,32 @@
     </row>
     <row r="17" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="26" t="s">
+        <v>383</v>
+      </c>
+      <c r="B17" s="20" t="s">
         <v>384</v>
       </c>
-      <c r="B17" s="20" t="s">
+      <c r="C17" s="31" t="s">
         <v>385</v>
-      </c>
-      <c r="C17" s="31" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="18" spans="1:8" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="34" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B18" s="35" t="s">
         <v>349</v>
       </c>
-      <c r="C18" s="46" t="s">
+      <c r="C18" s="45" t="s">
         <v>350</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="43" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="C19" s="31" t="s">
         <v>351</v>
@@ -9747,26 +9747,26 @@
     </row>
     <row r="21" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="26" t="s">
+        <v>522</v>
+      </c>
+      <c r="B21" s="26" t="s">
         <v>523</v>
       </c>
-      <c r="B21" s="26" t="s">
+      <c r="C21" s="42" t="s">
         <v>524</v>
-      </c>
-      <c r="C21" s="42" t="s">
-        <v>525</v>
       </c>
       <c r="D21" s="26"/>
       <c r="E21" s="26"/>
     </row>
     <row r="22" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="20" t="s">
+        <v>532</v>
+      </c>
+      <c r="B22" s="20" t="s">
         <v>533</v>
       </c>
-      <c r="B22" s="20" t="s">
+      <c r="C22" s="31" t="s">
         <v>534</v>
-      </c>
-      <c r="C22" s="31" t="s">
-        <v>535</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -9784,13 +9784,13 @@
     </row>
     <row r="24" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="20" t="s">
+        <v>513</v>
+      </c>
+      <c r="B24" s="20" t="s">
         <v>514</v>
       </c>
-      <c r="B24" s="20" t="s">
+      <c r="C24" s="31" t="s">
         <v>515</v>
-      </c>
-      <c r="C24" s="31" t="s">
-        <v>516</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -9812,10 +9812,10 @@
         <v>50</v>
       </c>
       <c r="B26" s="20" t="s">
+        <v>626</v>
+      </c>
+      <c r="C26" s="46" t="s">
         <v>627</v>
-      </c>
-      <c r="C26" s="47" t="s">
-        <v>628</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9859,13 +9859,13 @@
     </row>
     <row r="30" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A30" s="20" t="s">
+        <v>604</v>
+      </c>
+      <c r="B30" s="25" t="s">
         <v>605</v>
       </c>
-      <c r="B30" s="25" t="s">
+      <c r="C30" s="38" t="s">
         <v>606</v>
-      </c>
-      <c r="C30" s="38" t="s">
-        <v>607</v>
       </c>
       <c r="D30" s="25"/>
       <c r="E30" s="25"/>
@@ -9875,13 +9875,13 @@
     </row>
     <row r="31" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
+        <v>535</v>
+      </c>
+      <c r="B31" s="37" t="s">
         <v>536</v>
       </c>
-      <c r="B31" s="37" t="s">
+      <c r="C31" s="42" t="s">
         <v>537</v>
-      </c>
-      <c r="C31" s="42" t="s">
-        <v>538</v>
       </c>
       <c r="D31" s="37"/>
       <c r="E31" s="37"/>
@@ -9901,13 +9901,13 @@
     </row>
     <row r="33" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="20" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B33" s="20" t="s">
+        <v>585</v>
+      </c>
+      <c r="C33" s="31" t="s">
         <v>586</v>
-      </c>
-      <c r="C33" s="31" t="s">
-        <v>587</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9951,117 +9951,117 @@
     </row>
     <row r="37" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="26" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B37" s="20" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C37" s="31" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="20" t="s">
+        <v>377</v>
+      </c>
+      <c r="B38" s="20" t="s">
         <v>378</v>
       </c>
-      <c r="B38" s="20" t="s">
+      <c r="C38" s="31" t="s">
         <v>379</v>
-      </c>
-      <c r="C38" s="31" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="20" t="s">
+        <v>389</v>
+      </c>
+      <c r="B39" s="20" t="s">
         <v>390</v>
       </c>
-      <c r="B39" s="20" t="s">
+      <c r="C39" s="31" t="s">
         <v>391</v>
-      </c>
-      <c r="C39" s="31" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="26" t="s">
+        <v>398</v>
+      </c>
+      <c r="B40" s="20" t="s">
         <v>399</v>
       </c>
-      <c r="B40" s="20" t="s">
+      <c r="C40" s="31" t="s">
         <v>400</v>
-      </c>
-      <c r="C40" s="31" t="s">
-        <v>401</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="20" t="s">
+        <v>441</v>
+      </c>
+      <c r="B41" s="20" t="s">
         <v>442</v>
       </c>
-      <c r="B41" s="20" t="s">
-        <v>443</v>
-      </c>
       <c r="C41" s="20" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="B42" s="20" t="s">
         <v>393</v>
       </c>
-      <c r="B42" s="20" t="s">
+      <c r="C42" s="31" t="s">
         <v>394</v>
-      </c>
-      <c r="C42" s="31" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A43" s="20" t="s">
+        <v>576</v>
+      </c>
+      <c r="B43" s="25" t="s">
         <v>577</v>
       </c>
-      <c r="B43" s="25" t="s">
+      <c r="C43" s="38" t="s">
         <v>578</v>
-      </c>
-      <c r="C43" s="38" t="s">
-        <v>579</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="26" t="s">
+        <v>395</v>
+      </c>
+      <c r="B44" s="20" t="s">
         <v>396</v>
       </c>
-      <c r="B44" s="20" t="s">
+      <c r="C44" s="31" t="s">
         <v>397</v>
-      </c>
-      <c r="C44" s="31" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A45" s="20" t="s">
+        <v>558</v>
+      </c>
+      <c r="B45" s="25" t="s">
         <v>559</v>
       </c>
-      <c r="B45" s="25" t="s">
+      <c r="C45" s="38" t="s">
         <v>560</v>
-      </c>
-      <c r="C45" s="38" t="s">
-        <v>561</v>
       </c>
       <c r="D45" s="25"/>
       <c r="E45" s="25"/>
       <c r="F45" s="25"/>
       <c r="G45" s="25"/>
-      <c r="H45" s="45"/>
+      <c r="H45" s="44"/>
     </row>
     <row r="46" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="26" t="s">
+        <v>380</v>
+      </c>
+      <c r="B46" s="20" t="s">
+        <v>382</v>
+      </c>
+      <c r="C46" s="31" t="s">
         <v>381</v>
-      </c>
-      <c r="B46" s="20" t="s">
-        <v>383</v>
-      </c>
-      <c r="C46" s="31" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -10093,26 +10093,26 @@
     </row>
     <row r="49" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A49" s="20" t="s">
+        <v>568</v>
+      </c>
+      <c r="B49" s="25" t="s">
         <v>569</v>
       </c>
-      <c r="B49" s="25" t="s">
+      <c r="C49" s="38" t="s">
         <v>570</v>
-      </c>
-      <c r="C49" s="38" t="s">
-        <v>571</v>
       </c>
       <c r="D49" s="43"/>
       <c r="E49" s="43"/>
       <c r="F49" s="25"/>
       <c r="G49" s="27"/>
-      <c r="H49" s="45"/>
+      <c r="H49" s="44"/>
     </row>
     <row r="50" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="26" t="s">
+        <v>408</v>
+      </c>
+      <c r="B50" s="26" t="s">
         <v>409</v>
-      </c>
-      <c r="B50" s="26" t="s">
-        <v>410</v>
       </c>
       <c r="C50" s="42" t="s">
         <v>76</v>
@@ -10135,24 +10135,24 @@
     </row>
     <row r="52" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="26" t="s">
+        <v>374</v>
+      </c>
+      <c r="B52" s="20" t="s">
         <v>375</v>
       </c>
-      <c r="B52" s="20" t="s">
+      <c r="C52" s="31" t="s">
         <v>376</v>
-      </c>
-      <c r="C52" s="31" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="20" t="s">
+        <v>431</v>
+      </c>
+      <c r="B53" s="20" t="s">
         <v>432</v>
       </c>
-      <c r="B53" s="20" t="s">
+      <c r="C53" s="31" t="s">
         <v>433</v>
-      </c>
-      <c r="C53" s="31" t="s">
-        <v>434</v>
       </c>
     </row>
   </sheetData>

</xml_diff>